<commit_message>
Upgrade to edmaps v1.4.0
... File versions consistent with https://bitbucket.org/cebra/project-170607/commits/f2c782004dc27c66707bfda212f95d5fd8430ae3
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/project-170607/projects/case_studies/user_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4430F659-C7DA-0942-B176-BA5D7278F846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E989C6E-5B69-4B41-B5BB-31C8FAE5AB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{236919D7-CD01-A940-BDF2-FF56F5903D66}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,23 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
   <si>
     <t>risk_layers/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/oriental_fruitfly/cabi_dorsalis_20April19.csv</t>
-  </si>
-  <si>
     <t>khapra beetle</t>
   </si>
   <si>
     <t>gypsy moth</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/gypsy_moth/cabi_lymantria_dispar_6June19.csv</t>
-  </si>
-  <si>
     <t>Lymantria dispar</t>
   </si>
   <si>
@@ -61,9 +57,6 @@
     <t>risk_layers/abiotic/occurrences/BMSB/cabi_halyomorpha halys_9Jun19.csv</t>
   </si>
   <si>
-    <t>Halyomorpha halys</t>
-  </si>
-  <si>
     <t>tourists, residents, torres</t>
   </si>
   <si>
@@ -152,9 +145,6 @@
   </si>
   <si>
     <t>Occurrence path</t>
-  </si>
-  <si>
-    <t>CABI path</t>
   </si>
   <si>
     <t>Exclude BIOCLIM vars</t>
@@ -679,6 +669,15 @@
   </si>
   <si>
     <t>oriental fruitfly</t>
+  </si>
+  <si>
+    <t>risk_layers/abiotic/occurrences/gypsy_moth/cabi_lymantria_dispar_6June19.csv</t>
+  </si>
+  <si>
+    <t>Infected countries</t>
+  </si>
+  <si>
+    <t>risk_layers/abiotic/occurrences/oriental_fruitfly/cabi_dorsalis_20April19.csv</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1202,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1215,62 +1228,19 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -1285,6 +1255,173 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFE7E6E6"/>
@@ -1315,42 +1452,28 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1895,6 +2018,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF835D4-5F9A-AE4A-9F33-C8B7BF91B061}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1909,28 +2033,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23" t="b">
         <v>1</v>
@@ -1938,98 +2062,98 @@
     </row>
     <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C12" s="25">
         <f>LN(0.5)/200</f>
@@ -2038,10 +2162,10 @@
     </row>
     <row r="13" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C13" s="25">
         <f>LN(0.5)/10</f>
@@ -2051,10 +2175,10 @@
     </row>
     <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C14" s="25">
         <v>10633690</v>
@@ -2063,10 +2187,10 @@
     </row>
     <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C15" s="25">
         <v>12722820</v>
@@ -2076,10 +2200,10 @@
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C16" s="25">
         <v>51000</v>
@@ -2088,10 +2212,10 @@
     </row>
     <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C17" s="25">
         <v>152000000</v>
@@ -2100,10 +2224,10 @@
     </row>
     <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C18" s="25">
         <v>18612</v>
@@ -2112,10 +2236,10 @@
     </row>
     <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C19" s="25">
         <v>6907</v>
@@ -2124,10 +2248,10 @@
     </row>
     <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C20" s="25">
         <v>1216726</v>
@@ -2136,10 +2260,10 @@
     </row>
     <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="48" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C21" s="25">
         <v>4475</v>
@@ -2148,10 +2272,10 @@
     </row>
     <row r="22" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="50" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C22" s="28">
         <v>15832</v>
@@ -2161,47 +2285,47 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsBlanks" dxfId="47" priority="31">
+    <cfRule type="containsBlanks" dxfId="63" priority="31">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="46" priority="29">
+    <cfRule type="containsBlanks" dxfId="62" priority="29">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="45" priority="16">
+    <cfRule type="expression" dxfId="61" priority="16">
       <formula>ISBLANK($C$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="44" priority="12">
+    <cfRule type="expression" dxfId="60" priority="12">
       <formula>ISBLANK($C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="43" priority="8">
+    <cfRule type="expression" dxfId="59" priority="8">
       <formula>ISBLANK($C$11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="42" priority="13">
+    <cfRule type="expression" dxfId="58" priority="13">
       <formula>ISBLANK($C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="41" priority="6">
+    <cfRule type="expression" dxfId="57" priority="6">
       <formula>ISBLANK($C$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="40" priority="14">
+    <cfRule type="expression" dxfId="56" priority="14">
       <formula>ISBLANK($C$8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="55" priority="2">
       <formula>ISBLANK($C$7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2544,7 +2668,8 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D738B5-D0EE-C044-83A0-D9C8F02CE7C0}">
-  <dimension ref="A1:Z6"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2585,88 +2710,88 @@
   <sheetData>
     <row r="1" spans="1:26" s="38" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="I1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="N1" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="O1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="P1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="32" t="s">
+      <c r="Q1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="S1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="W1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="Y1" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="V1" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>53</v>
       </c>
       <c r="Z1" s="37"/>
     </row>
     <row r="2" spans="1:26" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="17" t="b">
         <v>1</v>
@@ -2678,11 +2803,11 @@
         <v>0</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I2" s="18">
         <v>1970</v>
@@ -2691,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
@@ -2722,10 +2847,10 @@
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -2737,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -2780,10 +2905,10 @@
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
@@ -2795,20 +2920,20 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3">
         <v>1970</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -2840,10 +2965,10 @@
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>1</v>
@@ -2855,20 +2980,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1970</v>
-      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N5" s="5">
         <f>0.000002381577*30/45</f>
@@ -2901,122 +3022,194 @@
       </c>
       <c r="Z5" s="29"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="D6" s="4"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="B2:I1048576 N2:Y1048576">
-    <cfRule type="containsBlanks" dxfId="20" priority="291">
-      <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="expression" dxfId="19" priority="43">
-      <formula>AND(NOT(ISBLANK($A2)),$E2 = TRUE, ISBLANK($G2))</formula>
+    <cfRule type="expression" dxfId="36" priority="67">
+      <formula>ISBLANK($G2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$E2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="expression" dxfId="18" priority="56">
-      <formula>AND(NOT(ISBLANK($A2)),ISBLANK($F2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="17" priority="83">
-      <formula>AND($C2=TRUE, ISBLANK($H2), NOT(ISBLANK($A2)), ISBLANK($J2))</formula>
+    <cfRule type="expression" dxfId="35" priority="80">
+      <formula>ISBLANK($F2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H1048576 J2:J1048576 L2:L1048576">
+    <cfRule type="expression" dxfId="34" priority="107">
+      <formula>AND(ISBLANK($H2), ISBLANK($J2), ISBLANK($L2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="expression" dxfId="16" priority="84">
-      <formula>AND($C2=TRUE, ISBLANK($I2), NOT(ISBLANK($A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>AND(NOT(ISBLANK($A2)),$C2=TRUE,ISBLANK($H2))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17">
-      <formula>OR(ISBLANK($A2), $C2=FALSE)</formula>
+    <cfRule type="expression" dxfId="33" priority="15">
+      <formula>ISBLANK($H2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K1048576">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>OR(ISBLANK($A2), $C2=FALSE)</formula>
+    <cfRule type="expression" dxfId="32" priority="39">
+      <formula>OR($C2=FALSE, AND(ISBLANK($H2), ISBLANK($J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S1048576">
-    <cfRule type="expression" dxfId="12" priority="258">
-      <formula>AND(SEARCH("vessels",$B2), ISBLANK($S2))</formula>
+    <cfRule type="expression" dxfId="31" priority="9">
+      <formula>NOT(ISNUMBER(SEARCH("vessels", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="282">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$B2)), ISBLANK($S2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="29" priority="26">
       <formula>OR(ISBLANK($A2),$C2=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="expression" dxfId="10" priority="281">
-      <formula>OR(ISBLANK($A2),$C2=FALSE,NOT(ISBLANK($L2)))</formula>
+  <conditionalFormatting sqref="H2:K1048576 M2:M1048576">
+    <cfRule type="expression" dxfId="28" priority="305">
+      <formula>NOT(ISBLANK($L2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="expression" dxfId="9" priority="131">
-      <formula>AND(SEARCH("residents",$B2), ISBLANK($O2))</formula>
+    <cfRule type="expression" dxfId="27" priority="13">
+      <formula>NOT(ISNUMBER(SEARCH("residents", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="155">
+      <formula>AND(ISNUMBER(SEARCH("residents",$B2)), ISBLANK($O2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P1048576">
-    <cfRule type="expression" dxfId="8" priority="282">
-      <formula>AND(SEARCH("torres",$B2), ISBLANK($P2))</formula>
+    <cfRule type="expression" dxfId="25" priority="12">
+      <formula>NOT(ISNUMBER(SEARCH("torres", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="306">
+      <formula>AND(ISNUMBER(SEARCH("torres",$B2)), ISBLANK($P2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q1048576">
-    <cfRule type="expression" dxfId="7" priority="283">
+    <cfRule type="expression" dxfId="23" priority="11">
+      <formula>NOT(ISNUMBER(SEARCH("mail", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="307">
       <formula>AND(SEARCH("mail",$B2), ISBLANK($Q2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R1048576">
-    <cfRule type="expression" dxfId="6" priority="285">
-      <formula>AND(SEARCH("vessels",$B2), ISBLANK($R2))</formula>
+    <cfRule type="expression" dxfId="21" priority="10">
+      <formula>NOT(ISNUMBER(SEARCH("vessels", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="309">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$B2)), ISBLANK($R2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T1048576">
-    <cfRule type="expression" dxfId="5" priority="286">
-      <formula>AND(SEARCH("fert",$B2), ISBLANK($T2))</formula>
+    <cfRule type="expression" dxfId="19" priority="8">
+      <formula>NOT(ISNUMBER(SEARCH("fert", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="310">
+      <formula>AND(ISNUMBER(SEARCH("fert",$B2)), ISBLANK($T2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U1048576">
-    <cfRule type="expression" dxfId="4" priority="287">
-      <formula>AND(SEARCH("machine",$B2), ISBLANK($U2))</formula>
+    <cfRule type="expression" dxfId="17" priority="7">
+      <formula>NOT(ISNUMBER(SEARCH("machine", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="311">
+      <formula>AND(ISNUMBER(SEARCH("machine",$B2)), ISBLANK($U2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V1048576">
-    <cfRule type="expression" dxfId="3" priority="288">
-      <formula>AND(SEARCH("container",$B2), ISBLANK($V2))</formula>
+    <cfRule type="expression" dxfId="15" priority="6">
+      <formula>NOT(ISNUMBER(SEARCH("container", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="312">
+      <formula>AND(ISNUMBER(SEARCH("container",$B2)), ISBLANK($V2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W1048576">
-    <cfRule type="expression" dxfId="2" priority="289">
-      <formula>AND(SEARCH("nursery",$B2), ISBLANK($W2))</formula>
+    <cfRule type="expression" dxfId="13" priority="5">
+      <formula>NOT(ISNUMBER(SEARCH("nursery", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="313">
+      <formula>AND(ISNUMBER(SEARCH("nursery",$B2)), ISBLANK($W2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X1048576">
-    <cfRule type="expression" dxfId="1" priority="290">
-      <formula>AND(SEARCH("food",$B2), ISBLANK($X2))</formula>
+    <cfRule type="expression" dxfId="11" priority="4">
+      <formula>NOT(ISNUMBER(SEARCH("food", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="314">
+      <formula>AND(ISNUMBER(SEARCH("food",$B2)), ISBLANK($X2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(SEARCH("tourists",$B2), ISBLANK($N2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="48">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>NOT(ISNUMBER(SEARCH("tourists",$B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="25">
+      <formula>AND(ISNUMBER(SEARCH("tourists",$B2)), ISBLANK($N2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="expression" dxfId="7" priority="24">
+      <formula>OR(ISBLANK($A4), $C4=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="6" priority="21">
+      <formula>ISBLANK($B2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:Y1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>ISBLANK($A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C1048576">
+    <cfRule type="expression" dxfId="4" priority="20">
+      <formula>ISBLANK($C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="expression" dxfId="3" priority="22">
+      <formula>ISBLANK($D2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="expression" dxfId="2" priority="18">
+      <formula>ISBLANK($E2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:M1048576">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$C2=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="45">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="F1" xr:uid="{610A6EDE-65F2-9448-845D-1D9D26647888}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A1" xr:uid="{AD160B45-C62D-E948-B89F-CBE0E706C1DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C1" xr:uid="{8A54E1E1-25E5-4A4C-A35B-02A189BDAE39}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="D1" xr:uid="{74C7EF83-30DD-F948-9522-90AFB2FCEC74}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="E1" xr:uid="{893B753C-83F4-644D-BD7E-F6B39072EB1E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="G1" xr:uid="{41980E33-1E39-AD45-8F05-868D6600E067}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF minimum year" prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="I1" xr:uid="{A33E5C3F-FEB5-E142-9E77-829BE9CDC095}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="N1" xr:uid="{7D0C5A9D-2B24-5E4B-B142-62EC654E71D3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="O1" xr:uid="{BFE515ED-E47C-8E4A-A50B-35E2286ACF32}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="P1" xr:uid="{0A697F1D-F494-C347-95D9-E59F4C6C383A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="Q1" xr:uid="{399C1480-40E4-5A41-A2FF-2E4F826C4DEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="R1" xr:uid="{1BBA7A75-F6E1-4F47-BC5E-4B3FDC509E65}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="S1" xr:uid="{12F7F3FA-47A2-8B43-B105-3D925A1D9D46}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="T1" xr:uid="{14C39FAF-9B97-1543-B73A-260E86BB654B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="U1" xr:uid="{9FFB111A-9910-744C-B50F-00F7A89B9CA3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="V1" xr:uid="{E6D7E48A-15CD-1A4F-BAD7-13A132F3D69F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="W1" xr:uid="{34153A47-9E0E-4F4D-B565-CC6104D4CF6D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per unit of food." sqref="X1" xr:uid="{DDEBC040-5553-4841-9E5B-5FB894300E90}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Name must begin with a letter or a period." promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A2:A1048576" xr:uid="{F8431168-FF74-CF44-A9C3-C9F4FDBC2E6C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="F1" xr:uid="{610A6EDE-65F2-9448-845D-1D9D26647888}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C2:C1048576" xr:uid="{B5EAF5EE-6EE5-6B49-99E2-F42D5D06C580}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Expert occurrence data path" prompt="File path (absolute or relative to working directory) to occurrence dataset." sqref="J1:J1048576" xr:uid="{344DBD62-32DD-2640-814E-8FECEF8AE89F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried." sqref="H1:H1048576" xr:uid="{867EBE5D-A33C-8641-98B7-84DD0D595AEA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Expert occurrence data path" prompt="File path (absolute or relative to working directory) to occurrence dataset. Ignored if &quot;Climate suitability path&quot; is provided." sqref="J1:J1048576" xr:uid="{344DBD62-32DD-2640-814E-8FECEF8AE89F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried. Ignored if &quot;Climate suitability path&quot; is provided." sqref="H1:H1048576" xr:uid="{867EBE5D-A33C-8641-98B7-84DD0D595AEA}"/>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="Q2:Q1048576" xr:uid="{77FCB406-D2F1-BD40-8A66-E8D4EB673AEF}">
       <formula1>0</formula1>
     </dataValidation>
@@ -3041,12 +3234,10 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per unit of food." sqref="X2:X1048576" xr:uid="{F4D6DD70-484B-8F4C-8022-F92827712D2D}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, or if less than or equal to 1000, the default value of 5000 will be used." sqref="Y1" xr:uid="{5D1E5874-099E-9046-99E1-7D5AE01B1EEA}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="D2:D1048576" xr:uid="{4885AF70-80FE-5741-BB46-A0C58FDF8CF8}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS classes" prompt="Comma-separated NVIS MVG classes (e.g. 1,2,3,5)." sqref="Y1" xr:uid="{D6F9B4AA-1732-254B-BD34-C3458D51A615}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CABI file path" prompt="File path (absolute or relative to working directory) to the CABI csv file." sqref="K1:K1048576 Y1" xr:uid="{1102FFA6-1227-9743-9757-11E831420417}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Infected countries" prompt="Either a comma-separated string containing country names, or a file path (absolute or relative to working directory) to a CABI pest data sheet csv file. _x000a__x000a_If provided, occurrence records are verified against the provided data, to ensure that all records a" sqref="K1:K1048576" xr:uid="{1102FFA6-1227-9743-9757-11E831420417}"/>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="GBIF maximum uncertainty" prompt="Highest tolerable coordinate uncertainty (in metres) when downloading GBIF occurrence data." sqref="J2:K1048576" xr:uid="{6FD266E6-D30F-E140-8841-0CC016C4626A}">
       <formula1>0</formula1>
     </dataValidation>
@@ -3067,30 +3258,7 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="P2:P1048576" xr:uid="{36BBB07A-382B-294E-8FD2-7455864CB2E2}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Aggregation resolution" prompt="An aggregation resolution (in metres)_x000a__x000a_DEFAULT: 5000 (5km)" sqref="Y1" xr:uid="{4F655586-D61C-B549-987D-5F3431414882}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A1" xr:uid="{AD160B45-C62D-E948-B89F-CBE0E706C1DD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C1" xr:uid="{8A54E1E1-25E5-4A4C-A35B-02A189BDAE39}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="D1" xr:uid="{74C7EF83-30DD-F948-9522-90AFB2FCEC74}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="E1" xr:uid="{893B753C-83F4-644D-BD7E-F6B39072EB1E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="G1" xr:uid="{41980E33-1E39-AD45-8F05-868D6600E067}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF minimum year" prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="I1" xr:uid="{A33E5C3F-FEB5-E142-9E77-829BE9CDC095}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exclude BIOCLIM variables" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19)._x000a__x000a_Ignored if &quot;Climate suitability path&quot; is provided._x000a__x000a_Default: No variables are excluded." sqref="M1:M1048576" xr:uid="{A215B8BE-50BD-544B-BB88-017607D43B99}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="N1" xr:uid="{7D0C5A9D-2B24-5E4B-B142-62EC654E71D3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="O1" xr:uid="{BFE515ED-E47C-8E4A-A50B-35E2286ACF32}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="P1" xr:uid="{0A697F1D-F494-C347-95D9-E59F4C6C383A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="Q1" xr:uid="{399C1480-40E4-5A41-A2FF-2E4F826C4DEE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="R1" xr:uid="{1BBA7A75-F6E1-4F47-BC5E-4B3FDC509E65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="S1" xr:uid="{12F7F3FA-47A2-8B43-B105-3D925A1D9D46}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="T1" xr:uid="{14C39FAF-9B97-1543-B73A-260E86BB654B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="U1" xr:uid="{9FFB111A-9910-744C-B50F-00F7A89B9CA3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="V1" xr:uid="{E6D7E48A-15CD-1A4F-BAD7-13A132F3D69F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="W1" xr:uid="{34153A47-9E0E-4F4D-B565-CC6104D4CF6D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per unit of food." sqref="X1" xr:uid="{DDEBC040-5553-4841-9E5B-5FB894300E90}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be either blank or else a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, or if less than or equal to 1000, the default value of 5000 will be used." sqref="Y2:Y1048576" xr:uid="{835B285B-8DD4-A24D-B7F3-92BE814D9770}">
-      <formula1>MOD(AY3,1000)=0</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="CABI file path" prompt="File path (absolute or relative to working directory) to the CABI csv file." sqref="F2:F1048576" xr:uid="{1CBF3D45-3CF8-6645-AD64-572A122AD92A}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(F2,ROW(INDIRECT("1:"&amp;LEN(F2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
@@ -3101,6 +3269,9 @@
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(G2,ROW(INDIRECT("1:"&amp;LEN(G2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate suitability path" prompt="Optional file path to a climate suitability raster. Must be binary (0=unsuitable; 1=suitable) or describe relative suitability between 0-1. Must be 1000 m res; Australian Albers (EPSG:3577); extent xmin=-1888000; xmax=2122000; ymin=-4847000; ymax=-1010000" sqref="L1:L1048576" xr:uid="{480B32ED-B00C-3F4B-AE28-DF01A191FCC5}"/>
+    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Aggregated output resolution must be a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, the default value of 5000 will be used." sqref="Y1:Y1048576" xr:uid="{D738A470-664E-C741-8411-D92C81327D2C}">
+      <formula1>AND($Y1 &gt;= 1000, MOD($Y1, 1000)=0)</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rows for gbif username and password
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/project-170607/projects/case_studies/user_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/edmaps-github/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C362E90A-1FDD-8342-9E34-21E4E07363F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6196267C-8105-4742-B409-1A5F0F5575F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{236919D7-CD01-A940-BDF2-FF56F5903D66}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>risk_layers/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
   </si>
@@ -687,6 +687,18 @@
   </si>
   <si>
     <t>Total volume of fresh foods arriving in Australia per annum (foods pathway)</t>
+  </si>
+  <si>
+    <t>GBIF username</t>
+  </si>
+  <si>
+    <t>Username for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
+  </si>
+  <si>
+    <t>GBIF password</t>
+  </si>
+  <si>
+    <t>Password for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
   </si>
 </sst>
 </file>
@@ -754,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1065,11 +1077,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1262,18 +1305,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1287,6 +1333,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -1601,6 +1654,26 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2100,9 +2173,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF835D4-5F9A-AE4A-9F33-C8B7BF91B061}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2141,390 +2214,388 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>21</v>
-      </c>
+    <row r="4" spans="1:10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="57"/>
     </row>
-    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>60</v>
-      </c>
+    <row r="5" spans="1:10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="57"/>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B13" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C13" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
+    <row r="14" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B14" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C14" s="25">
         <f>LN(0.5)/200</f>
         <v>-3.4657359027997266E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+    <row r="15" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B15" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C15" s="25">
         <f>LN(0.5)/10</f>
         <v>-6.9314718055994526E-2</v>
       </c>
-      <c r="J13" s="26"/>
-    </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="25">
-        <v>10633690</v>
-      </c>
-      <c r="J14" s="26"/>
-    </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="25">
-        <v>12722820</v>
-      </c>
-      <c r="E15" s="27"/>
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C16" s="25">
-        <v>51000</v>
+        <v>10633690</v>
       </c>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C17" s="25">
-        <v>152000000</v>
-      </c>
+        <v>12722820</v>
+      </c>
+      <c r="E17" s="27"/>
       <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="25">
-        <v>18612</v>
+        <v>51000</v>
       </c>
       <c r="J18" s="26"/>
     </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" s="25">
-        <v>6907</v>
+        <v>152000000</v>
       </c>
       <c r="J19" s="26"/>
     </row>
     <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" s="25">
-        <v>1216726</v>
+        <v>18612</v>
       </c>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C21" s="25">
-        <v>4475</v>
+        <v>6907</v>
       </c>
       <c r="J21" s="26"/>
     </row>
-    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="54">
-        <v>15832</v>
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1216726</v>
       </c>
       <c r="J22" s="26"/>
     </row>
-    <row r="23" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="25">
+        <v>4475</v>
+      </c>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="54">
+        <v>15832</v>
+      </c>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B25" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C25" s="28">
         <f>4*3864976</f>
         <v>15459904</v>
       </c>
-      <c r="J23" s="26"/>
+      <c r="J25" s="26"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="containsBlanks" dxfId="67" priority="33">
+      <formula>LEN(TRIM(C6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="containsBlanks" dxfId="66" priority="31">
+      <formula>LEN(TRIM(C3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="65" priority="18">
+      <formula>ISBLANK($C$8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="64" priority="14">
+      <formula>ISBLANK($C$12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="63" priority="10">
+      <formula>ISBLANK($C$13)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="62" priority="15">
+      <formula>ISBLANK($C$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="61" priority="8">
+      <formula>ISBLANK($C$7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="60" priority="16">
+      <formula>ISBLANK($C$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="59" priority="4">
+      <formula>ISBLANK($C$9)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="58" priority="2">
+      <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsBlanks" dxfId="65" priority="31">
-      <formula>LEN(TRIM(C4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="64" priority="29">
-      <formula>LEN(TRIM(C3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="63" priority="16">
-      <formula>ISBLANK($C$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="62" priority="12">
-      <formula>ISBLANK($C$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="61" priority="8">
-      <formula>ISBLANK($C$11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="60" priority="13">
-      <formula>ISBLANK($C$9)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="59" priority="6">
-      <formula>ISBLANK($C$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="58" priority="14">
-      <formula>ISBLANK($C$8)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="57" priority="2">
-      <formula>ISBLANK($C$7)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="35">
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C13" xr:uid="{E0754A1A-56A1-0F4E-B3F5-F1BC5ED3C00B}">
+    <cfRule type="expression" dxfId="57" priority="1">
+      <formula>AND(NOT(ISBLANK($C$5)), ISBLANK($C$4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="36">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C15" xr:uid="{E0754A1A-56A1-0F4E-B3F5-F1BC5ED3C00B}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="C12" xr:uid="{DCF42841-7DAF-D442-8729-D9AFD8CFB919}">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="C14" xr:uid="{DCF42841-7DAF-D442-8729-D9AFD8CFB919}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C3" xr:uid="{8C50D541-E85D-A945-8976-CDA6FEF257BB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A3:B3" xr:uid="{FA297C0D-9B3F-4143-ABAA-C88E59DC82EA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to CLUM land use raster" prompt="File path (absolute or relative to the R working directory) to the CLUM land use raster dataset. " sqref="A4:B5 C4" xr:uid="{89F1DD56-C087-B741-90D6-12119E25CC40}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A6:C6 C5" xr:uid="{7BBE4A4D-4356-EA4C-B734-B2EFC486A03A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="A12:B12" xr:uid="{44B8137E-6468-414A-8F72-6ECBA601CC4D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="A13:B13" xr:uid="{6BE692C5-F093-9B43-81FD-F9994EBCCEB3}"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="A14" xr:uid="{E99175B9-ED04-A14B-933C-B0BB7A9E97C2}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A3:B5" xr:uid="{FA297C0D-9B3F-4143-ABAA-C88E59DC82EA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to CLUM land use raster" prompt="File path (absolute or relative to the R working directory) to the CLUM land use raster dataset. " sqref="A6:B7 C6" xr:uid="{89F1DD56-C087-B741-90D6-12119E25CC40}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A8:C8 C7" xr:uid="{7BBE4A4D-4356-EA4C-B734-B2EFC486A03A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="A14:B14" xr:uid="{44B8137E-6468-414A-8F72-6ECBA601CC4D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="A15:B15" xr:uid="{6BE692C5-F093-9B43-81FD-F9994EBCCEB3}"/>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="A16" xr:uid="{E99175B9-ED04-A14B-933C-B0BB7A9E97C2}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total returning" error="Must be a whole number greater than or equal to 0." promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="C15" xr:uid="{473EE1A2-8E34-0B49-BAAC-16B7AB92D855}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total returning" error="Must be a whole number greater than or equal to 0." promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="C17" xr:uid="{473EE1A2-8E34-0B49-BAAC-16B7AB92D855}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="A16" xr:uid="{F32F3253-DAE6-2F4C-97B8-67E94B64D310}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total mail volume" prompt="Total number of mail items." sqref="A17:B17" xr:uid="{C8354B7F-2B29-F74A-A253-E26E4586F6DF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="A18:B18" xr:uid="{F14EE191-4689-1A47-BC93-2058938AF449}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="A19:B19" xr:uid="{C76B17BB-B0E2-884D-9EEE-127080AE7513}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="A20:B20" xr:uid="{07B35AE6-1FD0-A246-A699-4A228631433F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="A21 B21" xr:uid="{37AE5199-8030-F14C-89C0-9E545DAB410D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="B23" xr:uid="{FEDA9928-A834-F34C-8C33-9B203A66F7DD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to postal areas shapefile" prompt="File path (absolute or relative to the R working directory) to the postal areas shapefile (e.g. the path to POA_2011_AUST.shp)." sqref="A7:C7" xr:uid="{6BB1B62B-72FC-1249-82C1-17CA3D520CA6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to marine ports data" prompt="File path (absolute or relative to the R working directory) to a csv containing location information for marine ports." sqref="A9:C9" xr:uid="{DE662AD5-4431-DB43-9BDC-06A1A22D78D0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to fertiliser data" prompt="File path (absolute or relative to the R working directory) to a csv containing information about fertiliser usage by NRM." sqref="A10:C10" xr:uid="{D2DEC716-59BE-0241-9E4B-D7A33D079805}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NRM shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of NRMs (natural resource management areas)." sqref="A11:C11" xr:uid="{B16F0D1B-C53A-1D4E-8F1B-5DB6B9B8000E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to container data" prompt="File path (absolute or relative to the R working directory) to the dataset giving the distribution of containers by postcode." sqref="A8:C8" xr:uid="{CD6207FA-8833-374E-BF26-EE9A3C3ECC9E}"/>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="B14" xr:uid="{0ADB052B-600C-6646-B667-C3AF149E1A46}"/>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="A15:B15 B16" xr:uid="{6E17E750-03CF-6B47-B6A7-4B91C120696F}"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total tourists" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="C14" xr:uid="{402F080D-8C8E-5041-BC08-0DF01A3C9FA7}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="A18" xr:uid="{F32F3253-DAE6-2F4C-97B8-67E94B64D310}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total mail volume" prompt="Total number of mail items." sqref="A19:B19" xr:uid="{C8354B7F-2B29-F74A-A253-E26E4586F6DF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="A20:B20" xr:uid="{F14EE191-4689-1A47-BC93-2058938AF449}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="A21:B21" xr:uid="{C76B17BB-B0E2-884D-9EEE-127080AE7513}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="A22:B22" xr:uid="{07B35AE6-1FD0-A246-A699-4A228631433F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="A23:B23" xr:uid="{37AE5199-8030-F14C-89C0-9E545DAB410D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="A25:B25" xr:uid="{FEDA9928-A834-F34C-8C33-9B203A66F7DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to postal areas shapefile" prompt="File path (absolute or relative to the R working directory) to the postal areas shapefile (e.g. the path to POA_2011_AUST.shp)." sqref="A9:C9" xr:uid="{6BB1B62B-72FC-1249-82C1-17CA3D520CA6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to marine ports data" prompt="File path (absolute or relative to the R working directory) to a csv containing location information for marine ports." sqref="A11:C11" xr:uid="{DE662AD5-4431-DB43-9BDC-06A1A22D78D0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to fertiliser data" prompt="File path (absolute or relative to the R working directory) to a csv containing information about fertiliser usage by NRM." sqref="A12:C12" xr:uid="{D2DEC716-59BE-0241-9E4B-D7A33D079805}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NRM shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of NRMs (natural resource management areas)." sqref="A13:C13" xr:uid="{B16F0D1B-C53A-1D4E-8F1B-5DB6B9B8000E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to container data" prompt="File path (absolute or relative to the R working directory) to the dataset giving the distribution of containers by postcode." sqref="A10:C10" xr:uid="{CD6207FA-8833-374E-BF26-EE9A3C3ECC9E}"/>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="B16" xr:uid="{0ADB052B-600C-6646-B667-C3AF149E1A46}"/>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="A17:B17 B18" xr:uid="{6E17E750-03CF-6B47-B6A7-4B91C120696F}"/>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total tourists" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="C16" xr:uid="{402F080D-8C8E-5041-BC08-0DF01A3C9FA7}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total TSI" error="Must be a whole number greater than or equal to 0." promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="C16" xr:uid="{68D2826B-F784-FB49-9A54-A8EAF661542F}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total TSI" error="Must be a whole number greater than or equal to 0." promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="C18" xr:uid="{68D2826B-F784-FB49-9A54-A8EAF661542F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total mail" error="Must be a whole number greater than or equal to 0." promptTitle="Total mail volume" prompt="Total number of mail items." sqref="C17" xr:uid="{18A343C3-CE29-394F-B22D-4068C3DCCB49}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total mail" error="Must be a whole number greater than or equal to 0." promptTitle="Total mail volume" prompt="Total number of mail items." sqref="C19" xr:uid="{18A343C3-CE29-394F-B22D-4068C3DCCB49}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total vessels" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="C18" xr:uid="{7223FA03-7E77-B141-919A-28A1A4DD82AA}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total vessels" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="C20" xr:uid="{7223FA03-7E77-B141-919A-28A1A4DD82AA}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total fertiliser" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="C19" xr:uid="{1D00A6B6-7558-1B44-9FBD-AAB9D2E4629D}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total fertiliser" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="C21" xr:uid="{1D00A6B6-7558-1B44-9FBD-AAB9D2E4629D}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total machinery" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="C20" xr:uid="{7F42D11B-64A6-B944-BFF6-9A461C0BC1DE}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total machinery" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="C22" xr:uid="{7F42D11B-64A6-B944-BFF6-9A461C0BC1DE}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="C21" xr:uid="{DBAF1735-E114-6543-8269-DA7DAB886E5F}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="C23" xr:uid="{DBAF1735-E114-6543-8269-DA7DAB886E5F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total food" error="Must be a whole number greater than or equal to 0." promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="C23" xr:uid="{6E1746A6-DD63-C74D-95D0-29665BEEA790}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total food" error="Must be a whole number greater than or equal to 0." promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="C25" xr:uid="{6E1746A6-DD63-C74D-95D0-29665BEEA790}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="A22 B22" xr:uid="{C683FAD7-D8F5-9B45-98D1-5122B274E181}"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="C22" xr:uid="{43C580EA-AEDD-714E-824E-A451E2FD49DB}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="A24:B24" xr:uid="{C683FAD7-D8F5-9B45-98D1-5122B274E181}"/>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="C24" xr:uid="{43C580EA-AEDD-714E-824E-A451E2FD49DB}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="A23" xr:uid="{C42AF866-7646-4545-9743-6D0E0F0424D5}"/>
+    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="Username for GBIF account." sqref="C4" xr:uid="{8AF21302-064F-CB44-84F8-4E168B33F793}"/>
+    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="Password for GBIF account" sqref="C5" xr:uid="{9EC30B5B-A390-E84A-8933-18BCFB49B347}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="27" id="{A5F1242E-CF9A-DF46-B2F9-C5F7D9A46378}">
-            <xm:f>AND(ISBLANK($C$12), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C12</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="26" id="{06CC7A14-EECC-3048-BA79-B1A22164FD81}">
-            <xm:f>AND(ISBLANK($C$13), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="25" id="{BC74A6DF-154E-D549-AE49-D9A1F984125A}">
+          <x14:cfRule type="expression" priority="29" id="{A5F1242E-CF9A-DF46-B2F9-C5F7D9A46378}">
             <xm:f>AND(ISBLANK($C$14), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
@@ -2540,8 +2611,8 @@
           <xm:sqref>C14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="24" id="{504020AB-E4E7-0C40-8B68-A8312B9335F0}">
-            <xm:f>AND(ISBLANK($C$15), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "resident" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="28" id="{06CC7A14-EECC-3048-BA79-B1A22164FD81}">
+            <xm:f>AND(ISBLANK($C$15), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2556,8 +2627,8 @@
           <xm:sqref>C15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="23" id="{A0D7CB4F-10C8-EB4B-8494-F93073ED80A6}">
-            <xm:f>AND(ISBLANK($C$16), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="27" id="{BC74A6DF-154E-D549-AE49-D9A1F984125A}">
+            <xm:f>AND(ISBLANK($C$16), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2572,8 +2643,8 @@
           <xm:sqref>C16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="22" id="{73FA8A37-CB62-6949-9E4D-54FB9B4696DD}">
-            <xm:f>AND(ISBLANK($C$17), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "mail" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="26" id="{504020AB-E4E7-0C40-8B68-A8312B9335F0}">
+            <xm:f>AND(ISBLANK($C$17), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "resident" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2588,8 +2659,8 @@
           <xm:sqref>C17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="21" id="{DD621A04-C852-B94A-82F0-3F0BD93D3E43}">
-            <xm:f>AND(ISBLANK($C$18), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="25" id="{A0D7CB4F-10C8-EB4B-8494-F93073ED80A6}">
+            <xm:f>AND(ISBLANK($C$18), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2604,8 +2675,8 @@
           <xm:sqref>C18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="20" id="{86733FA6-7E7C-FC41-9F36-034977C77A1A}">
-            <xm:f>AND(ISBLANK($C$19), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="24" id="{73FA8A37-CB62-6949-9E4D-54FB9B4696DD}">
+            <xm:f>AND(ISBLANK($C$19), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "mail" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2620,8 +2691,8 @@
           <xm:sqref>C19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="19" id="{9FB9DB6A-0F94-9047-B0C2-E98EB38564FB}">
-            <xm:f>AND(ISBLANK($C$20), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "machine" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="23" id="{DD621A04-C852-B94A-82F0-3F0BD93D3E43}">
+            <xm:f>AND(ISBLANK($C$20), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2636,8 +2707,8 @@
           <xm:sqref>C20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="18" id="{E686E863-6F44-FE48-AE94-19AC4F3E9D3E}">
-            <xm:f>AND(ISBLANK($C$21), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "nursery" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="22" id="{86733FA6-7E7C-FC41-9F36-034977C77A1A}">
+            <xm:f>AND(ISBLANK($C$21), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2649,11 +2720,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C21:C22</xm:sqref>
+          <xm:sqref>C21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="17" id="{5347420B-A3B2-5A47-BB20-A3048FE54346}">
-            <xm:f>AND(ISBLANK($C$23), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "food" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="21" id="{9FB9DB6A-0F94-9047-B0C2-E98EB38564FB}">
+            <xm:f>AND(ISBLANK($C$22), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "machine" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2665,11 +2736,43 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C23</xm:sqref>
+          <xm:sqref>C22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="15" id="{41CEDCF0-5684-1847-B5BF-7ECDF326BB08}">
-            <xm:f>AND(ISBLANK($C$6),MATCH(TRUE,'Species-specific parameters'!$D:$D)&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="20" id="{E686E863-6F44-FE48-AE94-19AC4F3E9D3E}">
+            <xm:f>AND(ISBLANK($C$23), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "nursery" &amp; "*")&gt;0)</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C23:C24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="19" id="{5347420B-A3B2-5A47-BB20-A3048FE54346}">
+            <xm:f>AND(ISBLANK($C$25), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "food" &amp; "*")&gt;0)</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="17" id="{41CEDCF0-5684-1847-B5BF-7ECDF326BB08}">
+            <xm:f>AND(ISBLANK($C$8),MATCH(TRUE,'Species-specific parameters'!$D:$D)&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2678,11 +2781,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{029B3FA2-6D08-774A-A3AF-AF5C6DDA3389}">
-            <xm:f>AND(ISBLANK($C$9),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="5" id="{029B3FA2-6D08-774A-A3AF-AF5C6DDA3389}">
+            <xm:f>AND(ISBLANK($C$11),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2691,11 +2794,50 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C9</xm:sqref>
+          <xm:sqref>C11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{C1562361-73C7-0F4C-BE7B-829A5FC5A252}">
-            <xm:f>AND(ISBLANK($C$10),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="11" id="{C1562361-73C7-0F4C-BE7B-829A5FC5A252}">
+            <xm:f>AND(ISBLANK($C$12),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="9" id="{46D2826F-1D36-DD45-AF77-2CEFFD3FCCD2}">
+            <xm:f>AND(ISBLANK($C$13),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="7" id="{8B68D8F3-6E1D-9F41-B671-5026551F9C89}">
+            <xm:f>AND(ISBLANK($C$7),MATCH(TRUE,'Species-specific parameters'!E:E)&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="6" id="{BAC6748B-F327-CE42-8857-5D92456E4AB3}">
+            <xm:f>AND(ISBLANK($C$10),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2707,8 +2849,8 @@
           <xm:sqref>C10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{46D2826F-1D36-DD45-AF77-2CEFFD3FCCD2}">
-            <xm:f>AND(ISBLANK($C$11),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+          <x14:cfRule type="expression" priority="3" id="{4A75E809-16D5-604D-8D4E-510A397A1296}">
+            <xm:f>AND(ISBLANK($C$9),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2717,46 +2859,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{8B68D8F3-6E1D-9F41-B671-5026551F9C89}">
-            <xm:f>AND(ISBLANK($C$5),MATCH(TRUE,'Species-specific parameters'!E:E)&gt;0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{BAC6748B-F327-CE42-8857-5D92456E4AB3}">
-            <xm:f>AND(ISBLANK($C$8),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{4A75E809-16D5-604D-8D4E-510A397A1296}">
-            <xm:f>AND(ISBLANK($C$7),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3291,14 +3394,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X1048576">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>NOT(ISNUMBER(SEARCH("food", $B2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(ISNUMBER(SEARCH("food",$B2)), ISBLANK($X2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>NOT(ISNUMBER(SEARCH("food", $B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="48">
+  </conditionalFormatting>
+  <dataValidations count="47">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="F1" xr:uid="{610A6EDE-65F2-9448-845D-1D9D26647888}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A1" xr:uid="{AD160B45-C62D-E948-B89F-CBE0E706C1DD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C1" xr:uid="{8A54E1E1-25E5-4A4C-A35B-02A189BDAE39}"/>
@@ -3354,7 +3457,7 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="GBIF maximum uncertainty" prompt="Highest tolerable coordinate uncertainty (in metres) when downloading GBIF occurrence data." sqref="J2:K1048576" xr:uid="{6FD266E6-D30F-E140-8841-0CC016C4626A}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Entry pathways" prompt="Comma-separated entry pathways. Can be one or more of: containers, fertiliser, food, goods, machinery, mail, nursery, residents, torres, tourists, vessels." sqref="B2:B1048576" xr:uid="{0A63DA24-38A1-3843-A720-47364E20527C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Entry pathways" prompt="Comma-separated entry pathways. Can be one or more of: containers, fertiliser, food, goods, machinery, mail, nursery, residents, torres, tourists, vessels." sqref="B1:B1048576" xr:uid="{0A63DA24-38A1-3843-A720-47364E20527C}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="E2:E1048576" xr:uid="{9BD9BDED-3BB9-CE48-804B-E25C909FAD17}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -3389,7 +3492,6 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="X2:X1048576" xr:uid="{38477FC1-7814-BD4C-B77B-1DF8DEB88B39}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Entry pathways" prompt="Comma-separated entry pathways. Can be one or more of: containers, fertiliser, food, goods, machinery, mail, nursery, residents, torres, tourists, vessels." sqref="B1" xr:uid="{5889E747-253F-734B-BB7B-A11D6893348C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add grouping column to xlsx file, summarise groups to medians
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/edmaps-github/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6196267C-8105-4742-B409-1A5F0F5575F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BDB3EE-DED2-4C4C-9B31-9481545CDCCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{236919D7-CD01-A940-BDF2-FF56F5903D66}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>risk_layers/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
   </si>
@@ -699,6 +699,9 @@
   </si>
   <si>
     <t>Password for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
+  </si>
+  <si>
+    <t>Species group</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1315,11 +1318,32 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2175,7 +2199,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2470,57 +2494,57 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="containsBlanks" dxfId="67" priority="33">
+    <cfRule type="containsBlanks" dxfId="69" priority="33">
       <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="66" priority="31">
+    <cfRule type="containsBlanks" dxfId="68" priority="31">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="65" priority="18">
+    <cfRule type="expression" dxfId="67" priority="18">
       <formula>ISBLANK($C$8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="64" priority="14">
+    <cfRule type="expression" dxfId="66" priority="14">
       <formula>ISBLANK($C$12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="63" priority="10">
+    <cfRule type="expression" dxfId="65" priority="10">
       <formula>ISBLANK($C$13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="62" priority="15">
+    <cfRule type="expression" dxfId="64" priority="15">
       <formula>ISBLANK($C$11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="61" priority="8">
+    <cfRule type="expression" dxfId="63" priority="8">
       <formula>ISBLANK($C$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="60" priority="16">
+    <cfRule type="expression" dxfId="62" priority="16">
       <formula>ISBLANK($C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="59" priority="4">
+    <cfRule type="expression" dxfId="61" priority="4">
       <formula>ISBLANK($C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="60" priority="2">
       <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="57" priority="1">
+    <cfRule type="expression" dxfId="59" priority="1">
       <formula>AND(NOT(ISBLANK($C$5)), ISBLANK($C$4))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2596,7 +2620,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="29" id="{A5F1242E-CF9A-DF46-B2F9-C5F7D9A46378}">
-            <xm:f>AND(ISBLANK($C$14), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$14), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2612,7 +2636,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="28" id="{06CC7A14-EECC-3048-BA79-B1A22164FD81}">
-            <xm:f>AND(ISBLANK($C$15), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$15), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2628,7 +2652,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="27" id="{BC74A6DF-154E-D549-AE49-D9A1F984125A}">
-            <xm:f>AND(ISBLANK($C$16), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$16), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "tourist" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2644,7 +2668,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="26" id="{504020AB-E4E7-0C40-8B68-A8312B9335F0}">
-            <xm:f>AND(ISBLANK($C$17), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "resident" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$17), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "resident" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2660,7 +2684,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="25" id="{A0D7CB4F-10C8-EB4B-8494-F93073ED80A6}">
-            <xm:f>AND(ISBLANK($C$18), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$18), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "torres" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2676,7 +2700,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="24" id="{73FA8A37-CB62-6949-9E4D-54FB9B4696DD}">
-            <xm:f>AND(ISBLANK($C$19), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "mail" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$19), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "mail" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2692,7 +2716,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="23" id="{DD621A04-C852-B94A-82F0-3F0BD93D3E43}">
-            <xm:f>AND(ISBLANK($C$20), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$20), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2708,7 +2732,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="22" id="{86733FA6-7E7C-FC41-9F36-034977C77A1A}">
-            <xm:f>AND(ISBLANK($C$21), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$21), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2724,7 +2748,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="21" id="{9FB9DB6A-0F94-9047-B0C2-E98EB38564FB}">
-            <xm:f>AND(ISBLANK($C$22), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "machine" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$22), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "machine" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2740,7 +2764,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="20" id="{E686E863-6F44-FE48-AE94-19AC4F3E9D3E}">
-            <xm:f>AND(ISBLANK($C$23), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "nursery" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$23), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "nursery" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2756,7 +2780,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="19" id="{5347420B-A3B2-5A47-BB20-A3048FE54346}">
-            <xm:f>AND(ISBLANK($C$25), COUNTIF('Species-specific parameters'!B:B,"*" &amp; "food" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$25), COUNTIF('Species-specific parameters'!C:C,"*" &amp; "food" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2772,7 +2796,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="17" id="{41CEDCF0-5684-1847-B5BF-7ECDF326BB08}">
-            <xm:f>AND(ISBLANK($C$8),MATCH(TRUE,'Species-specific parameters'!$D:$D)&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$8),MATCH(TRUE,'Species-specific parameters'!$E:$E)&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2785,7 +2809,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="5" id="{029B3FA2-6D08-774A-A3AF-AF5C6DDA3389}">
-            <xm:f>AND(ISBLANK($C$11),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$11),COUNTIF('Species-specific parameters'!C:C,"*" &amp; "vessel" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2798,7 +2822,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="11" id="{C1562361-73C7-0F4C-BE7B-829A5FC5A252}">
-            <xm:f>AND(ISBLANK($C$12),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$12),COUNTIF('Species-specific parameters'!C:C,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2811,7 +2835,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{46D2826F-1D36-DD45-AF77-2CEFFD3FCCD2}">
-            <xm:f>AND(ISBLANK($C$13),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$13),COUNTIF('Species-specific parameters'!C:C,"*" &amp; "fert" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2824,7 +2848,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{8B68D8F3-6E1D-9F41-B671-5026551F9C89}">
-            <xm:f>AND(ISBLANK($C$7),MATCH(TRUE,'Species-specific parameters'!E:E)&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$7),MATCH(TRUE,'Species-specific parameters'!F:F)&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2837,7 +2861,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="6" id="{BAC6748B-F327-CE42-8857-5D92456E4AB3}">
-            <xm:f>AND(ISBLANK($C$10),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$10),COUNTIF('Species-specific parameters'!C:C,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2850,7 +2874,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{4A75E809-16D5-604D-8D4E-510A397A1296}">
-            <xm:f>AND(ISBLANK($C$9),COUNTIF('Species-specific parameters'!B:B,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
+            <xm:f>AND(ISBLANK($C$9),COUNTIF('Species-specific parameters'!C:C,"*" &amp; "container" &amp; "*")&gt;0)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2870,7 +2894,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D738B5-D0EE-C044-83A0-D9C8F02CE7C0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2882,184 +2906,187 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="8"/>
-    <col min="9" max="9" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.5" style="8"/>
-    <col min="12" max="12" width="21.5" style="10" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="10" customWidth="1"/>
-    <col min="14" max="14" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" style="12" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.5" style="11"/>
-    <col min="24" max="24" width="12.1640625" style="11" customWidth="1"/>
-    <col min="25" max="25" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14" style="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5" style="30"/>
-    <col min="28" max="16384" width="16.5" style="10"/>
+    <col min="2" max="2" width="14.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="10" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="8"/>
+    <col min="10" max="10" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.5" style="8"/>
+    <col min="13" max="13" width="21.5" style="10" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="10" customWidth="1"/>
+    <col min="15" max="15" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" style="12" customWidth="1"/>
+    <col min="21" max="21" width="12.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.5" style="11"/>
+    <col min="25" max="25" width="12.1640625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5" style="30"/>
+    <col min="29" max="16384" width="16.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="38" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="38" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="P1" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="U1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="W1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="X1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="Y1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Z1" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="AA1" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="16" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="17" t="b">
-        <v>1</v>
       </c>
       <c r="D2" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18">
+      <c r="J2" s="18">
         <v>1970</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="17"/>
       <c r="M2" s="17"/>
-      <c r="N2" s="19">
+      <c r="N2" s="17"/>
+      <c r="O2" s="19">
         <f>0.000002381577*30/45</f>
         <v>1.5877180000000001E-6</v>
       </c>
-      <c r="O2" s="19">
+      <c r="P2" s="19">
         <f>0.000002381577*15/45</f>
         <v>7.9385900000000007E-7</v>
       </c>
-      <c r="P2" s="19">
+      <c r="Q2" s="19">
         <f>21/51000</f>
         <v>4.1176470588235296E-4</v>
       </c>
-      <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="20"/>
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
       <c r="X2" s="19"/>
       <c r="Y2" s="19"/>
-      <c r="Z2" s="21">
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="21">
         <v>5000</v>
       </c>
-      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
     </row>
-    <row r="3" spans="1:27" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="4" t="b">
-        <v>0</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>0</v>
@@ -3067,58 +3094,59 @@
       <c r="E3" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
-      <c r="N3" s="5">
+      <c r="L3" s="2"/>
+      <c r="O3" s="5">
         <f>0.000001640642*30/45</f>
         <v>1.0937613333333331E-6</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="5">
         <f>0.000001640642*15/45</f>
         <v>5.4688066666666656E-7</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5">
         <f>0.00000007971014</f>
         <v>7.9710139999999995E-8</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S3" s="5">
         <f>3/18612</f>
         <v>1.6118633139909736E-4</v>
       </c>
-      <c r="S3" s="6">
+      <c r="T3" s="6">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
-      <c r="T3" s="5">
+      <c r="U3" s="5">
         <f>3/6907</f>
         <v>4.3434197191255248E-4</v>
       </c>
-      <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="13">
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="13">
         <v>5000</v>
       </c>
-      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
     </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="4" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="4" t="b">
-        <v>1</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>1</v>
@@ -3126,370 +3154,385 @@
       <c r="E4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>1970</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="5">
+      <c r="R4" s="5"/>
+      <c r="S4" s="5">
         <f>0.643/18612</f>
         <v>3.4547603696539868E-5</v>
       </c>
-      <c r="S4" s="6">
+      <c r="T4" s="6">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5">
+      <c r="U4" s="5"/>
+      <c r="V4" s="5">
         <f>14/1216726</f>
         <v>1.150628818649392E-5</v>
       </c>
-      <c r="V4" s="5">
+      <c r="W4" s="5">
         <f>2/2717750</f>
         <v>7.3590286082237149E-7</v>
       </c>
-      <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="13">
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="13">
         <v>5000</v>
       </c>
-      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
     </row>
-    <row r="5" spans="1:27" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C5" s="4" t="b">
-        <v>1</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <f>0.000002381577*30/45</f>
         <v>1.5877180000000001E-6</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <f>0.000002381577*15/45</f>
         <v>7.9385900000000007E-7</v>
       </c>
-      <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5">
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
         <f>0.002/1216726</f>
         <v>1.643755455213417E-9</v>
       </c>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5">
+      <c r="W5" s="5"/>
+      <c r="X5" s="5">
         <f>2/4475</f>
         <v>4.4692737430167598E-4</v>
       </c>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5">
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5">
         <f>2/15832</f>
         <v>1.2632642748863063E-4</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="AA5" s="13">
         <v>5000</v>
       </c>
-      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="expression" dxfId="40" priority="6">
+      <formula>$F2=FALSE</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="71">
+      <formula>ISBLANK($H2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="expression" dxfId="38" priority="4">
-      <formula>$E2=FALSE</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="69">
+    <cfRule type="expression" dxfId="38" priority="84">
       <formula>ISBLANK($G2)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I1048576 K2:K1048576 M2:M1048576">
+    <cfRule type="expression" dxfId="37" priority="111">
+      <formula>AND(ISBLANK($I2), ISBLANK($K2), ISBLANK($M2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J1048576">
+    <cfRule type="expression" dxfId="36" priority="19">
+      <formula>ISBLANK($I2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L1048576">
+    <cfRule type="expression" dxfId="35" priority="43">
+      <formula>OR($D2=FALSE, AND(ISBLANK($I2), ISBLANK($K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:T1048576">
+    <cfRule type="expression" dxfId="34" priority="13">
+      <formula>NOT(ISNUMBER(SEARCH("vessels", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="286">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($T2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M1048576">
+    <cfRule type="expression" dxfId="32" priority="30">
+      <formula>OR(ISBLANK($A2),$D2=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:L1048576 N2:N1048576">
+    <cfRule type="expression" dxfId="31" priority="309">
+      <formula>NOT(ISBLANK($M2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P1048576">
+    <cfRule type="expression" dxfId="30" priority="17">
+      <formula>NOT(ISNUMBER(SEARCH("residents", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="159">
+      <formula>AND(ISNUMBER(SEARCH("residents",$C2)), ISBLANK($P2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q1048576">
+    <cfRule type="expression" dxfId="28" priority="16">
+      <formula>NOT(ISNUMBER(SEARCH("torres", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="310">
+      <formula>AND(ISNUMBER(SEARCH("torres",$C2)), ISBLANK($Q2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R1048576">
+    <cfRule type="expression" dxfId="26" priority="15">
+      <formula>NOT(ISNUMBER(SEARCH("mail", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="311">
+      <formula>AND(SEARCH("mail",$C2), ISBLANK($R2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S1048576">
+    <cfRule type="expression" dxfId="24" priority="14">
+      <formula>NOT(ISNUMBER(SEARCH("vessels", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="313">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($S2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U1048576">
+    <cfRule type="expression" dxfId="22" priority="12">
+      <formula>NOT(ISNUMBER(SEARCH("fert", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="314">
+      <formula>AND(ISNUMBER(SEARCH("fert",$C2)), ISBLANK($U2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:V1048576">
+    <cfRule type="expression" dxfId="20" priority="11">
+      <formula>NOT(ISNUMBER(SEARCH("machine", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="315">
+      <formula>AND(ISNUMBER(SEARCH("machine",$C2)), ISBLANK($V2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:W1048576">
+    <cfRule type="expression" dxfId="18" priority="10">
+      <formula>NOT(ISNUMBER(SEARCH("container", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="316">
+      <formula>AND(ISNUMBER(SEARCH("container",$C2)), ISBLANK($W2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z2:Z1048576">
+    <cfRule type="expression" dxfId="16" priority="8">
+      <formula>NOT(ISNUMBER(SEARCH("goods", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="318">
+      <formula>AND(ISNUMBER(SEARCH("goods",$C2)), ISBLANK($Z2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O1048576">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>NOT(ISNUMBER(SEARCH("tourists",$C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="29">
+      <formula>AND(ISNUMBER(SEARCH("tourists",$C2)), ISBLANK($O2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
+    <cfRule type="expression" dxfId="12" priority="28">
+      <formula>OR(ISBLANK($A4), $D4=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C1048576">
+    <cfRule type="expression" dxfId="11" priority="25">
+      <formula>ISBLANK($C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:AA1048576 A2:A5 C2:AA5">
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>ISBLANK($A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="expression" dxfId="9" priority="24">
+      <formula>ISBLANK($D2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="expression" dxfId="8" priority="26">
+      <formula>ISBLANK($E2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="expression" dxfId="36" priority="82">
+    <cfRule type="expression" dxfId="7" priority="22">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1048576 J2:J1048576 L2:L1048576">
-    <cfRule type="expression" dxfId="35" priority="109">
-      <formula>AND(ISBLANK($H2), ISBLANK($J2), ISBLANK($L2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="expression" dxfId="34" priority="17">
-      <formula>ISBLANK($H2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K1048576">
-    <cfRule type="expression" dxfId="33" priority="41">
-      <formula>OR($C2=FALSE, AND(ISBLANK($H2), ISBLANK($J2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S1048576">
-    <cfRule type="expression" dxfId="32" priority="11">
-      <formula>NOT(ISNUMBER(SEARCH("vessels", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="284">
-      <formula>AND(ISNUMBER(SEARCH("vessels",$B2)), ISBLANK($S2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="expression" dxfId="30" priority="28">
-      <formula>OR(ISBLANK($A2),$C2=FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:K1048576 M2:M1048576">
-    <cfRule type="expression" dxfId="29" priority="307">
-      <formula>NOT(ISBLANK($L2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="expression" dxfId="28" priority="15">
-      <formula>NOT(ISNUMBER(SEARCH("residents", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="157">
-      <formula>AND(ISNUMBER(SEARCH("residents",$B2)), ISBLANK($O2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P1048576">
-    <cfRule type="expression" dxfId="26" priority="14">
-      <formula>NOT(ISNUMBER(SEARCH("torres", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="308">
-      <formula>AND(ISNUMBER(SEARCH("torres",$B2)), ISBLANK($P2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q1048576">
-    <cfRule type="expression" dxfId="24" priority="13">
-      <formula>NOT(ISNUMBER(SEARCH("mail", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="309">
-      <formula>AND(SEARCH("mail",$B2), ISBLANK($Q2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R1048576">
-    <cfRule type="expression" dxfId="22" priority="12">
-      <formula>NOT(ISNUMBER(SEARCH("vessels", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="311">
-      <formula>AND(ISNUMBER(SEARCH("vessels",$B2)), ISBLANK($R2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T1048576">
-    <cfRule type="expression" dxfId="20" priority="10">
-      <formula>NOT(ISNUMBER(SEARCH("fert", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="312">
-      <formula>AND(ISNUMBER(SEARCH("fert",$B2)), ISBLANK($T2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U1048576">
-    <cfRule type="expression" dxfId="18" priority="9">
-      <formula>NOT(ISNUMBER(SEARCH("machine", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="313">
-      <formula>AND(ISNUMBER(SEARCH("machine",$B2)), ISBLANK($U2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V1048576">
-    <cfRule type="expression" dxfId="16" priority="8">
-      <formula>NOT(ISNUMBER(SEARCH("container", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="314">
-      <formula>AND(ISNUMBER(SEARCH("container",$B2)), ISBLANK($V2))</formula>
+  <conditionalFormatting sqref="I2:N1048576">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>$D2=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X2:X1048576">
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>NOT(ISNUMBER(SEARCH("nursery", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="317">
+      <formula>AND(ISNUMBER(SEARCH("nursery",$C2)), ISBLANK($X2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y1048576">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>NOT(ISNUMBER(SEARCH("goods", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="316">
-      <formula>AND(ISNUMBER(SEARCH("goods",$B2)), ISBLANK($Y2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>NOT(ISNUMBER(SEARCH("tourists",$B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="27">
-      <formula>AND(ISNUMBER(SEARCH("tourists",$B2)), ISBLANK($N2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="10" priority="26">
-      <formula>OR(ISBLANK($A4), $C4=FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="9" priority="23">
-      <formula>ISBLANK($B2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:Z1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>NOT(ISNUMBER(SEARCH("food", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND(ISNUMBER(SEARCH("food",$C2)), ISBLANK($Y2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ISBLANK($A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="7" priority="22">
-      <formula>ISBLANK($C2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="expression" dxfId="6" priority="24">
-      <formula>ISBLANK($D2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="5" priority="20">
-      <formula>ISBLANK($E2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M1048576">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$C2=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W1048576">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>NOT(ISNUMBER(SEARCH("nursery", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="315">
-      <formula>AND(ISNUMBER(SEARCH("nursery",$B2)), ISBLANK($W2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>NOT(ISNUMBER(SEARCH("food", $B2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISNUMBER(SEARCH("food",$B2)), ISBLANK($X2))</formula>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK($A5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="47">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="F1" xr:uid="{610A6EDE-65F2-9448-845D-1D9D26647888}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A1" xr:uid="{AD160B45-C62D-E948-B89F-CBE0E706C1DD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C1" xr:uid="{8A54E1E1-25E5-4A4C-A35B-02A189BDAE39}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="D1" xr:uid="{74C7EF83-30DD-F948-9522-90AFB2FCEC74}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="E1" xr:uid="{893B753C-83F4-644D-BD7E-F6B39072EB1E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="G1" xr:uid="{41980E33-1E39-AD45-8F05-868D6600E067}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF minimum year" prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="I1" xr:uid="{A33E5C3F-FEB5-E142-9E77-829BE9CDC095}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="N1" xr:uid="{7D0C5A9D-2B24-5E4B-B142-62EC654E71D3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="O1" xr:uid="{BFE515ED-E47C-8E4A-A50B-35E2286ACF32}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="P1" xr:uid="{0A697F1D-F494-C347-95D9-E59F4C6C383A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="Q1" xr:uid="{399C1480-40E4-5A41-A2FF-2E4F826C4DEE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="R1" xr:uid="{1BBA7A75-F6E1-4F47-BC5E-4B3FDC509E65}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="S1" xr:uid="{12F7F3FA-47A2-8B43-B105-3D925A1D9D46}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="T1" xr:uid="{14C39FAF-9B97-1543-B73A-260E86BB654B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="U1" xr:uid="{9FFB111A-9910-744C-B50F-00F7A89B9CA3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="V1" xr:uid="{E6D7E48A-15CD-1A4F-BAD7-13A132F3D69F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="W1" xr:uid="{34153A47-9E0E-4F4D-B565-CC6104D4CF6D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Y1" xr:uid="{DDEBC040-5553-4841-9E5B-5FB894300E90}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Name must begin with a letter or a period." promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A2:A1048576" xr:uid="{F8431168-FF74-CF44-A9C3-C9F4FDBC2E6C}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="C2:C1048576" xr:uid="{B5EAF5EE-6EE5-6B49-99E2-F42D5D06C580}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="G1" xr:uid="{610A6EDE-65F2-9448-845D-1D9D26647888}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A1:B1" xr:uid="{AD160B45-C62D-E948-B89F-CBE0E706C1DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="D1" xr:uid="{8A54E1E1-25E5-4A4C-A35B-02A189BDAE39}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="E1" xr:uid="{74C7EF83-30DD-F948-9522-90AFB2FCEC74}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="F1" xr:uid="{893B753C-83F4-644D-BD7E-F6B39072EB1E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="H1" xr:uid="{41980E33-1E39-AD45-8F05-868D6600E067}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF minimum year" prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="J1" xr:uid="{A33E5C3F-FEB5-E142-9E77-829BE9CDC095}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="O1" xr:uid="{7D0C5A9D-2B24-5E4B-B142-62EC654E71D3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="P1" xr:uid="{BFE515ED-E47C-8E4A-A50B-35E2286ACF32}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="Q1" xr:uid="{0A697F1D-F494-C347-95D9-E59F4C6C383A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="R1" xr:uid="{399C1480-40E4-5A41-A2FF-2E4F826C4DEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="S1" xr:uid="{1BBA7A75-F6E1-4F47-BC5E-4B3FDC509E65}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="T1" xr:uid="{12F7F3FA-47A2-8B43-B105-3D925A1D9D46}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="U1" xr:uid="{14C39FAF-9B97-1543-B73A-260E86BB654B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="V1" xr:uid="{9FFB111A-9910-744C-B50F-00F7A89B9CA3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="W1" xr:uid="{E6D7E48A-15CD-1A4F-BAD7-13A132F3D69F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="X1" xr:uid="{34153A47-9E0E-4F4D-B565-CC6104D4CF6D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Z1" xr:uid="{DDEBC040-5553-4841-9E5B-5FB894300E90}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Name must begin with a letter or a period." promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A2:B1048576" xr:uid="{F8431168-FF74-CF44-A9C3-C9F4FDBC2E6C}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="D2:D1048576" xr:uid="{B5EAF5EE-6EE5-6B49-99E2-F42D5D06C580}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Expert occurrence data path" prompt="File path (absolute or relative to working directory) to occurrence dataset. Ignored if &quot;Climate suitability path&quot; is provided." sqref="J1:J1048576" xr:uid="{344DBD62-32DD-2640-814E-8FECEF8AE89F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried. Ignored if &quot;Climate suitability path&quot; is provided." sqref="H1:H1048576" xr:uid="{867EBE5D-A33C-8641-98B7-84DD0D595AEA}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="Q2:Q1048576" xr:uid="{77FCB406-D2F1-BD40-8A66-E8D4EB673AEF}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Expert occurrence data path" prompt="File path (absolute or relative to working directory) to occurrence dataset. Ignored if &quot;Climate suitability path&quot; is provided." sqref="K1:K1048576" xr:uid="{344DBD62-32DD-2640-814E-8FECEF8AE89F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried. Ignored if &quot;Climate suitability path&quot; is provided." sqref="I1:I1048576" xr:uid="{867EBE5D-A33C-8641-98B7-84DD0D595AEA}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="R2:R1048576" xr:uid="{77FCB406-D2F1-BD40-8A66-E8D4EB673AEF}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="R2:R1048576" xr:uid="{1C090300-AE72-0642-8D47-2A8F62A6DE24}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="S2:S1048576" xr:uid="{1C090300-AE72-0642-8D47-2A8F62A6DE24}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a negative number." promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="S2:S1048576" xr:uid="{A3790EC7-C576-B249-BCDF-06829DDB2534}">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a negative number." promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="T2:T1048576" xr:uid="{A3790EC7-C576-B249-BCDF-06829DDB2534}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="T2:T1048576" xr:uid="{68922F53-C9AE-0E41-8624-91096244AAAF}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="U2:U1048576" xr:uid="{68922F53-C9AE-0E41-8624-91096244AAAF}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="U2:U1048576" xr:uid="{27582A83-D06C-CC4A-9EC7-9633BED3D41F}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="V2:V1048576" xr:uid="{27582A83-D06C-CC4A-9EC7-9633BED3D41F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="V2:V1048576" xr:uid="{8F16EE93-B00F-524E-BFF0-7969CA884AD7}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="W2:W1048576" xr:uid="{8F16EE93-B00F-524E-BFF0-7969CA884AD7}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="W2:W1048576" xr:uid="{C098445D-3F03-A345-B8C0-17D8CCC3C159}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="X2:X1048576" xr:uid="{C098445D-3F03-A345-B8C0-17D8CCC3C159}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Y2:Y1048576" xr:uid="{F4D6DD70-484B-8F4C-8022-F92827712D2D}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Z2:Z1048576" xr:uid="{F4D6DD70-484B-8F4C-8022-F92827712D2D}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="D2:D1048576" xr:uid="{4885AF70-80FE-5741-BB46-A0C58FDF8CF8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="E2:E1048576" xr:uid="{4885AF70-80FE-5741-BB46-A0C58FDF8CF8}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Infected countries" prompt="Either a comma-separated string containing country names, or a file path (absolute or relative to working directory) to a CABI pest data sheet csv file. _x000a__x000a_If provided, occurrence records are verified against the provided data, to ensure that all records a" sqref="K1:K1048576" xr:uid="{1102FFA6-1227-9743-9757-11E831420417}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="GBIF maximum uncertainty" prompt="Highest tolerable coordinate uncertainty (in metres) when downloading GBIF occurrence data." sqref="J2:K1048576" xr:uid="{6FD266E6-D30F-E140-8841-0CC016C4626A}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Infected countries" prompt="Either a comma-separated string containing country names, or a file path (absolute or relative to working directory) to a CABI pest data sheet csv file. _x000a__x000a_If provided, occurrence records are verified against the provided data, to ensure that all records a" sqref="L1:L1048576" xr:uid="{1102FFA6-1227-9743-9757-11E831420417}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="GBIF maximum uncertainty" prompt="Highest tolerable coordinate uncertainty (in metres) when downloading GBIF occurrence data." sqref="K2:L1048576" xr:uid="{6FD266E6-D30F-E140-8841-0CC016C4626A}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Entry pathways" prompt="Comma-separated entry pathways. Can be one or more of: containers, fertiliser, food, goods, machinery, mail, nursery, residents, torres, tourists, vessels." sqref="B1:B1048576" xr:uid="{0A63DA24-38A1-3843-A720-47364E20527C}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="E2:E1048576" xr:uid="{9BD9BDED-3BB9-CE48-804B-E25C909FAD17}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Entry pathways" prompt="Comma-separated entry pathways. Can be one or more of: containers, fertiliser, food, goods, machinery, mail, nursery, residents, torres, tourists, vessels." sqref="C1:C1048576" xr:uid="{0A63DA24-38A1-3843-A720-47364E20527C}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="F2:F1048576" xr:uid="{9BD9BDED-3BB9-CE48-804B-E25C909FAD17}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be between 1800 and current year." promptTitle="GBIF minimum year " prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="I2:I1048576" xr:uid="{A9AFE441-945F-F444-97AF-D472113FEF8D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be between 1800 and current year." promptTitle="GBIF minimum year " prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="J2:J1048576" xr:uid="{A9AFE441-945F-F444-97AF-D472113FEF8D}">
       <formula1>1800</formula1>
       <formula2>YEAR(TODAY())</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest." sqref="N2:N1048576" xr:uid="{AE0D63DE-5D73-C748-BC40-4F0328B70F7F}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest." sqref="O2:O1048576" xr:uid="{AE0D63DE-5D73-C748-BC40-4F0328B70F7F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="O2:O1048576" xr:uid="{A08818E1-07F8-2947-B885-B6DCF40BE2A3}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="P2:P1048576" xr:uid="{A08818E1-07F8-2947-B885-B6DCF40BE2A3}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="P2:P1048576" xr:uid="{36BBB07A-382B-294E-8FD2-7455864CB2E2}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="Q2:Q1048576" xr:uid="{36BBB07A-382B-294E-8FD2-7455864CB2E2}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exclude BIOCLIM variables" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19)._x000a__x000a_Ignored if &quot;Climate suitability path&quot; is provided._x000a__x000a_Default: No variables are excluded." sqref="M1:M1048576" xr:uid="{A215B8BE-50BD-544B-BB88-017607D43B99}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="CABI file path" prompt="File path (absolute or relative to working directory) to the CABI csv file." sqref="F2:F1048576" xr:uid="{1CBF3D45-3CF8-6645-AD64-572A122AD92A}">
-      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(F2,ROW(INDIRECT("1:"&amp;LEN(F2))),1)," ,-:0123456789")))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 and 1:3 are equivalent to 1,2,3)." promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="F2:F1048576" xr:uid="{3F16D9CB-7B0B-584C-8750-92EBFD18A562}">
-      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(F2,ROW(INDIRECT("1:"&amp;LEN(F2))),1)," ,-:0123456789")))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="G2:G1048576" xr:uid="{D05F4B39-E78E-6A4C-9EA6-2DBD7B96B28E}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exclude BIOCLIM variables" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19)._x000a__x000a_Ignored if &quot;Climate suitability path&quot; is provided._x000a__x000a_Default: No variables are excluded." sqref="N1:N1048576" xr:uid="{A215B8BE-50BD-544B-BB88-017607D43B99}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="CABI file path" prompt="File path (absolute or relative to working directory) to the CABI csv file." sqref="G2:G1048576" xr:uid="{1CBF3D45-3CF8-6645-AD64-572A122AD92A}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(G2,ROW(INDIRECT("1:"&amp;LEN(G2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate suitability path" prompt="Optional file path to a climate suitability raster. Must be binary (0=unsuitable; 1=suitable) or describe relative suitability between 0-1. Must be 1000 m res; Australian Albers (EPSG:3577); extent xmin=-1888000; xmax=2122000; ymin=-4847000; ymax=-1010000" sqref="L1:L1048576" xr:uid="{480B32ED-B00C-3F4B-AE28-DF01A191FCC5}"/>
-    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Aggregated output resolution must be a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, the default value of 5000 will be used." sqref="Z1:Z1048576" xr:uid="{D738A470-664E-C741-8411-D92C81327D2C}">
-      <formula1>AND($Z1 &gt;= 1000, MOD($Z1, 1000)=0)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 and 1:3 are equivalent to 1,2,3)." promptTitle="CLUM v8 land use classes" prompt="Comma-separated land use classes (e.g. 340,341,342)." sqref="G2:G1048576" xr:uid="{3F16D9CB-7B0B-584C-8750-92EBFD18A562}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(G2,ROW(INDIRECT("1:"&amp;LEN(G2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="X1" xr:uid="{EA69C604-14E3-824E-AC96-8EBCAB1F127B}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="X2:X1048576" xr:uid="{38477FC1-7814-BD4C-B77B-1DF8DEB88B39}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="H2:H1048576" xr:uid="{D05F4B39-E78E-6A4C-9EA6-2DBD7B96B28E}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(H2,ROW(INDIRECT("1:"&amp;LEN(H2))),1)," ,-:0123456789")))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate suitability path" prompt="Optional file path to a climate suitability raster. Must be binary (0=unsuitable; 1=suitable) or describe relative suitability between 0-1. Must be 1000 m res; Australian Albers (EPSG:3577); extent xmin=-1888000; xmax=2122000; ymin=-4847000; ymax=-1010000" sqref="M1:M1048576" xr:uid="{480B32ED-B00C-3F4B-AE28-DF01A191FCC5}"/>
+    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Aggregated output resolution must be a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, the default value of 5000 will be used." sqref="AA1:AA1048576" xr:uid="{D738A470-664E-C741-8411-D92C81327D2C}">
+      <formula1>AND($AA1 &gt;= 1000, MOD($AA1, 1000)=0)</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="Y1" xr:uid="{EA69C604-14E3-824E-AC96-8EBCAB1F127B}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="Y2:Y1048576" xr:uid="{38477FC1-7814-BD4C-B77B-1DF8DEB88B39}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add validation for basemap_mode. Update tooltips
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/edmaps-github/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227BA7D9-A9BF-E843-9C47-18F6A36C18B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721615D5-33F6-E14C-9131-B4B323D053B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
@@ -1020,7 +1020,7 @@
     <t>Define whether maps should use OpenStreetMap ("osm") or polygon ("boundaries") basemaps.</t>
   </si>
   <si>
-    <t>boundaries</t>
+    <t>OpenStreetMap</t>
   </si>
 </sst>
 </file>
@@ -2750,7 +2750,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C7">
     <cfRule type="containsBlanks" dxfId="52" priority="11">
       <formula>LEN(TRIM(C7))=0</formula>
@@ -2861,8 +2860,10 @@
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C16" xr:uid="{74A9AB0E-B263-C746-9077-ED0626B99833}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="Username for GBIF account." sqref="C4" xr:uid="{72FDD181-E3BF-A844-A54A-B029705A8DC7}"/>
-    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="Password for GBIF account" sqref="C5:C6" xr:uid="{36FE115B-5D8C-BE47-8690-D0D99D6C9AD6}"/>
+    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C4" xr:uid="{72FDD181-E3BF-A844-A54A-B029705A8DC7}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or OpenStreetMap" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{36FE115B-5D8C-BE47-8690-D0D99D6C9AD6}">
+      <formula1>"boundaries,OpenStreetMap"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="C25" xr:uid="{2002C4F1-3088-5649-A22C-A4601DDF97D3}">
       <formula1>0</formula1>
     </dataValidation>
@@ -2871,10 +2872,10 @@
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="A26:B26" xr:uid="{8721A532-FF89-1D48-8215-293AA26D65F3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A4" xr:uid="{87006BA3-D1D7-1949-808C-03FE83C142DD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A4:B4" xr:uid="{87006BA3-D1D7-1949-808C-03FE83C142DD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A5 B5" xr:uid="{8DDA8AE4-5292-5A47-A751-FFAD9049BB67}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="B4" xr:uid="{437A1F5C-CE1B-FC49-ABAC-7CB8DA8F187B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A6 B6" xr:uid="{AFE7AC31-B1F9-7149-9143-0E28D5C59DCF}"/>
+    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C5" xr:uid="{AA10D887-7AF0-0C43-91DF-2606C73E2F37}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update OpenStreetMap basemap_mode to "osm" as per static_map
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/edmaps-github/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721615D5-33F6-E14C-9131-B4B323D053B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5086C1-F3FE-084F-A9F4-E0F986C04D7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
@@ -1020,7 +1020,7 @@
     <t>Define whether maps should use OpenStreetMap ("osm") or polygon ("boundaries") basemaps.</t>
   </si>
   <si>
-    <t>OpenStreetMap</t>
+    <t>osm</t>
   </si>
 </sst>
 </file>
@@ -2750,6 +2750,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C7">
     <cfRule type="containsBlanks" dxfId="52" priority="11">
       <formula>LEN(TRIM(C7))=0</formula>
@@ -2861,8 +2862,8 @@
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C4" xr:uid="{72FDD181-E3BF-A844-A54A-B029705A8DC7}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or OpenStreetMap" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{36FE115B-5D8C-BE47-8690-D0D99D6C9AD6}">
-      <formula1>"boundaries,OpenStreetMap"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{36FE115B-5D8C-BE47-8690-D0D99D6C9AD6}">
+      <formula1>"boundaries,osm"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="C25" xr:uid="{2002C4F1-3088-5649-A22C-A4601DDF97D3}">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
Sample probabilities from joint distribution of leakage and establishment
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/edmaps-github/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5086C1-F3FE-084F-A9F4-E0F986C04D7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E27D03-5BA6-C74F-A52A-6AC5EDA74D7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
   <sheets>
     <sheet name="Global parameters" sheetId="7" r:id="rId1"/>
@@ -35,33 +35,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={3F4991D8-F7F4-9043-8C53-522ABDB87E94}</author>
-    <author>tc={52D97D8B-AA8C-7B49-9DAC-3B43BC703016}</author>
-  </authors>
-  <commentList>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{3F4991D8-F7F4-9043-8C53-522ABDB87E94}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Modelled together to overcome potential identification problems</t>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="1" shapeId="0" xr:uid="{52D97D8B-AA8C-7B49-9DAC-3B43BC703016}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Modelled together to overcome potential identification problems</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={72FBB23E-4BBA-F24B-819F-177E1ED5B904}</author>
@@ -164,10 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="167">
-  <si>
-    <t>Citrus Canker</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="158">
   <si>
     <t>Asian Gypsy Moth</t>
   </si>
@@ -385,34 +355,7 @@
     <t>Exclude BIOCLIM vars</t>
   </si>
   <si>
-    <t>Prob tourists</t>
-  </si>
-  <si>
-    <t>Prob returning resident</t>
-  </si>
-  <si>
-    <t>Prob Torres passenger</t>
-  </si>
-  <si>
-    <t>Prob mail</t>
-  </si>
-  <si>
-    <t>Prob vessels</t>
-  </si>
-  <si>
     <t>Distance penalty (ports)</t>
-  </si>
-  <si>
-    <t>Prob fertiliser</t>
-  </si>
-  <si>
-    <t>Prob machinery</t>
-  </si>
-  <si>
-    <t>Prob containers</t>
-  </si>
-  <si>
-    <t>Prob nurserystock</t>
   </si>
   <si>
     <t>Aggregated res</t>
@@ -696,259 +639,15 @@
     </r>
   </si>
   <si>
-    <t>Total tourists</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of international tourists arriving via air passage per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tourists</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total returning residents</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of residents returning from overseas via air passage per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>residents</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total passengers from TSI</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of air passengers arriving from Torres Strait Islands per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>torres</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total mail</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of mail items arriving in Australia per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total vessels</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of vessels arriving at Australian ports per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">vessels </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total fertiliser</t>
-  </si>
-  <si>
-    <r>
-      <t>Total volume of fertiliser arriving in Australia per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">fertiliser </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total machinery</t>
-  </si>
-  <si>
-    <r>
-      <t>Total number of items of machinery arriving in Australia per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">machinery </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Total nurserystock</t>
-  </si>
-  <si>
-    <r>
-      <t>Total volume of nurserystock arriving in Australia per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">nurserystock </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pathway)</t>
-    </r>
-  </si>
-  <si>
     <t>lump with 3 and 4 (map to foods = goods)</t>
   </si>
   <si>
     <t>110-117, 120-125, 130-134, 210, 220-222, 310-314, 332, 341, 343, 345, 346, 410-414, 432, 441, 443, 445, 446, 541-543</t>
   </si>
   <si>
-    <t>348, 448, 540-544</t>
-  </si>
-  <si>
     <t>1-11, 13, 14, 16, 18-25, 27-29, 45, 47, 48, 51-56, 59-62, 65-69, 79, 80, 90, 91, 96-99</t>
   </si>
   <si>
-    <t>Prob goods</t>
-  </si>
-  <si>
-    <t>tourists, residents, mail</t>
-  </si>
-  <si>
-    <t>Total goods</t>
-  </si>
-  <si>
     <t>GBIF username</t>
   </si>
   <si>
@@ -964,56 +663,15 @@
     <t>Lymantria dispar japonica, Lymantria dispar</t>
   </si>
   <si>
-    <t>Total food</t>
-  </si>
-  <si>
-    <t>Total volume of fresh foods arriving in Australia per annum (foods pathway)</t>
-  </si>
-  <si>
-    <r>
-      <t>Total volume of goods arriving in Australia per annum (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>goods</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pathway)</t>
-    </r>
-  </si>
-  <si>
-    <t>Prob food</t>
-  </si>
-  <si>
     <t>Species group</t>
   </si>
   <si>
     <t>vessels, containers, machinery, goods</t>
   </si>
   <si>
-    <t>Xanthomonas citri, Xanthomonas axonopodis, Xanthomonas campestris subsp. citri</t>
-  </si>
-  <si>
     <t>risk_layers/abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/citrus_canker/cabi_Xanthomonas_citri_14Dec2020.csv</t>
-  </si>
-  <si>
     <t>Basemap mode</t>
   </si>
   <si>
@@ -1021,6 +679,87 @@
   </si>
   <si>
     <t>osm</t>
+  </si>
+  <si>
+    <t>Tourist leakage</t>
+  </si>
+  <si>
+    <t>Tourist establishment</t>
+  </si>
+  <si>
+    <t>Returning resident leakage</t>
+  </si>
+  <si>
+    <t>Torres passenger leakage</t>
+  </si>
+  <si>
+    <t>Torres establishment</t>
+  </si>
+  <si>
+    <t>Mail leakage</t>
+  </si>
+  <si>
+    <t>Mail establishment</t>
+  </si>
+  <si>
+    <t>Vessels leakage</t>
+  </si>
+  <si>
+    <t>Vessels establishment</t>
+  </si>
+  <si>
+    <t>Fertiliser leakage</t>
+  </si>
+  <si>
+    <t>Fertiliser establishment</t>
+  </si>
+  <si>
+    <t>Machinery leakage</t>
+  </si>
+  <si>
+    <t>Machinery establishment</t>
+  </si>
+  <si>
+    <t>Containers leakage</t>
+  </si>
+  <si>
+    <t>Containers establishment</t>
+  </si>
+  <si>
+    <t>Nurserystock leakage</t>
+  </si>
+  <si>
+    <t>Nurserystock establishment</t>
+  </si>
+  <si>
+    <t>Food leakage</t>
+  </si>
+  <si>
+    <t>Food establishment</t>
+  </si>
+  <si>
+    <t>Goods establishment</t>
+  </si>
+  <si>
+    <t>Returning resident establishment</t>
+  </si>
+  <si>
+    <t>0.05,0.5</t>
+  </si>
+  <si>
+    <t>0.01,0.1</t>
+  </si>
+  <si>
+    <t>0.005,0.05</t>
+  </si>
+  <si>
+    <t>0.002,0.02</t>
+  </si>
+  <si>
+    <t>0.1,1</t>
+  </si>
+  <si>
+    <t>Goods leakage</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1362,10 +1101,8 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1375,74 +1112,34 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1451,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1488,14 +1185,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1532,21 +1221,10 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -1555,10 +1233,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1626,43 +1300,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1671,14 +1322,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="49">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1699,7 +1365,63 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1854,13 +1576,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
@@ -1868,84 +1583,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFE7E6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2098,7 +1736,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Microsoft Office User" id="{6A9DCC67-FBF4-704D-B1D5-757B1F3E3D2F}" userId="Microsoft Office User" providerId="None"/>
   <person displayName="John Baumgartner" id="{FA70A01E-4BFB-914D-B201-A3FFB558879F}" userId="S::john.baumgartner@unimelb.edu.au::64e08097-c003-4539-ab7e-80504fe98ad0" providerId="AD"/>
 </personList>
 </file>
@@ -2400,17 +2037,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I2" dT="2020-12-09T03:13:13.86" personId="{6A9DCC67-FBF4-704D-B1D5-757B1F3E3D2F}" id="{3F4991D8-F7F4-9043-8C53-522ABDB87E94}">
-    <text>Modelled together to overcome potential identification problems</text>
-  </threadedComment>
-  <threadedComment ref="I3" dT="2020-12-09T03:13:18.71" personId="{6A9DCC67-FBF4-704D-B1D5-757B1F3E3D2F}" id="{52D97D8B-AA8C-7B49-9DAC-3B43BC703016}">
-    <text>Modelled together to overcome potential identification problems</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="B14" dT="2020-10-09T00:15:04.70" personId="{FA70A01E-4BFB-914D-B201-A3FFB558879F}" id="{72FBB23E-4BBA-F24B-819F-177E1ED5B904}">
     <text>Movement of Monochamus
 on timber pallets and packing
@@ -2455,403 +2081,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38E99D3-8DA3-8747-86C0-5C7DD6918E18}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" style="40" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="53" customWidth="1"/>
-    <col min="3" max="3" width="41.5" style="40" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="40"/>
+    <col min="1" max="1" width="34" style="34" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="41.5" style="34" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="48"/>
+    </row>
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="48"/>
+    </row>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
-    </row>
-    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="C8" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="42" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="B9" s="42" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="C9" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="45" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="56"/>
-    </row>
-    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="56"/>
-    </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="B10" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="C10" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="49" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="41" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="B11" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="48" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="B12" s="42" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
+      <c r="C12" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="48" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="B13" s="42" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="C13" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="48" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="B14" s="42" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="C14" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="49" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="B15" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="50">
+      <c r="C15" s="44">
         <f>LN(0.5)/200</f>
         <v>-3.4657359027997266E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="50">
+      <c r="A16" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="44">
         <f>LN(0.5)/10</f>
         <v>-6.9314718055994526E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="50">
-        <v>10633690</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="50">
-        <v>12722820</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="50">
-        <v>51000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="50">
-        <v>152000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="50">
-        <v>18612</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="50">
-        <v>6907</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="C23" s="50">
-        <v>1216726</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="50">
-        <v>4475</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25" s="58" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="59">
-        <v>15832</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="52">
-        <f>4*3864976</f>
-        <v>15459904</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="C7">
-    <cfRule type="containsBlanks" dxfId="52" priority="11">
+    <cfRule type="containsBlanks" dxfId="48" priority="13">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="51" priority="10">
+    <cfRule type="containsBlanks" dxfId="47" priority="12">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="50" priority="9">
+    <cfRule type="expression" dxfId="46" priority="11">
       <formula>ISBLANK($C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="49" priority="6">
+    <cfRule type="expression" dxfId="45" priority="8">
       <formula>ISBLANK($C$13)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="48" priority="5">
+    <cfRule type="expression" dxfId="44" priority="7">
       <formula>ISBLANK($C$14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="47" priority="7">
+    <cfRule type="expression" dxfId="43" priority="9">
       <formula>ISBLANK($C$12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="46" priority="4">
+    <cfRule type="expression" dxfId="42" priority="6">
       <formula>ISBLANK($C$8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="45" priority="8">
+    <cfRule type="expression" dxfId="41" priority="10">
       <formula>ISBLANK($C$11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="44" priority="3">
+    <cfRule type="expression" dxfId="40" priority="5">
       <formula>ISBLANK($C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C6">
-    <cfRule type="expression" dxfId="43" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="42" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>AND(NOT(ISBLANK($C$5)), ISBLANK($C$4))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="40">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="C24" xr:uid="{4BF11164-6F4E-B647-9B6D-1C44ECE77245}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total machinery" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="C23" xr:uid="{C466E930-DF04-5041-8EFF-FE4AA6710584}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total fertiliser" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="C22" xr:uid="{89216E67-55CE-4445-8BC0-C728B35D9DA5}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total vessels" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="C21" xr:uid="{11BACD9D-723E-674C-BD8E-C2448DF9C7AD}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total mail" error="Must be a whole number greater than or equal to 0." promptTitle="Total mail volume" prompt="Total number of mail items." sqref="C20" xr:uid="{04B798D9-6CA8-DB49-B51C-CC1EF601B496}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total TSI" error="Must be a whole number greater than or equal to 0." promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="C19" xr:uid="{E53955FA-851E-194D-9FC8-C51717F3BCD8}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total tourists" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="C17" xr:uid="{25AC0DE0-8FF7-4146-B4F5-F8E4CDB9D383}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="A18:B18 B19" xr:uid="{B0B2383C-F5E1-134E-900C-351ABBE437B7}"/>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="B17" xr:uid="{B1A125A9-908B-974A-B2C9-3AAA1E59D77B}"/>
+  <dataValidations count="19">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to container data" prompt="File path (absolute or relative to the R working directory) to the dataset giving the distribution of containers by postcode." sqref="A11:C11" xr:uid="{14B6D594-9A26-CA42-812B-5C5A86722895}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NRM shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of NRMs (natural resource management areas)." sqref="A14:C14" xr:uid="{8F72518D-BAB7-9142-9736-2536EA27E145}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to fertiliser data" prompt="File path (absolute or relative to the R working directory) to a csv containing information about fertiliser usage by NRM." sqref="A13:C13" xr:uid="{A4241D2D-0D39-E743-B011-0CB2B9A37836}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to marine ports data" prompt="File path (absolute or relative to the R working directory) to a csv containing location information for marine ports." sqref="A12:C12" xr:uid="{44AA65A2-6ACD-0941-B62C-2049F5C7A6C8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to postal areas shapefile" prompt="File path (absolute or relative to the R working directory) to the postal areas shapefile (e.g. the path to POA_2011_AUST.shp)." sqref="A10:C10" xr:uid="{67EF961C-1766-7A4E-B6D7-223B91566EBE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of nurserystock" prompt="Total volume of nurserystock entering Australia." sqref="A24:B24" xr:uid="{713381C6-7220-1D45-A0A8-298DA70EEFA4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of machinery" prompt="Total number of items of machinery arriving in Australia." sqref="A23:B23" xr:uid="{CF06620F-F4DD-F446-A1F7-11DCFF55AA38}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fertiliser" prompt="Total volume of fertiliser arriving in Australia." sqref="A22:B22" xr:uid="{32A88A5D-2C12-0345-80E1-EEF2A61A6371}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of vessels" prompt="Total number of vessels." sqref="A21:B21" xr:uid="{EE8AD24C-80B8-7B4B-8386-D76DF0F9D74E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total mail volume" prompt="Total number of mail items." sqref="A20:B20" xr:uid="{9DDE15F6-FE8D-6241-A602-284D486567B6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total TSI passenger volume" prompt="Total number of passengers from the Torres Strait Islands (if torres pathway applies)." sqref="A19" xr:uid="{6C8C5711-AEF2-214D-A457-D94DA51FA1DD}"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total returning" error="Must be a whole number greater than or equal to 0." promptTitle="Total returning resident volume" prompt="Total number of returning residents (if international passenger pathway applies)." sqref="C18" xr:uid="{500776A2-841C-034F-9692-A0C8D439FA9D}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a whole number greater than or equal to 0." promptTitle="Total tourist volume." prompt="Total number of tourists (if international passenger pathway applies)." sqref="A17" xr:uid="{C14F49AD-8C38-704B-98D8-849A5555BBE1}">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="A16:B16" xr:uid="{5FF41043-A82A-944B-945D-E8F2E51EF83B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="A15:B15" xr:uid="{33870E04-A8E1-8C4D-9B03-82E0D0B98A9C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A9:C9 C8" xr:uid="{30D6C85A-9048-7A40-93FE-19DD2761C260}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to CLUM land use raster" prompt="File path (absolute or relative to the R working directory) to the CLUM land use raster dataset. " sqref="A7:B8 C7" xr:uid="{16AA945C-95BC-C34D-8453-8B015EFC9A02}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="B3 A3" xr:uid="{AB6F6BFD-04DD-1F47-AB62-6109D668317E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A3:B3" xr:uid="{AB6F6BFD-04DD-1F47-AB62-6109D668317E}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C3" xr:uid="{14FD865C-56F7-6B42-A0EE-46BC6C1853BC}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -2861,35 +2341,27 @@
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C16" xr:uid="{74A9AB0E-B263-C746-9077-ED0626B99833}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C4" xr:uid="{72FDD181-E3BF-A844-A54A-B029705A8DC7}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{36FE115B-5D8C-BE47-8690-D0D99D6C9AD6}">
+    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C5" xr:uid="{B0433237-8341-1A41-BC52-20A6B784A23C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A6:B6" xr:uid="{08117AE8-D292-1842-9E84-80BB8B707392}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A5:B5" xr:uid="{AF8327F7-6AB4-254D-A562-85A05BFD02CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A4:B4" xr:uid="{5C32543D-BB85-AC49-99C0-4C6C3B4358FA}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{3CC3A8BE-AB30-1148-A192-70DE8AE49742}">
       <formula1>"boundaries,osm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total nurserystock" error="Must be a whole number greater than or equal to 0." promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="C25" xr:uid="{2002C4F1-3088-5649-A22C-A4601DDF97D3}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total volume of fresh food" prompt="Total volume of fresh food entering Australia." sqref="A25:B25" xr:uid="{6022A742-710F-5348-89C5-991449BFC68D}"/>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid total food" error="Must be a whole number greater than or equal to 0." promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="C26" xr:uid="{9DAAB0CF-9194-604A-A387-9A6AD4A522A0}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Total goods volume" prompt="Total volume of goods entering Australia." sqref="A26:B26" xr:uid="{8721A532-FF89-1D48-8215-293AA26D65F3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A4:B4" xr:uid="{87006BA3-D1D7-1949-808C-03FE83C142DD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A5 B5" xr:uid="{8DDA8AE4-5292-5A47-A751-FFAD9049BB67}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A6 B6" xr:uid="{AFE7AC31-B1F9-7149-9143-0E28D5C59DCF}"/>
-    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C5" xr:uid="{AA10D887-7AF0-0C43-91DF-2606C73E2F37}"/>
+    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C4" xr:uid="{D8D76911-8403-2F43-A010-EB7D062AA120}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F35787-E4E5-9646-9ED0-CA25B0854047}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F35787-E4E5-9646-9ED0-CA25B0854047}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2898,420 +2370,406 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="63" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.33203125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.5" style="21"/>
-    <col min="13" max="13" width="21.5" style="22" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="22" customWidth="1"/>
-    <col min="15" max="15" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.1640625" style="23" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" style="20" customWidth="1"/>
-    <col min="21" max="21" width="12.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5" style="23"/>
-    <col min="25" max="25" width="12.1640625" style="23" customWidth="1"/>
-    <col min="26" max="26" width="22.5" style="23" customWidth="1"/>
-    <col min="27" max="27" width="14" style="24" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.5" style="25"/>
-    <col min="29" max="16384" width="16.5" style="22"/>
+    <col min="1" max="1" width="27.6640625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.5" style="19"/>
+    <col min="13" max="13" width="21.5" style="20" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="20" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="17" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" style="17" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="17" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" style="17" customWidth="1"/>
+    <col min="22" max="23" width="13.1640625" style="17" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" style="17" customWidth="1"/>
+    <col min="26" max="26" width="12.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5" style="17" customWidth="1"/>
+    <col min="28" max="28" width="14.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5" style="17" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.33203125" style="17" customWidth="1"/>
+    <col min="32" max="33" width="16.5" style="17"/>
+    <col min="34" max="34" width="12.1640625" style="17" customWidth="1"/>
+    <col min="35" max="35" width="14" style="17" customWidth="1"/>
+    <col min="36" max="36" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.5" style="53" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" style="54" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.5" style="21"/>
+    <col min="40" max="16384" width="16.5" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="9" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="32" t="s">
+    <row r="1" spans="1:39" s="9" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="L1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="P1" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF1" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH1" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI1" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ1" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK1" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z1" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA1" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB1" s="8"/>
-    </row>
-    <row r="2" spans="1:28" s="16" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="AM1" s="8"/>
+    </row>
+    <row r="2" spans="1:39" s="14" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="11" t="b">
+      <c r="B2" s="49"/>
+      <c r="C2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="14" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="18">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="16">
         <v>1970</v>
       </c>
-      <c r="K2" s="10"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="64">
-        <v>5.5158148588071995E-10</v>
-      </c>
-      <c r="P2" s="64">
-        <v>2.7579074294035997E-10</v>
-      </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="64">
-        <v>2.69906694008609E-10</v>
-      </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="14">
-        <v>5000</v>
-      </c>
-      <c r="AB2" s="15"/>
-    </row>
-    <row r="3" spans="1:28" s="16" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" s="18">
-        <v>1970</v>
-      </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="64">
-        <v>2.6864388566516202E-8</v>
-      </c>
-      <c r="T3" s="20">
+        <v>127</v>
+      </c>
+      <c r="O2" s="18">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
-      <c r="U3" s="19"/>
-      <c r="V3" s="64">
-        <v>1.1992830685816E-12</v>
-      </c>
-      <c r="W3" s="64">
-        <v>1.2936690939348701E-10</v>
-      </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="64">
-        <v>1.1992830685816E-12</v>
-      </c>
-      <c r="AA3" s="14">
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y2" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC2" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD2" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE2" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="AK2" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL2" s="12">
         <v>5000</v>
       </c>
-      <c r="AB3" s="15"/>
+      <c r="AM2" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="41" priority="178">
+    <cfRule type="expression" dxfId="37" priority="193">
       <formula>$F2=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="200">
+    <cfRule type="expression" dxfId="36" priority="215">
       <formula>ISBLANK($H2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="expression" dxfId="39" priority="201">
+    <cfRule type="expression" dxfId="35" priority="216">
       <formula>ISBLANK($G2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M1048576 K2:K1048576 I3:I1048576">
-    <cfRule type="expression" dxfId="38" priority="202">
+  <conditionalFormatting sqref="M2:M1048576 K2:K1048576 I2:I1048576">
+    <cfRule type="expression" dxfId="34" priority="217">
       <formula>AND(ISBLANK($I2), ISBLANK($K2), ISBLANK($M2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="37" priority="191">
+    <cfRule type="expression" dxfId="33" priority="206">
       <formula>ISBLANK($I2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="expression" dxfId="36" priority="199">
+    <cfRule type="expression" dxfId="32" priority="214">
       <formula>OR($D2=FALSE, AND(ISBLANK($I2), ISBLANK($K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T1048576">
-    <cfRule type="expression" dxfId="35" priority="185">
-      <formula>NOT(ISNUMBER(SEARCH("vessels", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="204">
-      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($T2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="expression" dxfId="33" priority="198">
+    <cfRule type="expression" dxfId="31" priority="213">
       <formula>OR(ISBLANK($A2),$D2=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:L1048576 N2:N1048576 I3 J2:L3">
-    <cfRule type="expression" dxfId="32" priority="205">
+  <conditionalFormatting sqref="N2:O1048576 I2:L1048576">
+    <cfRule type="expression" dxfId="30" priority="220">
       <formula>NOT(ISBLANK($M2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P1048576">
-    <cfRule type="expression" dxfId="31" priority="189">
+  <conditionalFormatting sqref="R2:S1048576">
+    <cfRule type="expression" dxfId="29" priority="204">
       <formula>NOT(ISNUMBER(SEARCH("residents", $C2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="203">
-      <formula>AND(ISNUMBER(SEARCH("residents",$C2)), ISBLANK($P2))</formula>
+    <cfRule type="expression" dxfId="28" priority="218">
+      <formula>AND(ISNUMBER(SEARCH("residents",$C2)), ISBLANK($R2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q1048576">
-    <cfRule type="expression" dxfId="29" priority="188">
+  <conditionalFormatting sqref="T2:U1048576">
+    <cfRule type="expression" dxfId="27" priority="203">
       <formula>NOT(ISNUMBER(SEARCH("torres", $C2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="206">
-      <formula>AND(ISNUMBER(SEARCH("torres",$C2)), ISBLANK($Q2))</formula>
+    <cfRule type="expression" dxfId="26" priority="221">
+      <formula>AND(ISNUMBER(SEARCH("torres",$C2)), ISBLANK($T2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R1048576">
-    <cfRule type="expression" dxfId="27" priority="187">
+  <conditionalFormatting sqref="V2:W1048576">
+    <cfRule type="expression" dxfId="25" priority="202">
       <formula>NOT(ISNUMBER(SEARCH("mail", $C2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="207">
-      <formula>AND(SEARCH("mail",$C2), ISBLANK($R2))</formula>
+    <cfRule type="expression" dxfId="24" priority="222">
+      <formula>AND(SEARCH("mail",$C2), ISBLANK($V2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S1048576">
-    <cfRule type="expression" dxfId="25" priority="186">
+  <conditionalFormatting sqref="X2:Y1048576">
+    <cfRule type="expression" dxfId="23" priority="201">
       <formula>NOT(ISNUMBER(SEARCH("vessels", $C2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="208">
-      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($S2))</formula>
+    <cfRule type="expression" dxfId="22" priority="223">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($X2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U1048576">
-    <cfRule type="expression" dxfId="23" priority="184">
-      <formula>NOT(ISNUMBER(SEARCH("fert", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="209">
-      <formula>AND(ISNUMBER(SEARCH("fert",$C2)), ISBLANK($U2))</formula>
+  <conditionalFormatting sqref="P2:Q1048576">
+    <cfRule type="expression" dxfId="21" priority="205">
+      <formula>NOT(ISNUMBER(SEARCH("tourists",$C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="212">
+      <formula>AND(ISNUMBER(SEARCH("tourists",$C2)), ISBLANK($P2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V1048576">
-    <cfRule type="expression" dxfId="21" priority="183">
-      <formula>NOT(ISNUMBER(SEARCH("machine", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="210">
-      <formula>AND(ISNUMBER(SEARCH("machine",$C2)), ISBLANK($V2))</formula>
+  <conditionalFormatting sqref="C2:C1048576">
+    <cfRule type="expression" dxfId="19" priority="209">
+      <formula>ISBLANK($C2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W1048576">
-    <cfRule type="expression" dxfId="19" priority="182">
-      <formula>NOT(ISNUMBER(SEARCH("container", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="211">
-      <formula>AND(ISNUMBER(SEARCH("container",$C2)), ISBLANK($W2))</formula>
+  <conditionalFormatting sqref="A2:AL1048576">
+    <cfRule type="expression" dxfId="18" priority="192">
+      <formula>ISBLANK($A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X1048576">
-    <cfRule type="expression" dxfId="17" priority="181">
-      <formula>NOT(ISNUMBER(SEARCH("nursery", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="212">
-      <formula>AND(ISNUMBER(SEARCH("nursery",$C2)), ISBLANK($X2))</formula>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="expression" dxfId="17" priority="208">
+      <formula>ISBLANK($D2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z1048576">
-    <cfRule type="expression" dxfId="15" priority="180">
-      <formula>NOT(ISNUMBER(SEARCH("goods", $C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="213">
-      <formula>AND(ISNUMBER(SEARCH("goods",$C2)), ISBLANK($Z2))</formula>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="expression" dxfId="16" priority="210">
+      <formula>ISBLANK($E2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="expression" dxfId="15" priority="207">
+      <formula>ISBLANK($F2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:O1048576">
+    <cfRule type="expression" dxfId="14" priority="194">
+      <formula>$D2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="expression" dxfId="13" priority="190">
-      <formula>NOT(ISNUMBER(SEARCH("tourists",$C2)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="197">
-      <formula>AND(ISNUMBER(SEARCH("tourists",$C2)), ISBLANK($O2))</formula>
+    <cfRule type="expression" dxfId="13" priority="229">
+      <formula>NOT(ISNUMBER(SEARCH("vessels", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="230">
+      <formula>AND(ISNUMBER(SEARCH("vessels",$C2)), ISBLANK($O2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="11" priority="194">
-      <formula>ISBLANK($C2)</formula>
+  <conditionalFormatting sqref="Z2:AA1048576">
+    <cfRule type="expression" dxfId="11" priority="231">
+      <formula>NOT(ISNUMBER(SEARCH("fert", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="232">
+      <formula>AND(ISNUMBER(SEARCH("fert",$C2)), ISBLANK($Z2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H3 A4:Y1048576 Z2:AA1048576 I3 J2:Y3">
-    <cfRule type="expression" dxfId="10" priority="177">
-      <formula>ISBLANK($A2)</formula>
+  <conditionalFormatting sqref="AB2:AC1048576">
+    <cfRule type="expression" dxfId="9" priority="233">
+      <formula>NOT(ISNUMBER(SEARCH("machine", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="234">
+      <formula>AND(ISNUMBER(SEARCH("machine",$C2)), ISBLANK($AB2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="expression" dxfId="9" priority="193">
-      <formula>ISBLANK($D2)</formula>
+  <conditionalFormatting sqref="AD2:AE1048576">
+    <cfRule type="expression" dxfId="7" priority="235">
+      <formula>NOT(ISNUMBER(SEARCH("container", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="236">
+      <formula>AND(ISNUMBER(SEARCH("container",$C2)), ISBLANK($AD2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="8" priority="195">
-      <formula>ISBLANK($E2)</formula>
+  <conditionalFormatting sqref="AF2:AG1048576">
+    <cfRule type="expression" dxfId="5" priority="237">
+      <formula>NOT(ISNUMBER(SEARCH("nursery", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="238">
+      <formula>AND(ISNUMBER(SEARCH("nursery",$C2)), ISBLANK($AF2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="expression" dxfId="7" priority="192">
-      <formula>ISBLANK($F2)</formula>
+  <conditionalFormatting sqref="AJ2:AK1048576">
+    <cfRule type="expression" dxfId="3" priority="239">
+      <formula>NOT(ISNUMBER(SEARCH("goods", $C2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="240">
+      <formula>AND(ISNUMBER(SEARCH("goods",$C2)), ISBLANK($AJ2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:N1048576 I3 J2:N3">
-    <cfRule type="expression" dxfId="6" priority="179">
-      <formula>$D2=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="5" priority="166">
-      <formula>ISBLANK($A2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="4" priority="168">
-      <formula>AND(ISBLANK($I2), ISBLANK($K2), ISBLANK($M2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="3" priority="169">
-      <formula>NOT(ISBLANK($M2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="2" priority="167">
-      <formula>$D2=FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y1048576">
-    <cfRule type="expression" dxfId="1" priority="86">
+  <conditionalFormatting sqref="AH2:AI1048576">
+    <cfRule type="expression" dxfId="1" priority="241">
       <formula>NOT(ISNUMBER(SEARCH("food", $C2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="87">
-      <formula>AND(ISNUMBER(SEARCH("food",$C2)), ISBLANK($Y2))</formula>
+    <cfRule type="expression" dxfId="0" priority="242">
+      <formula>AND(ISNUMBER(SEARCH("food",$C2)), ISBLANK($AH2))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="47">
@@ -3322,52 +2780,52 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Include NVIS?" prompt="Should NVIS contribute to biotic weight? _x000a__x000a_NOTE: Useful for pests that impact native vegetation" sqref="F1" xr:uid="{27524273-1C90-D04F-832E-935EB4104323}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NVIS major vegetation subgroups" prompt="Comma-separated NVIS MVS classes (e.g. 1,2,3,5)." sqref="H1" xr:uid="{048997E5-1BBB-0B4F-8524-4F71F4D0963D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF minimum year" prompt="Earliest year (1800 to current) for which GBIF data will be obtained. Ignored if gbif_species column is blank._x000a__x000a_DEFAULT: 1970 (If required &amp; left blank)" sqref="J1" xr:uid="{544504DF-2050-134C-8497-26394E3031A2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="O1" xr:uid="{1A6AAEBE-B93B-A343-B662-CF1F257FCCFA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="P1" xr:uid="{9BB29CB2-A334-AA40-AB0B-AD97B6DB1CE7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="Q1" xr:uid="{5B5B5D23-E41C-034B-BB8C-780D7C7B7330}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="R1" xr:uid="{F6FEE5E1-D9A3-A740-9E8B-638C32FDD00D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="S1" xr:uid="{1DC9DEE7-7379-6842-A6EB-0DF269E933D8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="T1" xr:uid="{086160EC-9D52-9C49-8D24-EF29A51F2A54}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="U1" xr:uid="{565002BF-0DFE-B94A-9B26-10772C7EEF0D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="V1" xr:uid="{C6C5C3CE-9CCE-AF4C-A1D8-D400932E1554}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="W1" xr:uid="{C489A9C9-F330-A341-B9CC-483398DDC7E6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="X1" xr:uid="{E9F751EA-A832-8B49-BA7D-522EA0666BB8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Z1" xr:uid="{8F08BC14-7836-4049-A576-C8460E7AB591}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Name must begin with a letter or a period." promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A4:B1048576 A2:B3" xr:uid="{FCA27B26-0010-EE4F-8B6E-B6BCF0DF1EDC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried. Ignored if &quot;Climate suitability path&quot; is provided." sqref="I1 I4:I1048576" xr:uid="{589C2EB4-9ABA-5940-9C6D-3DE7287152B9}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest." sqref="O2:O1048576" xr:uid="{53D33507-D28B-5C4D-BF9A-79E197DEB5E3}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest._x000a_" sqref="P1:Q1" xr:uid="{1A6AAEBE-B93B-A343-B662-CF1F257FCCFA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="R1:S1" xr:uid="{9BB29CB2-A334-AA40-AB0B-AD97B6DB1CE7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="T1:U1" xr:uid="{5B5B5D23-E41C-034B-BB8C-780D7C7B7330}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="V1:W1" xr:uid="{F6FEE5E1-D9A3-A740-9E8B-638C32FDD00D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="X1:Y1" xr:uid="{1DC9DEE7-7379-6842-A6EB-0DF269E933D8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="O1" xr:uid="{086160EC-9D52-9C49-8D24-EF29A51F2A54}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="Z1:AA1" xr:uid="{565002BF-0DFE-B94A-9B26-10772C7EEF0D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="AB1:AC1" xr:uid="{C6C5C3CE-9CCE-AF4C-A1D8-D400932E1554}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="AD1:AE1" xr:uid="{C489A9C9-F330-A341-B9CC-483398DDC7E6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="AF1:AG1" xr:uid="{E9F751EA-A832-8B49-BA7D-522EA0666BB8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="AJ1:AK1" xr:uid="{8F08BC14-7836-4049-A576-C8460E7AB591}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Name must begin with a letter or a period." promptTitle="Species name" prompt="Name that should be prepended to output files for this species. Must begin with a letter or period." sqref="A3:B1048576 A2:B2" xr:uid="{FCA27B26-0010-EE4F-8B6E-B6BCF0DF1EDC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF search names" prompt="Comma-separated species names to query GBIF. If this is empty, GBIF will not be queried. Ignored if &quot;Climate suitability path&quot; is provided." sqref="I1 I3:I1048576" xr:uid="{589C2EB4-9ABA-5940-9C6D-3DE7287152B9}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on tourist" prompt="Probability of international tourist carrying pest." sqref="P2:Q1048576" xr:uid="{53D33507-D28B-5C4D-BF9A-79E197DEB5E3}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="P2:P1048576" xr:uid="{B9883FA4-A475-184A-88E9-1113938EC677}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on return resident" prompt="Probability of pest on returning resident." sqref="R2:S1048576" xr:uid="{B9883FA4-A475-184A-88E9-1113938EC677}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="Y1" xr:uid="{32FFCBBD-4497-364E-9334-FC28356E20CA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="AH1:AI1" xr:uid="{32FFCBBD-4497-364E-9334-FC28356E20CA}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include abiotic weights?" prompt="Should abiotic weights be included?" sqref="D2:D1048576" xr:uid="{C2DF29EF-AFB7-9F42-B4CE-CEBE92710EDB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Expert occurrence data path" prompt="File path (absolute or relative to working directory) to occurrence dataset. Ignored if &quot;Climate suitability path&quot; is provided." sqref="K1:K1048576" xr:uid="{3B00E97C-487B-FE42-8EA0-D06CE5C55537}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="R2:R1048576" xr:uid="{4B2739D8-37B1-6A47-B64D-AAE7AC7BF8F4}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per mail item" prompt="Probability of arrival of pest per piece of mail." sqref="V2:W1048576" xr:uid="{4B2739D8-37B1-6A47-B64D-AAE7AC7BF8F4}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="S2:S1048576" xr:uid="{1A254FEC-45D6-9548-A95C-2F801D81556E}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival per vessel" prompt="Probability of arrival of pest per vessel." sqref="X2:Y1048576" xr:uid="{1A254FEC-45D6-9548-A95C-2F801D81556E}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a negative number." promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="T2:T1048576" xr:uid="{BB861B61-09C3-7D44-8C41-E4DF88FE6A0F}">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a negative number." promptTitle="Distance penalty (ports)" prompt="Parameter controlling the rate of decrease in the likelihood of pest arrival with distance from marine ports." sqref="O2:O1048576" xr:uid="{BB861B61-09C3-7D44-8C41-E4DF88FE6A0F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="U2:U1048576" xr:uid="{97457597-1B84-4E4E-9BCA-1BDFB9D1502F}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob per unit of fertiliser" prompt="Probability of arrival of pest per unit of fertiliser." sqref="Z2:AA1048576" xr:uid="{97457597-1B84-4E4E-9BCA-1BDFB9D1502F}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="V2:V1048576" xr:uid="{8608EAF9-50F2-654A-B512-BB4F8D87B150}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (machinery)" prompt="Probability of arrival of pest per unit of machinery." sqref="AB2:AC1048576" xr:uid="{8608EAF9-50F2-654A-B512-BB4F8D87B150}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="W2:W1048576" xr:uid="{4455259B-CE18-4E46-A458-ED2133A3F305}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (containers)" prompt="Probability of arrival per container entering Australia." sqref="AD2:AE1048576" xr:uid="{4455259B-CE18-4E46-A458-ED2133A3F305}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="X2:X1048576" xr:uid="{0AC6E29F-5654-D346-A355-51641DAF84DA}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (nurserystock)" prompt="Probability of arrival of pest per unit of nurserystock entering Australia." sqref="AF2:AG1048576" xr:uid="{0AC6E29F-5654-D346-A355-51641DAF84DA}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="Z2:Z1048576" xr:uid="{84635E57-CD86-A74B-B4DC-4E8F7D6B29DD}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (goods)" prompt="Probability of arrival of pest per unit of goods." sqref="AJ2:AK1048576" xr:uid="{84635E57-CD86-A74B-B4DC-4E8F7D6B29DD}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be TRUE or FALSE." promptTitle="Include NDVI?" prompt="Should NDVI contribute to biotic weight?" sqref="E2:E1048576" xr:uid="{701D4CA7-2B69-4447-A97B-9709BB40773C}">
@@ -3385,10 +2843,10 @@
       <formula1>1800</formula1>
       <formula2>YEAR(TODAY())</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="Q2:Q1048576" xr:uid="{C7F4FAC2-1E09-D24A-8BAC-5FD6219BE806}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of pest on Torres passenger" prompt="Probability of pest on Torres Strait passenger." sqref="T2:U1048576" xr:uid="{C7F4FAC2-1E09-D24A-8BAC-5FD6219BE806}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exclude BIOCLIM variables" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19)._x000a__x000a_Ignored if &quot;Climate suitability path&quot; is provided._x000a__x000a_Default: No variables are excluded." sqref="N1:N1048576" xr:uid="{9E2FCDB2-1FF7-8147-8F38-8F31C7C4B682}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exclude BIOCLIM variables" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19)._x000a__x000a_Ignored if &quot;Climate suitability path&quot; is provided._x000a__x000a_Default: No variables are excluded." sqref="N1:O1048576" xr:uid="{9E2FCDB2-1FF7-8147-8F38-8F31C7C4B682}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Can only contain numbers, commas, spaces, and range indicators (i.e. specified by colons or hyphens, e.g. 1-3 or 1:3)." promptTitle="CABI file path" prompt="File path (absolute or relative to working directory) to the CABI csv file." sqref="G2:G1048576" xr:uid="{AD5DFB87-82FB-B44D-A12A-6DEF487A5237}">
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(G2,ROW(INDIRECT("1:"&amp;LEN(G2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
@@ -3399,15 +2857,14 @@
       <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(H2,ROW(INDIRECT("1:"&amp;LEN(H2))),1)," ,-:0123456789")))</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate suitability path" prompt="Optional file path to a climate suitability raster. Must be binary (0=unsuitable; 1=suitable) or describe relative suitability between 0-1. Must be 1000 m res; Australian Albers (EPSG:3577); extent xmin=-1888000; xmax=2122000; ymin=-4847000; ymax=-1010000" sqref="M1:M1048576" xr:uid="{43224EB0-F4AD-E443-B771-F1DA3AECF215}"/>
-    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Aggregated output resolution must be a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, the default value of 5000 will be used." sqref="AA1:AA1048576" xr:uid="{A4DB3E19-43E0-034B-BC9C-138C8662B41E}">
-      <formula1>AND($AA1 &gt;= 1000, MOD($AA1, 1000)=0)</formula1>
+    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Aggregated output resolution must be a multiple of 1000." promptTitle="Aggregated output resolution" prompt="Spatial resolution of aggregated establishment likelihood rasters. Must be specified in metres and must be a multiple of 1000. If not provided, the default value of 5000 will be used." sqref="AL1:AL1048576" xr:uid="{A4DB3E19-43E0-034B-BC9C-138C8662B41E}">
+      <formula1>AND($AL1 &gt;= 1000, MOD($AL1, 1000)=0)</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="Y2:Y1048576" xr:uid="{79122985-12E1-4145-9493-CB195B7CBF1B}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a number greater than or equal to 0." promptTitle="Prob of arrival (food)" prompt="Probability of arrival of pest per consignment of fresh food entering Australia." sqref="AH2:AI1048576" xr:uid="{79122985-12E1-4145-9493-CB195B7CBF1B}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3430,615 +2887,615 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to README and tweak of parameters.xlsx to work with data repository
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/cebra/20121001-multi-pest-early-detection-maps/data/user_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcamac/Dropbox/Projects/CEBRA/edmaps/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA83374-46AC-8140-8AF8-217F65F27095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F8CE92-9EBB-5147-AF21-CD6A6DD35A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="500" windowWidth="28380" windowHeight="21100" activeTab="1" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
@@ -825,12 +825,6 @@
     <t>110-117, 120-125, 130-134, 210, 220-222, 310-314, 320-338, 340-349, 350-353, 360-365, 410-414, 420-424, 430-439, 440-449, 450-454, 460-465, 510-515, 520-528, 530-538, 540-545, 550-555, 560-567, 570-575, 580-584, 590-595, 610-614, 620-623, 630-633, 640-644, 650-654, 660-663</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
-  </si>
-  <si>
     <t>GBIF username</t>
   </si>
   <si>
@@ -855,36 +849,9 @@
     <t>Bee mite</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
-  </si>
-  <si>
     <t>Bactrocera cucurbitae, Zeugodacus cucurbitae</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
-  </si>
-  <si>
     <t>Basemap mode</t>
   </si>
   <si>
@@ -1140,9 +1107,6 @@
     <t>0.03,0.16</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
-  </si>
-  <si>
     <t>GBIF focal species name(s)</t>
   </si>
   <si>
@@ -1191,15 +1155,6 @@
     <t>Food, Nursery, Residents</t>
   </si>
   <si>
-    <t>risk_layers/abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>risk_layers/biotic/citrus_hosts.tif</t>
-  </si>
-  <si>
-    <t>risk_layers/abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
-  </si>
-  <si>
     <t>Tourists, Residents, Food, Torres, Goods</t>
   </si>
   <si>
@@ -1264,6 +1219,51 @@
   </si>
   <si>
     <t>om#V&gt;nzeCa3E^aU2.n8xZLCS</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>biotic/citrus_native_hosts_example.tif</t>
   </si>
 </sst>
 </file>
@@ -3297,43 +3297,43 @@
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>138</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>139</v>
-      </c>
       <c r="C5" s="36" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C7" s="36">
         <v>1.0000000000000001E-5</v>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -3572,10 +3572,10 @@
   <dimension ref="A1:AT21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,7 +3626,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C1" s="48" t="s">
         <v>8</v>
@@ -3647,19 +3647,19 @@
         <v>65</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="L1" s="50" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="N1" s="48" t="s">
         <v>67</v>
@@ -3668,106 +3668,106 @@
         <v>68</v>
       </c>
       <c r="P1" s="49" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="Q1" s="51" t="s">
         <v>69</v>
       </c>
       <c r="R1" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="U1" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="X1" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y1" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z1" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB1" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC1" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD1" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE1" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="AF1" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="AG1" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="U1" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="V1" s="48" t="s">
+      <c r="AH1" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="W1" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="X1" s="48" t="s">
+      <c r="AI1" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="AJ1" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="AK1" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AL1" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM1" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC1" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD1" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE1" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF1" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG1" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH1" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="AI1" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="AJ1" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="AK1" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="AL1" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="AM1" s="48" t="s">
-        <v>175</v>
-      </c>
       <c r="AN1" s="48" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="AO1" s="48" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="AP1" s="48" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="AQ1" s="48" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AR1" s="48" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="AS1" s="48" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="AT1" s="52" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="41" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" s="41" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="8" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="8"/>
@@ -3796,10 +3796,10 @@
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
@@ -3808,10 +3808,10 @@
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="AD2" s="8"/>
       <c r="AE2" s="8"/>
@@ -3820,10 +3820,10 @@
       <c r="AH2" s="8"/>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="8" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="AL2" s="8"/>
       <c r="AM2" s="8"/>
@@ -3839,11 +3839,11 @@
     </row>
     <row r="3" spans="1:46" s="41" customFormat="1" ht="86" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="12" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D3" s="11" t="b">
         <v>1</v>
@@ -3863,14 +3863,14 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L3" s="13">
         <v>1970</v>
       </c>
       <c r="M3" s="12"/>
       <c r="N3" s="12" t="s">
-        <v>144</v>
+        <v>266</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
@@ -3887,24 +3887,24 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
       <c r="AD3" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="AF3" s="12" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AH3" s="12"/>
       <c r="AI3" s="12"/>
@@ -3924,13 +3924,13 @@
     </row>
     <row r="4" spans="1:46" s="41" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D4" s="11" t="b">
         <v>1</v>
@@ -3948,7 +3948,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="12" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="L4" s="13">
         <v>1970</v>
@@ -3964,38 +3964,38 @@
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
       <c r="AF4" s="12" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="AH4" s="12"/>
       <c r="AI4" s="12"/>
       <c r="AJ4" s="12" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AL4" s="12"/>
       <c r="AM4" s="12"/>
@@ -4011,13 +4011,13 @@
     </row>
     <row r="5" spans="1:46" s="41" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D5" s="11" t="b">
         <v>1</v>
@@ -4037,7 +4037,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="M5" s="12" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="11"/>
@@ -4049,38 +4049,38 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
       <c r="T5" s="12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
       <c r="AE5" s="12"/>
       <c r="AF5" s="12" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="12" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AL5" s="12"/>
       <c r="AM5" s="12"/>
@@ -4100,7 +4100,7 @@
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="12" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D6" s="11" t="b">
         <v>1</v>
@@ -4120,10 +4120,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
       <c r="M6" s="12" t="s">
-        <v>135</v>
+        <v>268</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>152</v>
+        <v>269</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -4134,44 +4134,44 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
       <c r="AD6" s="12" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="AF6" s="12" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AH6" s="12"/>
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="AM6" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AN6" s="12"/>
       <c r="AO6" s="12"/>
@@ -4185,10 +4185,10 @@
     </row>
     <row r="7" spans="1:46" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D7" s="17" t="b">
         <v>0</v>
@@ -4203,33 +4203,33 @@
         <v>0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="R7" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AJ7" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AL7" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="AM7" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AT7" s="39">
         <v>5000</v>
@@ -4237,10 +4237,10 @@
     </row>
     <row r="8" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D8" s="17" t="b">
         <v>1</v>
@@ -4255,7 +4255,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>71</v>
@@ -4264,40 +4264,40 @@
         <v>1970</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>134</v>
+        <v>270</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>153</v>
+        <v>271</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="W8" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AJ8" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AL8" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="AM8" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AT8" s="39">
         <v>5000</v>
@@ -4305,10 +4305,10 @@
     </row>
     <row r="9" spans="1:46" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D9" s="17" t="b">
         <v>0</v>
@@ -4323,38 +4323,38 @@
         <v>0</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="N9" s="12"/>
       <c r="R9" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="W9" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AJ9" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AL9" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="AM9" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AT9" s="39">
         <v>5000</v>
@@ -4362,10 +4362,10 @@
     </row>
     <row r="10" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D10" s="17" t="b">
         <v>1</v>
@@ -4380,47 +4380,47 @@
         <v>0</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L10" s="13">
         <v>1970</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12" t="s">
-        <v>145</v>
+        <v>272</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="W10" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AJ10" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AL10" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="AM10" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AT10" s="39">
         <v>5000</v>
@@ -4428,13 +4428,13 @@
     </row>
     <row r="11" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D11" s="17" t="b">
         <v>1</v>
@@ -4449,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>80</v>
@@ -4458,37 +4458,37 @@
         <v>1970</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="P11" s="54">
         <v>100000</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="AH11" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="AI11" s="12" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="AJ11" s="12" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AN11" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="AO11" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AT11" s="39">
         <v>5000</v>
@@ -4496,13 +4496,13 @@
     </row>
     <row r="12" spans="1:46" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D12" s="17" t="b">
         <v>0</v>
@@ -4517,27 +4517,27 @@
         <v>0</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="T12" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="AH12" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="AI12" s="12" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="AJ12" s="12" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="AT12" s="39">
         <v>5000</v>
@@ -4545,10 +4545,10 @@
     </row>
     <row r="13" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D13" s="17" t="b">
         <v>0</v>
@@ -4566,28 +4566,28 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="T13" s="12" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="AF13" s="12" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="AJ13" s="12" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AL13" s="12" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="AM13" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AT13" s="39">
         <v>5000</v>
@@ -4595,10 +4595,10 @@
     </row>
     <row r="14" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D14" s="17" t="b">
         <v>0</v>
@@ -4616,22 +4616,22 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="T14" s="12" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AF14" s="12" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="AG14" s="12" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="AL14" s="12" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="AM14" s="12" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="AT14" s="39">
         <v>5000</v>
@@ -4639,10 +4639,10 @@
     </row>
     <row r="15" spans="1:46" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D15" s="17" t="b">
         <v>1</v>
@@ -4665,25 +4665,25 @@
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12" t="s">
-        <v>147</v>
+        <v>275</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AF15" s="12" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="AG15" s="12" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="AL15" s="12" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="AM15" s="12" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="AT15" s="39">
         <v>5000</v>
@@ -4691,13 +4691,13 @@
     </row>
     <row r="16" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="45" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D16" s="17" t="b">
         <v>1</v>
@@ -4720,29 +4720,29 @@
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12" t="s">
-        <v>148</v>
+        <v>276</v>
       </c>
       <c r="Q16" s="14">
         <f t="shared" ref="Q16" si="0">LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Z16" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="AA16" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AL16" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="AM16" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AT16" s="39">
         <v>5000</v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="17" spans="1:46" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D17" s="17" t="b">
         <v>1</v>
@@ -4779,29 +4779,29 @@
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="12" t="s">
-        <v>149</v>
+        <v>277</v>
       </c>
       <c r="Q17" s="14">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Z17" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="AA17" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AL17" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="AM17" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AT17" s="39">
         <v>5000</v>
@@ -4809,13 +4809,13 @@
     </row>
     <row r="18" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="45" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D18" s="17" t="b">
         <v>1</v>
@@ -4838,29 +4838,29 @@
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12" t="s">
-        <v>150</v>
+        <v>278</v>
       </c>
       <c r="Q18" s="14">
         <f t="shared" ref="Q18" si="1">LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Z18" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="AA18" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AL18" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="AM18" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AT18" s="39">
         <v>5000</v>
@@ -4868,13 +4868,13 @@
     </row>
     <row r="19" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A19" s="45" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D19" s="17" t="b">
         <v>1</v>
@@ -4897,29 +4897,29 @@
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="12" t="s">
-        <v>151</v>
+        <v>279</v>
       </c>
       <c r="Q19" s="14">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Z19" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="AA19" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="AL19" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="AM19" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AT19" s="39">
         <v>5000</v>
@@ -4927,13 +4927,13 @@
     </row>
     <row r="20" spans="1:46" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D20" s="17" t="b">
         <v>0</v>
@@ -4948,16 +4948,16 @@
         <v>0</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="AH20" s="12" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="AI20" s="12" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="AT20" s="39">
         <v>5000</v>
@@ -4965,11 +4965,11 @@
     </row>
     <row r="21" spans="1:46" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="45" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="12" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D21" s="17" t="b">
         <v>1</v>
@@ -4989,7 +4989,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="12" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="N21" s="40"/>
       <c r="O21" s="17"/>
@@ -5007,20 +5007,20 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="AA21" s="12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
       <c r="AF21" s="12" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="AG21" s="12" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="AH21" s="12"/>
       <c r="AI21" s="12"/>

</xml_diff>

<commit_message>
Update paramegters.xlsx example to match data repository, also updated dockerfile
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcamac/Dropbox/Projects/CEBRA/edmaps/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F8CE92-9EBB-5147-AF21-CD6A6DD35A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B8F98-AF0D-1C4A-8DF1-7551927E4E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="500" windowWidth="28380" windowHeight="21100" activeTab="1" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
+    <workbookView xWindow="10020" yWindow="500" windowWidth="28380" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
   <sheets>
     <sheet name="Global parameters" sheetId="7" r:id="rId1"/>
@@ -39,12 +39,9 @@
   <authors>
     <author>tc={B5A97D6C-3EB5-6940-A766-351C93294C30}</author>
     <author>tc={03D81196-E77D-0F4D-A067-33B2632A711C}</author>
-    <author>tc={0196C33E-8F8E-E84B-9ABD-5D6E98C41E55}</author>
-    <author>tc={08970612-EB31-8641-B619-72C12D702C77}</author>
     <author>tc={52D97D8B-AA8C-7B49-9DAC-3B43BC703016}</author>
     <author>tc={95D4E981-0722-DC45-973F-DAC9CDE6DA9E}</author>
     <author>tc={30BEA44C-71B5-C346-82C3-2AF8168E4B6B}</author>
-    <author>tc={A62E6B1F-E4EB-984E-B747-9546652AB2B8}</author>
     <author>tc={24C12BAB-7D3D-1D41-A58D-58EA66DA6BBC}</author>
     <author>tc={1B8A75AC-A9FE-EB43-AD87-1FE8467FBB89}</author>
     <author>tc={54D29E90-6B5C-7E47-B3EC-ABC5E05A1AF6}</author>
@@ -69,23 +66,7 @@
     Insufficient occurrence data</t>
       </text>
     </comment>
-    <comment ref="M2" authorId="2" shapeId="0" xr:uid="{0196C33E-8F8E-E84B-9ABD-5D6E98C41E55}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Very few records of Citrus canker. Decided to use CABI records as approximation data rather than the 50 odd GBIF records</t>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="3" shapeId="0" xr:uid="{08970612-EB31-8641-B619-72C12D702C77}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Need to extra work here. Some records are in USA jurisdictions which don’t have it. Will need to manually remove.</t>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="4" shapeId="0" xr:uid="{52D97D8B-AA8C-7B49-9DAC-3B43BC703016}">
+    <comment ref="K3" authorId="2" shapeId="0" xr:uid="{52D97D8B-AA8C-7B49-9DAC-3B43BC703016}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -93,7 +74,7 @@
     Modelled together to overcome potential identification problems</t>
       </text>
     </comment>
-    <comment ref="D7" authorId="5" shapeId="0" xr:uid="{95D4E981-0722-DC45-973F-DAC9CDE6DA9E}">
+    <comment ref="D7" authorId="3" shapeId="0" xr:uid="{95D4E981-0722-DC45-973F-DAC9CDE6DA9E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -101,7 +82,7 @@
     Too few records to estimate climate suitability</t>
       </text>
     </comment>
-    <comment ref="C8" authorId="6" shapeId="0" xr:uid="{30BEA44C-71B5-C346-82C3-2AF8168E4B6B}">
+    <comment ref="C8" authorId="4" shapeId="0" xr:uid="{30BEA44C-71B5-C346-82C3-2AF8168E4B6B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -109,15 +90,7 @@
     Note that for fruit flies we have broken up the passenger pathway by resident &amp; tourist. We also add a Torres strait passenger pathway… and because there are two separate food pathways with different establishment parameters we’ve used goods to distribute the second.</t>
       </text>
     </comment>
-    <comment ref="K8" authorId="7" shapeId="0" xr:uid="{A62E6B1F-E4EB-984E-B747-9546652AB2B8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Have added synonyms as per risk maps phase 1</t>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="8" shapeId="0" xr:uid="{24C12BAB-7D3D-1D41-A58D-58EA66DA6BBC}">
+    <comment ref="D9" authorId="5" shapeId="0" xr:uid="{24C12BAB-7D3D-1D41-A58D-58EA66DA6BBC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -125,7 +98,7 @@
     Too few records for estimating climate</t>
       </text>
     </comment>
-    <comment ref="C11" authorId="9" shapeId="0" xr:uid="{1B8A75AC-A9FE-EB43-AD87-1FE8467FBB89}">
+    <comment ref="C11" authorId="6" shapeId="0" xr:uid="{1B8A75AC-A9FE-EB43-AD87-1FE8467FBB89}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -133,7 +106,7 @@
     Using the nursery pathway for smuggled budwood (though it is distributed the same as food). Food is used for smuggled curry leaves etc</t>
       </text>
     </comment>
-    <comment ref="C12" authorId="10" shapeId="0" xr:uid="{54D29E90-6B5C-7E47-B3EC-ABC5E05A1AF6}">
+    <comment ref="C12" authorId="7" shapeId="0" xr:uid="{54D29E90-6B5C-7E47-B3EC-ABC5E05A1AF6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -141,7 +114,7 @@
     Using the nursery pathway for smuggled budwood (though it is distributed the same as food)</t>
       </text>
     </comment>
-    <comment ref="C13" authorId="11" shapeId="0" xr:uid="{8CF3C082-6166-8F42-B7A9-381AB738D432}">
+    <comment ref="C13" authorId="8" shapeId="0" xr:uid="{8CF3C082-6166-8F42-B7A9-381AB738D432}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -149,7 +122,7 @@
     Some stored product needed to be distributed by residents as opposed to the conventional “food” pathway because of differing establishment probs. This shouldn’t make a difference as both pathways are distributed the same way</t>
       </text>
     </comment>
-    <comment ref="D14" authorId="12" shapeId="0" xr:uid="{5768F99D-9AC8-9B43-BDB9-4E209772FF9A}">
+    <comment ref="D14" authorId="9" shapeId="0" xr:uid="{5768F99D-9AC8-9B43-BDB9-4E209772FF9A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -157,7 +130,7 @@
     Too few records to reliably estimate climate suitability</t>
       </text>
     </comment>
-    <comment ref="A16" authorId="13" shapeId="0" xr:uid="{07597060-6049-9840-92E5-7BD1213CB6F8}">
+    <comment ref="A16" authorId="10" shapeId="0" xr:uid="{07597060-6049-9840-92E5-7BD1213CB6F8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -272,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="279">
   <si>
     <t>Citrus Canker</t>
   </si>
@@ -562,25 +535,16 @@
     <t>Defining distribution of host land use</t>
   </si>
   <si>
-    <t>risk_layers/biotic/raw_data/ACLUM/clum_50m1218m.tif</t>
-  </si>
-  <si>
     <t>NVIS raster path</t>
   </si>
   <si>
     <t>Defining distribution of vegetation classes in which the pest might establish</t>
   </si>
   <si>
-    <t>risk_layers/biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
-  </si>
-  <si>
     <t>NDVI raster path</t>
   </si>
   <si>
     <t>Optional component of habitat</t>
-  </si>
-  <si>
-    <t>risk_layers/biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
   </si>
   <si>
     <t xml:space="preserve">Postcode shapefile path </t>
@@ -612,13 +576,7 @@
     </r>
   </si>
   <si>
-    <t>risk_layers/pathway/raw_data/Containers/postal_areas/POA_2011_AUST.shp</t>
-  </si>
-  <si>
     <t>Containers data path</t>
-  </si>
-  <si>
-    <t>risk_layers/pathway/raw_data/Containers/containers_bypostcode.xls</t>
   </si>
   <si>
     <t>Marine ports data path</t>
@@ -650,9 +608,6 @@
     </r>
   </si>
   <si>
-    <t>risk_layers/pathway/raw_data/Ports/ports.csv</t>
-  </si>
-  <si>
     <t>Fertiliser data path</t>
   </si>
   <si>
@@ -680,9 +635,6 @@
       </rPr>
       <t xml:space="preserve"> pathway)</t>
     </r>
-  </si>
-  <si>
-    <t>risk_layers/pathway/raw_data/Fertiliser/fertiliser2016_17.csv</t>
   </si>
   <si>
     <t>NRM shapefile path</t>
@@ -725,9 +677,6 @@
     </r>
   </si>
   <si>
-    <t>risk_layers/pathway/raw_data/Fertiliser/nrm_regions/NRMR_2016_AUST.shp</t>
-  </si>
-  <si>
     <t>Airport distance penalty (tourists)</t>
   </si>
   <si>
@@ -837,9 +786,6 @@
     <t>Password for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
   </si>
   <si>
-    <t>cebra</t>
-  </si>
-  <si>
     <t>Lymantria dispar japonica, Lymantria dispar</t>
   </si>
   <si>
@@ -1146,9 +1092,6 @@
     <t>Defines wind speed polygons to be rasterised to the coastline</t>
   </si>
   <si>
-    <t>risk_layers/pathway/raw_data/Wind/wind.gpkg</t>
-  </si>
-  <si>
     <t>Food, Nursery, Residents, northwind</t>
   </si>
   <si>
@@ -1218,9 +1161,6 @@
     <t>Apis mellifera</t>
   </si>
   <si>
-    <t>om#V&gt;nzeCa3E^aU2.n8xZLCS</t>
-  </si>
-  <si>
     <t>abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
   </si>
   <si>
@@ -1264,6 +1204,33 @@
   </si>
   <si>
     <t>biotic/citrus_native_hosts_example.tif</t>
+  </si>
+  <si>
+    <t>biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
+  </si>
+  <si>
+    <t>biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Containers/postal_areas/POA_2011_AUST.gpkg</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Containers/containers_bypostcode.xls</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Ports/ports.csv</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Fertiliser/fertiliser2016_17.csv</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Fertiliser/nrm_regions/NRMR_2016_AUST.shp</t>
+  </si>
+  <si>
+    <t>pathway/raw_data/Wind/wind.gpkg</t>
+  </si>
+  <si>
+    <t>biotic/raw_data/ACLUM/clum_50m1220m.tif</t>
   </si>
 </sst>
 </file>
@@ -2857,7 +2824,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="James Camac" id="{5FECB3BD-2E80-7D43-8674-E02E36A53731}" userId="James Camac" providerId="None"/>
   <person displayName="Microsoft Office User" id="{6A9DCC67-FBF4-704D-B1D5-757B1F3E3D2F}" userId="Microsoft Office User" providerId="None"/>
   <person displayName="James Camac" id="{DA9BAF45-D29A-2944-A4AB-C22BE1376504}" userId="S::james.camac@unimelb.edu.au::f4070045-96f0-48f7-a1ff-0423c56da654" providerId="AD"/>
   <person displayName="John Baumgartner" id="{FA70A01E-4BFB-914D-B201-A3FFB558879F}" userId="S::john.baumgartner@unimelb.edu.au::64e08097-c003-4539-ab7e-80504fe98ad0" providerId="AD"/>
@@ -3167,12 +3133,6 @@
   <threadedComment ref="D2" dT="2021-04-16T05:14:03.11" personId="{DA9BAF45-D29A-2944-A4AB-C22BE1376504}" id="{03D81196-E77D-0F4D-A067-33B2632A711C}">
     <text>Insufficient occurrence data</text>
   </threadedComment>
-  <threadedComment ref="M2" dT="2021-03-23T02:28:08.28" personId="{DA9BAF45-D29A-2944-A4AB-C22BE1376504}" id="{0196C33E-8F8E-E84B-9ABD-5D6E98C41E55}">
-    <text>Very few records of Citrus canker. Decided to use CABI records as approximation data rather than the 50 odd GBIF records</text>
-  </threadedComment>
-  <threadedComment ref="N2" dT="2021-03-19T04:28:18.01" personId="{5FECB3BD-2E80-7D43-8674-E02E36A53731}" id="{08970612-EB31-8641-B619-72C12D702C77}">
-    <text>Need to extra work here. Some records are in USA jurisdictions which don’t have it. Will need to manually remove.</text>
-  </threadedComment>
   <threadedComment ref="K3" dT="2020-12-09T03:13:18.71" personId="{6A9DCC67-FBF4-704D-B1D5-757B1F3E3D2F}" id="{52D97D8B-AA8C-7B49-9DAC-3B43BC703016}">
     <text>Modelled together to overcome potential identification problems</text>
   </threadedComment>
@@ -3181,9 +3141,6 @@
   </threadedComment>
   <threadedComment ref="C8" dT="2021-03-23T00:25:42.82" personId="{DA9BAF45-D29A-2944-A4AB-C22BE1376504}" id="{30BEA44C-71B5-C346-82C3-2AF8168E4B6B}">
     <text>Note that for fruit flies we have broken up the passenger pathway by resident &amp; tourist. We also add a Torres strait passenger pathway… and because there are two separate food pathways with different establishment parameters we’ve used goods to distribute the second.</text>
-  </threadedComment>
-  <threadedComment ref="K8" dT="2020-10-19T00:39:51.74" personId="{FA70A01E-4BFB-914D-B201-A3FFB558879F}" id="{A62E6B1F-E4EB-984E-B747-9546652AB2B8}">
-    <text>Have added synonyms as per risk maps phase 1</text>
   </threadedComment>
   <threadedComment ref="D9" dT="2021-03-23T00:03:24.66" personId="{DA9BAF45-D29A-2944-A4AB-C22BE1376504}" id="{24C12BAB-7D3D-1D41-A58D-58EA66DA6BBC}">
     <text>Too few records for estimating climate</text>
@@ -3255,7 +3212,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3297,49 +3256,45 @@
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>138</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>265</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C7" s="36">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>94</v>
       </c>
@@ -3347,103 +3302,103 @@
         <v>95</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>96</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="C9" s="30" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>101</v>
-      </c>
       <c r="C10" s="30" t="s">
-        <v>102</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>105</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>107</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>116</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C17" s="31">
         <f>LN(0.5)/200</f>
@@ -3452,10 +3407,10 @@
     </row>
     <row r="18" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C18" s="31">
         <f>LN(0.5)/10</f>
@@ -3571,11 +3526,11 @@
   </sheetPr>
   <dimension ref="A1:AT21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C1" s="48" t="s">
         <v>8</v>
@@ -3647,19 +3602,19 @@
         <v>65</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="J1" s="49" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="L1" s="50" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="N1" s="48" t="s">
         <v>67</v>
@@ -3668,94 +3623,94 @@
         <v>68</v>
       </c>
       <c r="P1" s="49" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="Q1" s="51" t="s">
         <v>69</v>
       </c>
       <c r="R1" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="X1" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y1" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z1" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB1" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="AD1" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="AE1" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="U1" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="V1" s="48" t="s">
+      <c r="AF1" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="W1" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="X1" s="48" t="s">
+      <c r="AG1" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="AH1" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="AI1" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AJ1" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AK1" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="AC1" s="48" t="s">
+      <c r="AL1" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM1" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="AD1" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE1" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF1" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="AG1" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="AH1" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="AI1" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="AJ1" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK1" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL1" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="AM1" s="48" t="s">
-        <v>164</v>
-      </c>
       <c r="AN1" s="48" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="AO1" s="48" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="AP1" s="48" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="AQ1" s="48" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="AR1" s="48" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="AS1" s="48" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="AT1" s="52" t="s">
         <v>70</v>
@@ -3767,13 +3722,13 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="8" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F2" s="9" t="b">
         <v>0</v>
@@ -3783,7 +3738,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="8"/>
@@ -3796,10 +3751,10 @@
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
@@ -3808,10 +3763,10 @@
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="AD2" s="8"/>
       <c r="AE2" s="8"/>
@@ -3820,10 +3775,10 @@
       <c r="AH2" s="8"/>
       <c r="AI2" s="8"/>
       <c r="AJ2" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="AL2" s="8"/>
       <c r="AM2" s="8"/>
@@ -3839,17 +3794,17 @@
     </row>
     <row r="3" spans="1:46" s="41" customFormat="1" ht="86" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D3" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F3" s="11" t="b">
         <v>1</v>
@@ -3858,19 +3813,19 @@
         <v>1</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="12" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="L3" s="13">
         <v>1970</v>
       </c>
       <c r="M3" s="12"/>
       <c r="N3" s="12" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
@@ -3887,24 +3842,24 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
       <c r="AD3" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="AF3" s="12" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AH3" s="12"/>
       <c r="AI3" s="12"/>
@@ -3924,19 +3879,19 @@
     </row>
     <row r="4" spans="1:46" s="41" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D4" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F4" s="11" t="b">
         <v>1</v>
@@ -3948,7 +3903,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="12" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="L4" s="13">
         <v>1970</v>
@@ -3964,38 +3919,38 @@
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
       <c r="AF4" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="AH4" s="12"/>
       <c r="AI4" s="12"/>
       <c r="AJ4" s="12" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AL4" s="12"/>
       <c r="AM4" s="12"/>
@@ -4011,19 +3966,19 @@
     </row>
     <row r="5" spans="1:46" s="41" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D5" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F5" s="11" t="b">
         <v>1</v>
@@ -4037,7 +3992,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="M5" s="12" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="11"/>
@@ -4049,38 +4004,38 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
       <c r="T5" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
       <c r="AE5" s="12"/>
       <c r="AF5" s="12" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="12" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AL5" s="12"/>
       <c r="AM5" s="12"/>
@@ -4100,13 +4055,13 @@
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D6" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F6" s="11" t="b">
         <v>1</v>
@@ -4120,10 +4075,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
       <c r="M6" s="12" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -4134,44 +4089,44 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
       <c r="AD6" s="12" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="AF6" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AH6" s="12"/>
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="AM6" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AN6" s="12"/>
       <c r="AO6" s="12"/>
@@ -4185,16 +4140,16 @@
     </row>
     <row r="7" spans="1:46" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D7" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F7" s="11" t="b">
         <v>1</v>
@@ -4203,33 +4158,33 @@
         <v>0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="R7" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AJ7" s="12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AL7" s="12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="AM7" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AT7" s="39">
         <v>5000</v>
@@ -4237,16 +4192,16 @@
     </row>
     <row r="8" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D8" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F8" s="11" t="b">
         <v>1</v>
@@ -4255,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>71</v>
@@ -4264,40 +4219,40 @@
         <v>1970</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="W8" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AJ8" s="12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AL8" s="12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="AM8" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AT8" s="39">
         <v>5000</v>
@@ -4305,16 +4260,16 @@
     </row>
     <row r="9" spans="1:46" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D9" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F9" s="11" t="b">
         <v>1</v>
@@ -4323,38 +4278,38 @@
         <v>0</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="N9" s="12"/>
       <c r="R9" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="W9" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AJ9" s="12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AL9" s="12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="AM9" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AT9" s="39">
         <v>5000</v>
@@ -4362,16 +4317,16 @@
     </row>
     <row r="10" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D10" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F10" s="11" t="b">
         <v>1</v>
@@ -4380,47 +4335,47 @@
         <v>0</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="L10" s="13">
         <v>1970</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="W10" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AJ10" s="12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AL10" s="12" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="AM10" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AT10" s="39">
         <v>5000</v>
@@ -4428,19 +4383,19 @@
     </row>
     <row r="11" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D11" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F11" s="11" t="b">
         <v>1</v>
@@ -4449,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>80</v>
@@ -4458,37 +4413,37 @@
         <v>1970</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="P11" s="54">
         <v>100000</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="AH11" s="12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="AI11" s="12" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="AJ11" s="12" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AN11" s="12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="AO11" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AT11" s="39">
         <v>5000</v>
@@ -4496,19 +4451,19 @@
     </row>
     <row r="12" spans="1:46" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D12" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F12" s="11" t="b">
         <v>1</v>
@@ -4517,27 +4472,27 @@
         <v>0</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="T12" s="12" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="AH12" s="12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="AI12" s="12" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="AJ12" s="12" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AT12" s="39">
         <v>5000</v>
@@ -4545,16 +4500,16 @@
     </row>
     <row r="13" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D13" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F13" s="11" t="b">
         <v>0</v>
@@ -4566,28 +4521,28 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="T13" s="12" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="AF13" s="12" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AJ13" s="12" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AL13" s="12" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="AM13" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AT13" s="39">
         <v>5000</v>
@@ -4595,16 +4550,16 @@
     </row>
     <row r="14" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D14" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F14" s="11" t="b">
         <v>1</v>
@@ -4616,22 +4571,22 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="T14" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AF14" s="12" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="AG14" s="12" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="AL14" s="12" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="AM14" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AT14" s="39">
         <v>5000</v>
@@ -4639,16 +4594,16 @@
     </row>
     <row r="15" spans="1:46" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D15" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F15" s="11" t="b">
         <v>1</v>
@@ -4665,25 +4620,25 @@
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AF15" s="12" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="AG15" s="12" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="AL15" s="12" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="AM15" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="AT15" s="39">
         <v>5000</v>
@@ -4691,19 +4646,19 @@
     </row>
     <row r="16" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="45" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D16" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F16" s="11" t="b">
         <v>1</v>
@@ -4720,49 +4675,49 @@
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="Q16" s="14">
         <f t="shared" ref="Q16" si="0">LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="Z16" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="AA16" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AL16" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="AM16" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AT16" s="39">
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="1:46" ht="119" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D17" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F17" s="11" t="b">
         <v>1</v>
@@ -4779,29 +4734,29 @@
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="12" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="Q17" s="14">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="Z17" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="AA17" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AL17" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="AM17" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AT17" s="39">
         <v>5000</v>
@@ -4809,19 +4764,19 @@
     </row>
     <row r="18" spans="1:46" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="45" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D18" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F18" s="11" t="b">
         <v>1</v>
@@ -4838,49 +4793,49 @@
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="Q18" s="14">
         <f t="shared" ref="Q18" si="1">LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="Z18" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="AA18" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AL18" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="AM18" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AT18" s="39">
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:46" ht="102" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:46" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="45" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D19" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F19" s="11" t="b">
         <v>1</v>
@@ -4897,29 +4852,29 @@
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="Q19" s="14">
         <f>LN(0.5)/1</f>
         <v>-0.69314718055994529</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="Z19" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="AA19" s="12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AL19" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="AM19" s="12" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AT19" s="39">
         <v>5000</v>
@@ -4927,19 +4882,19 @@
     </row>
     <row r="20" spans="1:46" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D20" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F20" s="16" t="b">
         <v>0</v>
@@ -4948,16 +4903,16 @@
         <v>0</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="AH20" s="12" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="AI20" s="12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="AT20" s="39">
         <v>5000</v>
@@ -4965,17 +4920,17 @@
     </row>
     <row r="21" spans="1:46" s="43" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="45" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="12" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D21" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F21" s="17" t="b">
         <v>1</v>
@@ -4989,7 +4944,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="12" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="N21" s="40"/>
       <c r="O21" s="17"/>
@@ -5007,20 +4962,20 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AA21" s="12" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
       <c r="AF21" s="12" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="AG21" s="12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="AH21" s="12"/>
       <c r="AI21" s="12"/>
@@ -5914,7 +5869,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Use config package for gbif credentials
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/packages/edmaps/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B817A594-CAAB-DD49-BCDC-E3A618AB1033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC6030-EC0E-E14C-9955-841F4E442569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="135">
   <si>
     <t>Citrus Canker</t>
   </si>
@@ -170,18 +170,6 @@
   </si>
   <si>
     <t>110-117, 120-125, 130-134, 210, 220-222, 310-314, 320-338, 340-349, 350-353, 360-365, 410-414, 420-424, 430-439, 440-449, 450-454, 460-465, 510-515, 520-528, 530-538, 540-545, 550-555, 560-567, 570-575, 580-584, 590-595, 610-614, 620-623, 630-633, 640-644, 650-654, 660-663</t>
-  </si>
-  <si>
-    <t>GBIF username</t>
-  </si>
-  <si>
-    <t>GBIF password</t>
-  </si>
-  <si>
-    <t>Username for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
-  </si>
-  <si>
-    <t>Password for authenticated GBIF downloads. This is optional, but is more efficient for large queries.</t>
   </si>
   <si>
     <t>Lymantria dispar japonica, Lymantria dispar</t>
@@ -928,20 +916,9 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE7E6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE7E6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -999,9 +976,20 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -1405,11 +1393,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECE737A-7CDD-D24C-B69F-489918F5C8E0}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1431,7 +1417,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>17</v>
@@ -1439,21 +1425,21 @@
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="44">
         <v>1000</v>
@@ -1461,13 +1447,13 @@
     </row>
     <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1483,184 +1469,152 @@
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="43"/>
-    </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="43"/>
-    </row>
-    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="43">
+      <c r="C8" s="43">
         <v>1.0000000000000001E-5</v>
       </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>74</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D11" s="47"/>
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
     </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-    </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-    </row>
-    <row r="14" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>72</v>
+    <row r="12" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="D11:F13"/>
+    <mergeCell ref="D9:F11"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(ISBLANK($C$3), ISBLANK($C$5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>AND(ISBLANK($C$4), ISBLANK($C$5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>ISBLANK($C$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>AND(NOT(ISBLANK($C$8)), ISBLANK($C$7))</formula>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>ISBLANK($C$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="5" priority="8">
-      <formula>AND(NOT(ISBLANK($C$7)), ISBLANK($C$8))</formula>
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>ISBLANK($C$8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>ISBLANK($C$9)</formula>
+  <conditionalFormatting sqref="C9 C12">
+    <cfRule type="containsBlanks" dxfId="8" priority="12">
+      <formula>LEN(TRIM(C9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>ISBLANK($C$10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11 C14">
-    <cfRule type="containsBlanks" dxfId="2" priority="12">
-      <formula>LEN(TRIM(C11))=0</formula>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>ISBLANK($C$11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="1" priority="10">
-      <formula>ISBLANK($C$12)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="0" priority="11">
-      <formula>ISBLANK($C$13)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="17">
+  <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Output resolution" prompt="Spatial resolution of outputs. This will override the resolution of a tempate raster, if provided below. Enter a single value, i.e., horizontal resolution must equal vertical resolution." sqref="A4:C4" xr:uid="{A90ADFE1-5D41-E64D-84D1-33456EA8CD47}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Template raster" prompt="Path to a raster file defining the output extent, resolution, and Coordinate Reference System of outputs. If Output resolution and/or Coordinate Reference System are specified above, they will be used in place of the raster's corresponding attributes." sqref="A5:C5" xr:uid="{BC4AAD4F-5F0F-B34C-9013-8108ED21140C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Coordinate reference system" prompt="Define the coordinate reference system (projection) of outputs as an EPSG code. Default is Mollweide (global equal area). See https://projectionwizard.org and https://epsg.io for guidance. This will override the CRS of the template raster (if provided)." sqref="A3:C3" xr:uid="{5AAE6BEA-C593-B74E-851D-4F7F3BCA0A11}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to land use raster" prompt="File path (absolute or relative to the R working directory) to the land use raster dataset. " sqref="A11:C11" xr:uid="{C065FC62-2EB2-7745-9D49-CE87D1DAA229}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to vegetation class raster" prompt="File path (absolute or relative to the R working directory) to the vegetation class raster dataset. " sqref="A12:C12" xr:uid="{DC61A581-1C0C-1A4F-A664-9D47F1851D6F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="A14:C14" xr:uid="{7A8D64D8-DAED-8047-8A02-77BFC5102C46}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="A10:B10" xr:uid="{5551A4E7-D518-FA46-B47B-11BEACBD3309}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be a number between 0 and 1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="C10" xr:uid="{2EC6111F-600F-C947-8E18-A1F2DAB839DB}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to land use raster" prompt="File path (absolute or relative to the R working directory) to the land use raster dataset. " sqref="A9:C9" xr:uid="{C065FC62-2EB2-7745-9D49-CE87D1DAA229}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to vegetation class raster" prompt="File path (absolute or relative to the R working directory) to the vegetation class raster dataset. " sqref="A10:C10" xr:uid="{DC61A581-1C0C-1A4F-A664-9D47F1851D6F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="A12:C12" xr:uid="{7A8D64D8-DAED-8047-8A02-77BFC5102C46}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="A8:B8" xr:uid="{5551A4E7-D518-FA46-B47B-11BEACBD3309}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be a number between 0 and 1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="C8" xr:uid="{2EC6111F-600F-C947-8E18-A1F2DAB839DB}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C7" xr:uid="{D38028ED-82BC-9849-9F8B-366567697BB4}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C9" xr:uid="{3F0B3965-4CB6-8B44-8C48-BC8387D0780B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C7" xr:uid="{3F0B3965-4CB6-8B44-8C48-BC8387D0780B}">
       <formula1>"boundaries,osm"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A7:B7" xr:uid="{FD0C643F-04C4-D148-9780-278EF840A653}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A8:B8" xr:uid="{E3419BB0-89D5-A241-999A-9B20029F871D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A9:B9" xr:uid="{2137D998-D258-7341-8143-F5827C46783C}"/>
-    <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C8" xr:uid="{D3C64AEF-B848-544A-B1D9-B92F96FD39F0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A7:B7" xr:uid="{2137D998-D258-7341-8143-F5827C46783C}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C6" xr:uid="{29A5A917-42A1-FA48-BF43-0D0D31D1E9C3}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A6:B6" xr:uid="{DC6BABA3-649A-3642-B4F4-F5BF65DA5D95}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A13:C13" xr:uid="{087AD0AA-D382-B946-9A47-A4BE5E5C03F8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A11:C11" xr:uid="{087AD0AA-D382-B946-9A47-A4BE5E5C03F8}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1694,37 +1648,37 @@
   <sheetData>
     <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>6</v>
@@ -1733,7 +1687,7 @@
         <v>7</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1746,13 +1700,13 @@
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>93</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
@@ -1764,7 +1718,7 @@
     </row>
     <row r="3" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="30" t="s">
@@ -1774,47 +1728,47 @@
         <v>34</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H3" s="29"/>
       <c r="I3" s="29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J3" s="31">
         <v>1970</v>
       </c>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="39"/>
     </row>
     <row r="4" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>35</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J4" s="27">
         <v>1970</v>
@@ -1826,27 +1780,27 @@
     </row>
     <row r="5" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="31"/>
       <c r="K5" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
@@ -1862,27 +1816,27 @@
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="27"/>
       <c r="K6" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M6" s="25"/>
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="30" t="s">
@@ -1890,13 +1844,13 @@
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F7" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -1908,7 +1862,7 @@
     </row>
     <row r="8" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26" t="s">
@@ -1916,13 +1870,13 @@
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25" t="s">
@@ -1932,17 +1886,17 @@
         <v>1970</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="30" t="s">
@@ -1950,13 +1904,13 @@
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -1968,7 +1922,7 @@
     </row>
     <row r="10" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="32" t="s">
@@ -1976,31 +1930,31 @@
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J10" s="27">
         <v>1970</v>
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>4</v>
@@ -2010,13 +1964,13 @@
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29" t="s">
@@ -2026,17 +1980,17 @@
         <v>1970</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>4</v>
@@ -2046,11 +2000,11 @@
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -2062,7 +2016,7 @@
     </row>
     <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="30" t="s">
@@ -2070,11 +2024,11 @@
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
@@ -2086,7 +2040,7 @@
     </row>
     <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
@@ -2094,11 +2048,11 @@
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -2110,7 +2064,7 @@
     </row>
     <row r="15" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="30" t="s">
@@ -2118,11 +2072,11 @@
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29" t="s">
@@ -2133,14 +2087,14 @@
       </c>
       <c r="K15" s="29"/>
       <c r="L15" s="29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="M15" s="29"/>
       <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>3</v>
@@ -2150,11 +2104,11 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25" t="s">
@@ -2165,14 +2119,14 @@
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="38"/>
     </row>
     <row r="17" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>3</v>
@@ -2182,11 +2136,11 @@
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29" t="s">
@@ -2197,14 +2151,14 @@
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="M17" s="29"/>
       <c r="N17" s="39"/>
     </row>
     <row r="18" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>3</v>
@@ -2214,11 +2168,11 @@
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="25" t="s">
@@ -2229,14 +2183,14 @@
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M18" s="25"/>
       <c r="N18" s="38"/>
     </row>
     <row r="19" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>3</v>
@@ -2246,11 +2200,11 @@
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="29" t="s">
@@ -2261,14 +2215,14 @@
       </c>
       <c r="K19" s="29"/>
       <c r="L19" s="29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M19" s="29"/>
       <c r="N19" s="39"/>
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>3</v>
@@ -2278,11 +2232,11 @@
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
@@ -2294,7 +2248,7 @@
     </row>
     <row r="21" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="35" t="s">
@@ -2302,17 +2256,17 @@
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
       <c r="J21" s="36"/>
       <c r="K21" s="34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
@@ -2320,22 +2274,22 @@
     </row>
     <row r="22" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>35</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -2403,22 +2357,22 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2426,7 +2380,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12">
         <v>1.595</v>
@@ -2441,7 +2395,7 @@
         <v>0.2</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2449,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C3" s="12">
         <v>20</v>
@@ -2464,7 +2418,7 @@
         <v>1E-4</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2472,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" s="12">
         <v>20</v>
@@ -2487,15 +2441,15 @@
         <v>1E-4</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12">
         <v>0.05</v>
@@ -2510,15 +2464,15 @@
         <v>0.1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12">
         <v>0.01</v>
@@ -2533,15 +2487,15 @@
         <v>0.02</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12">
         <v>0.16500000000000001</v>
@@ -2556,15 +2510,15 @@
         <v>0.05</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" s="12">
         <v>8.6999999999999994E-2</v>
@@ -2579,15 +2533,15 @@
         <v>0.9</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C9" s="12">
         <v>0.04</v>
@@ -2602,15 +2556,15 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C10" s="12">
         <v>2.8000000000000001E-2</v>
@@ -2625,15 +2579,15 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C11" s="12">
         <v>7.0000000000000001E-3</v>
@@ -2648,15 +2602,15 @@
         <v>0.01</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C12" s="12">
         <v>8.6999999999999994E-2</v>
@@ -2671,15 +2625,15 @@
         <v>0.9</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="12">
         <v>0.04</v>
@@ -2694,15 +2648,15 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C14" s="12">
         <v>2.8000000000000001E-2</v>
@@ -2717,15 +2671,15 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C15" s="12">
         <v>7.0000000000000001E-3</v>
@@ -2740,7 +2694,7 @@
         <v>0.01</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2748,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C16" s="12">
         <v>2</v>
@@ -2763,7 +2717,7 @@
         <v>0.05</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2771,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C17" s="12">
         <v>3</v>
@@ -2786,7 +2740,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2794,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C18" s="12">
         <v>3</v>
@@ -2809,7 +2763,7 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2817,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -2832,7 +2786,7 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2840,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C20" s="12">
         <v>0.1</v>
@@ -2855,15 +2809,15 @@
         <v>0.1</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C21" s="12">
         <v>7</v>
@@ -2878,15 +2832,15 @@
         <v>0.01</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C22" s="12">
         <v>3</v>
@@ -2901,15 +2855,15 @@
         <v>0.01</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C23" s="12">
         <v>1.4890000000000001</v>
@@ -2924,15 +2878,15 @@
         <v>0.05</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C24" s="12">
         <v>0.5</v>
@@ -2947,15 +2901,15 @@
         <v>0.01</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C25" s="12">
         <v>7</v>
@@ -2970,15 +2924,15 @@
         <v>0.01</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C26" s="12">
         <v>3</v>
@@ -2993,15 +2947,15 @@
         <v>0.01</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C27" s="12">
         <v>1</v>
@@ -3016,15 +2970,15 @@
         <v>0.01</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C28" s="12">
         <v>1.4890000000000001</v>
@@ -3039,15 +2993,15 @@
         <v>0.05</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C29" s="12">
         <v>0.5</v>
@@ -3062,15 +3016,15 @@
         <v>0.01</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C30" s="12">
         <v>7</v>
@@ -3085,15 +3039,15 @@
         <v>0.01</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="12">
         <v>3</v>
@@ -3108,15 +3062,15 @@
         <v>0.01</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C32" s="12">
         <v>1</v>
@@ -3131,15 +3085,15 @@
         <v>0.01</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C33" s="12">
         <v>1.4890000000000001</v>
@@ -3154,15 +3108,15 @@
         <v>0.05</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C34" s="12">
         <v>0.5</v>
@@ -3177,15 +3131,15 @@
         <v>0.01</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C35" s="12">
         <v>7</v>
@@ -3200,15 +3154,15 @@
         <v>0.01</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C36" s="12">
         <v>3</v>
@@ -3223,15 +3177,15 @@
         <v>0.01</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C37" s="12">
         <v>1</v>
@@ -3246,15 +3200,15 @@
         <v>0.01</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C38" s="12">
         <v>1.4890000000000001</v>
@@ -3269,15 +3223,15 @@
         <v>0.05</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="12">
         <v>0.5</v>
@@ -3292,15 +3246,15 @@
         <v>0.01</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C40" s="12">
         <v>0.89200000000000002</v>
@@ -3315,15 +3269,15 @@
         <v>0.3</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41" s="12">
         <v>0.3</v>
@@ -3338,15 +3292,15 @@
         <v>0.3</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C42" s="12">
         <v>5</v>
@@ -3361,15 +3315,15 @@
         <v>0.01</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C43" s="12">
         <v>0.3</v>
@@ -3384,15 +3338,15 @@
         <v>0.1</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C44" s="12">
         <v>0.89200000000000002</v>
@@ -3407,15 +3361,15 @@
         <v>0.3</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C45" s="12">
         <v>0.3</v>
@@ -3430,15 +3384,15 @@
         <v>0.3</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="12">
         <v>5</v>
@@ -3453,15 +3407,15 @@
         <v>0.01</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C47" s="12">
         <v>6.0119999999999996</v>
@@ -3476,15 +3430,15 @@
         <v>0.02</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C48" s="12">
         <v>14.872</v>
@@ -3499,15 +3453,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C49" s="12">
         <v>1.0369999999999999</v>
@@ -3522,15 +3476,15 @@
         <v>0.1</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C50" s="12">
         <v>1.7649999999999999</v>
@@ -3545,15 +3499,15 @@
         <v>0.05</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C51" s="12">
         <v>1.488</v>
@@ -3568,15 +3522,15 @@
         <v>0.01</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C52" s="12">
         <v>10</v>
@@ -3591,15 +3545,15 @@
         <v>1E-3</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C53" s="12">
         <v>15.692</v>
@@ -3614,15 +3568,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C54" s="12">
         <v>1.488</v>
@@ -3637,15 +3591,15 @@
         <v>0.01</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C55" s="12">
         <v>10</v>
@@ -3660,15 +3614,15 @@
         <v>1E-3</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C56" s="12">
         <v>15.692</v>
@@ -3683,15 +3637,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -3706,15 +3660,15 @@
         <v>0.05</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C58" s="12">
         <v>0.1</v>
@@ -3729,15 +3683,15 @@
         <v>0.1</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C59" s="12">
         <v>3.6080000000000001</v>
@@ -3752,15 +3706,15 @@
         <v>0.05</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C60" s="12">
         <v>1</v>
@@ -3775,15 +3729,15 @@
         <v>0.05</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C61" s="12">
         <v>0.1</v>
@@ -3798,15 +3752,15 @@
         <v>0.1</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C62" s="12">
         <v>3.6080000000000001</v>
@@ -3821,15 +3775,15 @@
         <v>0.05</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C63" s="12">
         <v>1</v>
@@ -3844,15 +3798,15 @@
         <v>0.05</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C64" s="12">
         <v>0.1</v>
@@ -3867,15 +3821,15 @@
         <v>0.1</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C65" s="12">
         <v>3.6080000000000001</v>
@@ -3890,15 +3844,15 @@
         <v>0.05</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C66" s="12">
         <v>1</v>
@@ -3913,15 +3867,15 @@
         <v>0.05</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C67" s="12">
         <v>0.1</v>
@@ -3936,15 +3890,15 @@
         <v>0.1</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C68" s="12">
         <v>3.6080000000000001</v>
@@ -3959,15 +3913,15 @@
         <v>0.05</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C69" s="12">
         <v>1.8879999999999999</v>
@@ -3982,15 +3936,15 @@
         <v>0.2</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C70" s="12">
         <v>0.2</v>
@@ -4005,15 +3959,15 @@
         <v>0.2</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C71" s="12">
         <v>0.04</v>
@@ -4028,15 +3982,15 @@
         <v>0.5</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C72" s="12">
         <v>0.03</v>
@@ -4051,33 +4005,33 @@
         <v>0.5</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND(NOT(ISBLANK(A2)),COUNTIFS(A$2:A$1048576,A2,B$2:B$1048576,B2) &gt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>AND(NOT(ISBLANK(A2)),COUNTIFS(A$2:A$1048576,A2,B$2:B$1048576,B2)&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576 E2:E1048576">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(NOT(ISBLANK(C2)),NOT(ISBLANK(D2)),C2&gt;D2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576 F2:F1048576">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(NOT(ISBLANK(D2)),NOT(ISBLANK(C2)),D2&lt;C2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(NOT(ISBLANK($A2)),ISBLANK(B2))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implement targets; update parameters.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/packages/edmaps/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC6030-EC0E-E14C-9955-841F4E442569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321F5DF8-C4AE-6A4E-B474-F504356B5A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
   <sheets>
     <sheet name="Global parameters" sheetId="12" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="137">
   <si>
     <t>Citrus Canker</t>
   </si>
@@ -211,262 +211,268 @@
     <t>Occurrence csv file</t>
   </si>
   <si>
+    <t>Bee mites (Apis cerana)</t>
+  </si>
+  <si>
+    <t>Carambola fruit fly</t>
+  </si>
+  <si>
+    <t>Oriental fruit fly</t>
+  </si>
+  <si>
+    <t>New Guinea fruit fly</t>
+  </si>
+  <si>
+    <t>Pine sawyer beetle</t>
+  </si>
+  <si>
+    <t>Cicadella viridis (Xylella vector)</t>
+  </si>
+  <si>
+    <t>Xylella fastidiosa</t>
+  </si>
+  <si>
+    <t>Xylella (Graphocephala atropunctata)</t>
+  </si>
+  <si>
+    <t>Xylella (Homalodisca vitripennis)</t>
+  </si>
+  <si>
+    <t>Xylella (Philaenus spumarius)</t>
+  </si>
+  <si>
+    <t>HLB (Asiatic citrus psyllid)</t>
+  </si>
+  <si>
+    <t>HLB (African citrus psyllid)</t>
+  </si>
+  <si>
+    <t>Khapra beetle</t>
+  </si>
+  <si>
+    <t>Melon fruit fly</t>
+  </si>
+  <si>
+    <t>Processed data directory</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
+  </si>
+  <si>
+    <t>data/processed</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Population2016/pop_density_1000m.tif</t>
+  </si>
+  <si>
+    <t>These paths can be modified (e.g. to refer to updated datasets). However, it is the user's responsibility to ensure that the format/structure of the datasets match that of the datasets in the data repository found at https://github.com/jscamac/edmaps_data_Australia</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/biotic/citrus_native_hosts_example.tif</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/ACLUM/clum_50m1218m.tif</t>
+  </si>
+  <si>
+    <t>Use NDVI?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Climate suitability raster</t>
+  </si>
+  <si>
+    <t>Host raster</t>
+  </si>
+  <si>
+    <t>Vegetation classes</t>
+  </si>
+  <si>
+    <t>Land use classes</t>
+  </si>
+  <si>
+    <t>Species name</t>
+  </si>
+  <si>
+    <t>Use climate suitability</t>
+  </si>
+  <si>
+    <t>Leakage rate lower</t>
+  </si>
+  <si>
+    <t>Leakage rate upper</t>
+  </si>
+  <si>
+    <t>Viability lower</t>
+  </si>
+  <si>
+    <t>Viability upper</t>
+  </si>
+  <si>
+    <t>Arrival weights (raster)</t>
+  </si>
+  <si>
+    <t>Returning resident</t>
+  </si>
+  <si>
+    <t>Fertiliser</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Vessels</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>Goods</t>
+  </si>
+  <si>
+    <t>Tourist</t>
+  </si>
+  <si>
+    <t>Torres passenger</t>
+  </si>
+  <si>
+    <t>Nurserystock</t>
+  </si>
+  <si>
+    <t>North wind</t>
+  </si>
+  <si>
+    <t>Japanese pine sawyer beetle</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/fert_weights.tif</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/vessels_weight.tif</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/containers_weight.tif</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/tourists_weight.tif</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/torres_weight.tif</t>
+  </si>
+  <si>
+    <t>outputs/not_pest_specific/wind_weight.tif</t>
+  </si>
+  <si>
+    <t>Vegetation class raster path</t>
+  </si>
+  <si>
+    <t>Land use class raster path</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Pathway name</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Output resolution</t>
+  </si>
+  <si>
+    <t>Defines the coordinate reference system (projection) of outputs.</t>
+  </si>
+  <si>
+    <t>Defines the resolution (in map units) of outputs.</t>
+  </si>
+  <si>
+    <t>Coordinate reference system (EPSG code)</t>
+  </si>
+  <si>
+    <t>Used to define output coordinate reference system, extent, and resolution. Overrides the coordinate reference system and resolution specified above.</t>
+  </si>
+  <si>
+    <t>Template raster path</t>
+  </si>
+  <si>
+    <t>Defines directory to be used to store processed datasets. Must exist.</t>
+  </si>
+  <si>
+    <t>GBIF username</t>
+  </si>
+  <si>
+    <t>GBIF email address</t>
+  </si>
+  <si>
+    <t>WorldClim resolution</t>
+  </si>
+  <si>
+    <t>Resolution of climate data used when fitting/predicting climate suitability models. Data will be sourced from WorldClim, and projected/resampled to the target coordinate reference system and output resolution specified above.</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
     <t>Bee mites (Apis mellifera)</t>
   </si>
   <si>
-    <t>Bee mites (Apis cerana)</t>
-  </si>
-  <si>
-    <t>Carambola fruit fly</t>
-  </si>
-  <si>
-    <t>Oriental fruit fly</t>
-  </si>
-  <si>
-    <t>New Guinea fruit fly</t>
-  </si>
-  <si>
-    <t>Pine sawyer beetle</t>
-  </si>
-  <si>
-    <t>Cicadella viridis (Xylella vector)</t>
-  </si>
-  <si>
-    <t>Xylella fastidiosa</t>
-  </si>
-  <si>
-    <t>Xylella (Graphocephala atropunctata)</t>
-  </si>
-  <si>
-    <t>Xylella (Homalodisca vitripennis)</t>
-  </si>
-  <si>
-    <t>Xylella (Philaenus spumarius)</t>
-  </si>
-  <si>
-    <t>HLB (Asiatic citrus psyllid)</t>
-  </si>
-  <si>
-    <t>HLB (African citrus psyllid)</t>
-  </si>
-  <si>
-    <t>Khapra beetle</t>
-  </si>
-  <si>
-    <t>Melon fruit fly</t>
-  </si>
-  <si>
     <t>Apis mellifera</t>
   </si>
   <si>
-    <t>Processed data directory</t>
-  </si>
-  <si>
-    <t>data/biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
-  </si>
-  <si>
-    <t>data/biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
-  </si>
-  <si>
-    <t>data/processed</t>
-  </si>
-  <si>
-    <t>data/pathway/raw_data/Population2016/pop_density_1000m.tif</t>
-  </si>
-  <si>
-    <t>These paths can be modified (e.g. to refer to updated datasets). However, it is the user's responsibility to ensure that the format/structure of the datasets match that of the datasets in the data repository found at https://github.com/jscamac/edmaps_data_Australia</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>data/biotic/citrus_native_hosts_example.tif</t>
-  </si>
-  <si>
-    <t>data/biotic/raw_data/ACLUM/clum_50m1218m.tif</t>
-  </si>
-  <si>
-    <t>Use NDVI?</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Climate suitability raster</t>
-  </si>
-  <si>
-    <t>Host raster</t>
-  </si>
-  <si>
-    <t>Vegetation classes</t>
-  </si>
-  <si>
-    <t>Land use classes</t>
-  </si>
-  <si>
-    <t>Species name</t>
-  </si>
-  <si>
-    <t>Use climate suitability</t>
-  </si>
-  <si>
-    <t>Leakage rate lower</t>
-  </si>
-  <si>
-    <t>Leakage rate upper</t>
-  </si>
-  <si>
-    <t>Viability lower</t>
-  </si>
-  <si>
-    <t>Viability upper</t>
-  </si>
-  <si>
-    <t>Arrival weights (raster)</t>
-  </si>
-  <si>
-    <t>Returning resident</t>
-  </si>
-  <si>
-    <t>Fertiliser</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Vessels</t>
-  </si>
-  <si>
-    <t>Machinery</t>
-  </si>
-  <si>
-    <t>Containers</t>
-  </si>
-  <si>
-    <t>Goods</t>
-  </si>
-  <si>
-    <t>Tourist</t>
-  </si>
-  <si>
-    <t>Torres passenger</t>
-  </si>
-  <si>
-    <t>Nurserystock</t>
-  </si>
-  <si>
-    <t>North wind</t>
-  </si>
-  <si>
-    <t>Japanese pine sawyer beetle</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/fert_weights.tif</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/vessels_weight.tif</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/containers_weight.tif</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/tourists_weight.tif</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/torres_weight.tif</t>
-  </si>
-  <si>
-    <t>outputs/not_pest_specific/wind_weight.tif</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Vegetation class raster path</t>
-  </si>
-  <si>
-    <t>Land use class raster path</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Pathway name</t>
-  </si>
-  <si>
-    <t>Resolution</t>
-  </si>
-  <si>
-    <t>Output resolution</t>
-  </si>
-  <si>
-    <t>Defines the coordinate reference system (projection) of outputs.</t>
-  </si>
-  <si>
-    <t>Defines the resolution (in map units) of outputs.</t>
-  </si>
-  <si>
-    <t>Coordinate reference system (EPSG code)</t>
-  </si>
-  <si>
-    <t>ESRI:54009</t>
-  </si>
-  <si>
-    <t>Used to define output coordinate reference system, extent, and resolution. Overrides the coordinate reference system and resolution specified above.</t>
-  </si>
-  <si>
-    <t>United States, Germany, France, United Kingdom</t>
-  </si>
-  <si>
-    <t>/Users/jbau/projects/packages/edmaps/data/climate_suitability/Oriental_fruit_fly_aust_climsuit_1000.tif</t>
-  </si>
-  <si>
-    <t>Template raster path</t>
-  </si>
-  <si>
-    <t>Defines directory to be used to store processed datasets. Must exist.</t>
+    <t>data/climate_suitability/Oriental_fruit_fly_aust_climsuit_1000.tif</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,12 +559,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,7 +897,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -914,7 +914,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -990,6 +1070,46 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -1393,14 +1513,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECE737A-7CDD-D24C-B69F-489918F5C8E0}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="42" customWidth="1"/>
     <col min="3" max="3" width="41.5" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
   </cols>
@@ -1417,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>17</v>
@@ -1425,208 +1545,266 @@
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>129</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C3" s="44"/>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="44">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="44"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="44"/>
+    </row>
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="44">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="B8" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="43" t="b">
+      <c r="C9" s="43" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C10" s="43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B11" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C11" s="43">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="21" t="s">
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-    </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+    </row>
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+    </row>
+    <row r="15" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-    </row>
-    <row r="12" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="D9:F11"/>
+    <mergeCell ref="D12:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="16" priority="4">
-      <formula>AND(ISBLANK($C$3), ISBLANK($C$5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="15" priority="5">
-      <formula>AND(ISBLANK($C$4), ISBLANK($C$5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="containsBlanks" dxfId="14" priority="1">
-      <formula>LEN(TRIM(C5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>ISBLANK($C$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="10" priority="3">
-      <formula>ISBLANK($C$7)</formula>
+    <cfRule type="expression" dxfId="23" priority="6">
+      <formula>AND(ISBLANK($C$3), ISBLANK($C$8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>ISBLANK($C$8)</formula>
+    <cfRule type="containsBlanks" dxfId="20" priority="3">
+      <formula>LEN(TRIM(C8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9 C12">
-    <cfRule type="containsBlanks" dxfId="8" priority="12">
-      <formula>LEN(TRIM(C9))=0</formula>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="19" priority="4">
+      <formula>ISBLANK($C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>ISBLANK($C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>ISBLANK($C$11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="13">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Output resolution" prompt="Spatial resolution of outputs. This will override the resolution of a tempate raster, if provided below. Enter a single value, i.e., horizontal resolution must equal vertical resolution." sqref="A4:C4" xr:uid="{A90ADFE1-5D41-E64D-84D1-33456EA8CD47}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Template raster" prompt="Path to a raster file defining the output extent, resolution, and Coordinate Reference System of outputs. If Output resolution and/or Coordinate Reference System are specified above, they will be used in place of the raster's corresponding attributes." sqref="A5:C5" xr:uid="{BC4AAD4F-5F0F-B34C-9013-8108ED21140C}"/>
+  <conditionalFormatting sqref="C12 C15">
+    <cfRule type="containsBlanks" dxfId="16" priority="14">
+      <formula>LEN(TRIM(C12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="15" priority="12">
+      <formula>ISBLANK($C$13)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>ISBLANK($C$14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="15">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Output resolution" prompt="Spatial resolution of outputs. This will override the resolution of a tempate raster, if provided below. Enter a single value, i.e., horizontal resolution must equal vertical resolution." sqref="A4:C4 A6:C7" xr:uid="{A90ADFE1-5D41-E64D-84D1-33456EA8CD47}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Template raster" prompt="Path to a raster file defining the output extent, resolution, and Coordinate Reference System of outputs. If Output resolution and/or Coordinate Reference System are specified above, they will be used in place of the raster's corresponding attributes." sqref="A8:C8" xr:uid="{BC4AAD4F-5F0F-B34C-9013-8108ED21140C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Coordinate reference system" prompt="Define the coordinate reference system (projection) of outputs as an EPSG code. Default is Mollweide (global equal area). See https://projectionwizard.org and https://epsg.io for guidance. This will override the CRS of the template raster (if provided)." sqref="A3:C3" xr:uid="{5AAE6BEA-C593-B74E-851D-4F7F3BCA0A11}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to land use raster" prompt="File path (absolute or relative to the R working directory) to the land use raster dataset. " sqref="A9:C9" xr:uid="{C065FC62-2EB2-7745-9D49-CE87D1DAA229}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to vegetation class raster" prompt="File path (absolute or relative to the R working directory) to the vegetation class raster dataset. " sqref="A10:C10" xr:uid="{DC61A581-1C0C-1A4F-A664-9D47F1851D6F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="A12:C12" xr:uid="{7A8D64D8-DAED-8047-8A02-77BFC5102C46}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="A8:B8" xr:uid="{5551A4E7-D518-FA46-B47B-11BEACBD3309}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be a number between 0 and 1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="C8" xr:uid="{2EC6111F-600F-C947-8E18-A1F2DAB839DB}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to land use raster" prompt="File path (absolute or relative to the R working directory) to the land use raster dataset. " sqref="A12:C12" xr:uid="{C065FC62-2EB2-7745-9D49-CE87D1DAA229}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to vegetation class raster" prompt="File path (absolute or relative to the R working directory) to the vegetation class raster dataset. " sqref="A13:C13" xr:uid="{DC61A581-1C0C-1A4F-A664-9D47F1851D6F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="A15:C15" xr:uid="{7A8D64D8-DAED-8047-8A02-77BFC5102C46}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="A11:B11" xr:uid="{5551A4E7-D518-FA46-B47B-11BEACBD3309}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be a number between 0 and 1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="C11" xr:uid="{2EC6111F-600F-C947-8E18-A1F2DAB839DB}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C7" xr:uid="{3F0B3965-4CB6-8B44-8C48-BC8387D0780B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C10" xr:uid="{3F0B3965-4CB6-8B44-8C48-BC8387D0780B}">
       <formula1>"boundaries,osm"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A7:B7" xr:uid="{2137D998-D258-7341-8143-F5827C46783C}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C6" xr:uid="{29A5A917-42A1-FA48-BF43-0D0D31D1E9C3}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A10:B10" xr:uid="{2137D998-D258-7341-8143-F5827C46783C}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C9" xr:uid="{29A5A917-42A1-FA48-BF43-0D0D31D1E9C3}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A6:B6" xr:uid="{DC6BABA3-649A-3642-B4F4-F5BF65DA5D95}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A11:C11" xr:uid="{087AD0AA-D382-B946-9A47-A4BE5E5C03F8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A9:B9" xr:uid="{DC6BABA3-649A-3642-B4F4-F5BF65DA5D95}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A14:C14" xr:uid="{087AD0AA-D382-B946-9A47-A4BE5E5C03F8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="WorldClim resolution" prompt="Spatial resolution of WorldClim data. Select from available options." sqref="A5:B5" xr:uid="{672B443D-2D67-4843-B4DA-4374ED0F2065}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="WorldClim resolution" prompt="Spatial resolution of WorldClim data. Select from available options." sqref="C5" xr:uid="{C0A39B1E-DD85-D54B-B2E0-D3536CC73AE4}">
+      <formula1>"30 seconds,2.5 minutes,5 minutes,10 minutes"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{B20C3D3A-2037-224B-B3BF-12091F9C4F1D}">
+            <xm:f>AND(COUNTA(Species!I2:I1048576) &gt; 0, ISBLANK($C$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{515D1723-BCD0-7549-BEE2-99A1F903D09D}">
+            <xm:f>AND(COUNTA(Species!I2:I1048576) &gt; 0, ISBLANK($C$7))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DF3872-8040-0A45-AED4-6D30278E4A8A}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1648,28 +1826,28 @@
   <sheetData>
     <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>47</v>
@@ -1687,7 +1865,7 @@
         <v>7</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -1700,13 +1878,13 @@
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
@@ -1728,11 +1906,11 @@
         <v>34</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H3" s="29"/>
       <c r="I3" s="29" t="s">
@@ -1743,14 +1921,14 @@
       </c>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="39"/>
     </row>
     <row r="4" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>38</v>
@@ -1760,15 +1938,15 @@
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25" t="s">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="J4" s="27">
         <v>1970</v>
@@ -1780,7 +1958,7 @@
     </row>
     <row r="5" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>38</v>
@@ -1790,17 +1968,17 @@
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="31"/>
       <c r="K5" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
@@ -1816,27 +1994,27 @@
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="27"/>
       <c r="K6" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M6" s="25"/>
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="30" t="s">
@@ -1844,13 +2022,13 @@
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -1862,7 +2040,7 @@
     </row>
     <row r="8" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26" t="s">
@@ -1870,13 +2048,13 @@
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25" t="s">
@@ -1886,17 +2064,17 @@
         <v>1970</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M8" s="25"/>
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="30" t="s">
@@ -1904,13 +2082,13 @@
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -1922,7 +2100,7 @@
     </row>
     <row r="10" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="32" t="s">
@@ -1930,13 +2108,13 @@
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25" t="s">
@@ -1947,14 +2125,14 @@
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>4</v>
@@ -1964,13 +2142,13 @@
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29" t="s">
@@ -1980,17 +2158,17 @@
         <v>1970</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>4</v>
@@ -2000,11 +2178,11 @@
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -2016,7 +2194,7 @@
     </row>
     <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="30" t="s">
@@ -2024,11 +2202,11 @@
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
@@ -2040,7 +2218,7 @@
     </row>
     <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
@@ -2048,11 +2226,11 @@
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -2064,7 +2242,7 @@
     </row>
     <row r="15" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="30" t="s">
@@ -2072,11 +2250,11 @@
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29" t="s">
@@ -2087,14 +2265,14 @@
       </c>
       <c r="K15" s="29"/>
       <c r="L15" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M15" s="29"/>
       <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>3</v>
@@ -2104,11 +2282,11 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25" t="s">
@@ -2119,14 +2297,14 @@
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="38"/>
     </row>
     <row r="17" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>3</v>
@@ -2136,11 +2314,11 @@
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29" t="s">
@@ -2151,14 +2329,14 @@
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M17" s="29"/>
       <c r="N17" s="39"/>
     </row>
     <row r="18" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>3</v>
@@ -2168,11 +2346,11 @@
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="25" t="s">
@@ -2183,14 +2361,14 @@
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M18" s="25"/>
       <c r="N18" s="38"/>
     </row>
     <row r="19" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>3</v>
@@ -2200,11 +2378,11 @@
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="29" t="s">
@@ -2215,14 +2393,14 @@
       </c>
       <c r="K19" s="29"/>
       <c r="L19" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M19" s="29"/>
       <c r="N19" s="39"/>
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>3</v>
@@ -2232,11 +2410,11 @@
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
@@ -2256,53 +2434,30 @@
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
       <c r="J21" s="36"/>
       <c r="K21" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
       <c r="N21" s="40"/>
     </row>
-    <row r="22" spans="1:14" ht="136" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E23" s="2"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="17">
+  <dataValidations count="17">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Use NDVI?" prompt="Should relative establishment likelihood be scaled by NDVI as a measure of plant productivity? If not specified, NDVI will not be used." sqref="E1" xr:uid="{7E257CAA-8CC0-A340-B447-5367CF8B862A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Use climate suitability?" prompt="Should relative establishment likelihood be scaled by climatic suitability? If not specified, climatic suitability will not be considered." sqref="G1" xr:uid="{0C8F4E0D-27AA-554C-BBAF-B9F2080199AE}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Output resolution (optional)" prompt="Enter a single number defining the output resolution in units of the CRS defined at &quot;Global parameters&quot;. Must be a single value. This will override the resolution specified in the &quot;Global parameters&quot; tab (including if a template raster is supplied)." sqref="N1" xr:uid="{F3720B0D-204E-8340-A38E-13A15677467F}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Species names must be unique" error="Each species name can only occur once in this column. If you need to enter the species more than once, you could distinguish the entries with a suffix (e.g. BMSB 1, BMSB 2)." promptTitle="Species name" prompt="Enter a unique species name." sqref="A1:A1048576" xr:uid="{1A8A2484-F308-084A-B95D-EF4AA6FD4C66}">
-      <formula1>COUNTIF($A:$A,A1)=1</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid year" error="Must be either blank, in which case the default of 1970 is used), or a 4-digit year no later than the current year." promptTitle="Earliest year for GBIF query" prompt="Earliest year (4-digit, 1800 to current) for which occurrence records will be obtained from GBIF. Ignored if column I is blank. " sqref="J1:J1048576" xr:uid="{A67F9B3B-7593-574C-8866-86E075A6CD75}">
       <formula1>AND(ISNUMBER(J1), J1 &lt;= YEAR(TODAY()), LEN(J1)=4)</formula1>
     </dataValidation>
@@ -2320,13 +2475,16 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Infected countries (optional)" prompt="Either a comma-separated string containing country names (spaces ignored), or a file path (absolute or relative to working directory) to a CABI pest data sheet csv file. _x000a__x000a_If provided, occurrence records are constrained to these countries." sqref="L1:L1048576" xr:uid="{90363BEF-37F4-A143-A7C3-D66B0E3DA222}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Excluded BIOCLIM vars (optional)" prompt="Comma-separated BIOCLIM variables to exclude from range bagging model (e.g. bio01,bio02,bio11,bio19) when climate suitability is estimated. By default, all variables are used. Ignored if &quot;Climate suitability raster&quot; is provided at column H." sqref="M1:M1048576" xr:uid="{061FE79F-8502-FB46-81BC-44BF0D550D15}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid land use classes" error="May only contain: numerals (0 through 9), hyphen (&quot;-&quot;), and comma (&quot;,&quot;)." promptTitle="Suitable land use classes" prompt="Comma-separated land use class numbers, corresponding to the land use raster defined in the &quot;Global parameters&quot; worksheet. Ranges can be defined with a hyphen, e.g.: &quot;1, 20-25, 30&quot; is equivalent to &quot;1, 20, 21, 22, 23, 24, 25, 30&quot;. Spaces ignored. Unioned " sqref="C1:C1048576" xr:uid="{00D007D3-3FA6-E34C-98F6-4CF0D16B9D95}">
-      <formula1>ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(C1,ROW($1:$2997),1),"0123456789 ,-")))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid vegetation classes" error="May only contain: numerals (0 through 9), hyphen (&quot;-&quot;), and comma (&quot;,&quot;)." promptTitle="Suitable vegetation classes" prompt="Comma-separated vegetation class numbers, corresponding to the vagetation class raster defined in the &quot;Global parameters&quot; worksheet. Ranges can be defined with a hyphen, e.g.: &quot;1, 20-25, 30&quot; is equivalent to &quot;1, 20, 21, 22, 23, 24, 25, 30&quot;. Spaces ignored" sqref="D1:D1048576" xr:uid="{12AB12C3-DF4C-AE42-9ABD-D28288D753FD}">
-      <formula1>ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(C1,ROW($1:$2997),1),"0123456789 ,-")))</formula1>
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(C1,ROW($1:$2996),1),"0123456789 ,-")))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid resolution" error="Enter a single number." promptTitle="Output resolution (optional)" prompt="Enter a single number defining the output resolution in units of the CRS defined at &quot;Global parameters&quot;. Must be a single value. This will override the resolution specified in the &quot;Global parameters&quot; tab (including if a template raster is supplied)." sqref="N2:N1048576" xr:uid="{FB03172F-A5A2-A14B-ABA7-CB71F634FE0A}">
       <formula1>ISNUMBER(N2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Species names must be unique" error="Each species name can only occur once in this column. If you need to enter the species more than once, you could distinguish the entries with a suffix (e.g. BMSB 1, BMSB 2)." promptTitle="Species name" prompt="Enter a unique species name." sqref="A1:A1048576" xr:uid="{1A8A2484-F308-084A-B95D-EF4AA6FD4C66}">
+      <formula1>COUNTIF($A:$A,A1)=1</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid vegetation classes" error="May only contain: numerals (0 through 9), hyphen (&quot;-&quot;), and comma (&quot;,&quot;)." promptTitle="Suitable vegetation classes" prompt="Comma-separated vegetation class numbers, corresponding to the vagetation class raster defined in the &quot;Global parameters&quot; worksheet. Ranges can be defined with a hyphen, e.g.: &quot;1, 20-25, 30&quot; is equivalent to &quot;1, 20, 21, 22, 23, 24, 25, 30&quot;. Spaces ignored" sqref="D1:D1048576" xr:uid="{12AB12C3-DF4C-AE42-9ABD-D28288D753FD}">
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(C1,ROW($1:$2996),1),"0123456789 ,-")))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2337,8 +2495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ACEFBA-62FC-F844-98A7-98CB731D18DF}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2357,22 +2515,22 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2380,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="12">
         <v>1.595</v>
@@ -2395,7 +2553,7 @@
         <v>0.2</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2403,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="12">
         <v>20</v>
@@ -2418,7 +2576,7 @@
         <v>1E-4</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2426,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="12">
         <v>20</v>
@@ -2441,7 +2599,7 @@
         <v>1E-4</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2449,7 +2607,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="12">
         <v>0.05</v>
@@ -2464,7 +2622,7 @@
         <v>0.1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2472,7 +2630,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="12">
         <v>0.01</v>
@@ -2487,7 +2645,7 @@
         <v>0.02</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2495,7 +2653,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="12">
         <v>0.16500000000000001</v>
@@ -2510,15 +2668,15 @@
         <v>0.05</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12">
         <v>8.6999999999999994E-2</v>
@@ -2533,15 +2691,15 @@
         <v>0.9</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="12">
         <v>0.04</v>
@@ -2556,15 +2714,15 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="12">
         <v>2.8000000000000001E-2</v>
@@ -2579,15 +2737,15 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="12">
         <v>7.0000000000000001E-3</v>
@@ -2602,15 +2760,15 @@
         <v>0.01</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="12">
         <v>8.6999999999999994E-2</v>
@@ -2625,15 +2783,15 @@
         <v>0.9</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" s="12">
         <v>0.04</v>
@@ -2648,15 +2806,15 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="12">
         <v>2.8000000000000001E-2</v>
@@ -2671,15 +2829,15 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="12">
         <v>7.0000000000000001E-3</v>
@@ -2694,7 +2852,7 @@
         <v>0.01</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2702,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="12">
         <v>2</v>
@@ -2717,7 +2875,7 @@
         <v>0.05</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2725,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" s="12">
         <v>3</v>
@@ -2740,7 +2898,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2748,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C18" s="12">
         <v>3</v>
@@ -2763,7 +2921,7 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2771,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -2786,7 +2944,7 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2794,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="12">
         <v>0.1</v>
@@ -2809,15 +2967,15 @@
         <v>0.1</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" s="12">
         <v>7</v>
@@ -2832,15 +2990,15 @@
         <v>0.01</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="12">
         <v>3</v>
@@ -2855,15 +3013,15 @@
         <v>0.01</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C23" s="12">
         <v>1.4890000000000001</v>
@@ -2878,15 +3036,15 @@
         <v>0.05</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="12">
         <v>0.5</v>
@@ -2901,15 +3059,15 @@
         <v>0.01</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="12">
         <v>7</v>
@@ -2924,15 +3082,15 @@
         <v>0.01</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="12">
         <v>3</v>
@@ -2947,15 +3105,15 @@
         <v>0.01</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="12">
         <v>1</v>
@@ -2970,15 +3128,15 @@
         <v>0.01</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C28" s="12">
         <v>1.4890000000000001</v>
@@ -2993,15 +3151,15 @@
         <v>0.05</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C29" s="12">
         <v>0.5</v>
@@ -3016,15 +3174,15 @@
         <v>0.01</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C30" s="12">
         <v>7</v>
@@ -3039,15 +3197,15 @@
         <v>0.01</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" s="12">
         <v>3</v>
@@ -3062,15 +3220,15 @@
         <v>0.01</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C32" s="12">
         <v>1</v>
@@ -3085,15 +3243,15 @@
         <v>0.01</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C33" s="12">
         <v>1.4890000000000001</v>
@@ -3108,15 +3266,15 @@
         <v>0.05</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C34" s="12">
         <v>0.5</v>
@@ -3131,15 +3289,15 @@
         <v>0.01</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" s="12">
         <v>7</v>
@@ -3154,15 +3312,15 @@
         <v>0.01</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" s="12">
         <v>3</v>
@@ -3177,15 +3335,15 @@
         <v>0.01</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C37" s="12">
         <v>1</v>
@@ -3200,15 +3358,15 @@
         <v>0.01</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C38" s="12">
         <v>1.4890000000000001</v>
@@ -3223,15 +3381,15 @@
         <v>0.05</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="12">
         <v>0.5</v>
@@ -3246,15 +3404,15 @@
         <v>0.01</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C40" s="12">
         <v>0.89200000000000002</v>
@@ -3269,15 +3427,15 @@
         <v>0.3</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C41" s="12">
         <v>0.3</v>
@@ -3292,15 +3450,15 @@
         <v>0.3</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" s="12">
         <v>5</v>
@@ -3315,15 +3473,15 @@
         <v>0.01</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="12">
         <v>0.3</v>
@@ -3338,15 +3496,15 @@
         <v>0.1</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C44" s="12">
         <v>0.89200000000000002</v>
@@ -3361,15 +3519,15 @@
         <v>0.3</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45" s="12">
         <v>0.3</v>
@@ -3384,15 +3542,15 @@
         <v>0.3</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C46" s="12">
         <v>5</v>
@@ -3407,15 +3565,15 @@
         <v>0.01</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" s="12">
         <v>6.0119999999999996</v>
@@ -3430,15 +3588,15 @@
         <v>0.02</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C48" s="12">
         <v>14.872</v>
@@ -3453,15 +3611,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="12">
         <v>1.0369999999999999</v>
@@ -3476,15 +3634,15 @@
         <v>0.1</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C50" s="12">
         <v>1.7649999999999999</v>
@@ -3499,15 +3657,15 @@
         <v>0.05</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="12">
         <v>1.488</v>
@@ -3522,15 +3680,15 @@
         <v>0.01</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="12">
         <v>10</v>
@@ -3545,15 +3703,15 @@
         <v>1E-3</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" s="12">
         <v>15.692</v>
@@ -3568,15 +3726,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" s="12">
         <v>1.488</v>
@@ -3591,15 +3749,15 @@
         <v>0.01</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C55" s="12">
         <v>10</v>
@@ -3614,15 +3772,15 @@
         <v>1E-3</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C56" s="12">
         <v>15.692</v>
@@ -3637,15 +3795,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -3660,15 +3818,15 @@
         <v>0.05</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C58" s="12">
         <v>0.1</v>
@@ -3683,15 +3841,15 @@
         <v>0.1</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="12">
         <v>3.6080000000000001</v>
@@ -3706,15 +3864,15 @@
         <v>0.05</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C60" s="12">
         <v>1</v>
@@ -3729,15 +3887,15 @@
         <v>0.05</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C61" s="12">
         <v>0.1</v>
@@ -3752,15 +3910,15 @@
         <v>0.1</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C62" s="12">
         <v>3.6080000000000001</v>
@@ -3775,15 +3933,15 @@
         <v>0.05</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C63" s="12">
         <v>1</v>
@@ -3798,15 +3956,15 @@
         <v>0.05</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C64" s="12">
         <v>0.1</v>
@@ -3821,15 +3979,15 @@
         <v>0.1</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C65" s="12">
         <v>3.6080000000000001</v>
@@ -3844,15 +4002,15 @@
         <v>0.05</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C66" s="12">
         <v>1</v>
@@ -3867,15 +4025,15 @@
         <v>0.05</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C67" s="12">
         <v>0.1</v>
@@ -3890,15 +4048,15 @@
         <v>0.1</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C68" s="12">
         <v>3.6080000000000001</v>
@@ -3913,15 +4071,15 @@
         <v>0.05</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C69" s="12">
         <v>1.8879999999999999</v>
@@ -3936,15 +4094,15 @@
         <v>0.2</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C70" s="12">
         <v>0.2</v>
@@ -3959,7 +4117,7 @@
         <v>0.2</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -3967,7 +4125,7 @@
         <v>46</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C71" s="12">
         <v>0.04</v>
@@ -3982,7 +4140,7 @@
         <v>0.5</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -3990,7 +4148,7 @@
         <v>46</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C72" s="12">
         <v>0.03</v>
@@ -4005,34 +4163,73 @@
         <v>0.5</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="5" priority="7">
+  <conditionalFormatting sqref="A2:A11 A13:A1048576">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>AND(NOT(ISBLANK(A2)),COUNTIFS(A$2:A$1048576,A2,B$2:B$1048576,B2) &gt; 1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="B2:B11 B13:B1048576">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>AND(NOT(ISBLANK(A2)),COUNTIFS(A$2:A$1048576,A2,B$2:B$1048576,B2)&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1048576 E2:E1048576">
-    <cfRule type="expression" dxfId="3" priority="5">
+  <conditionalFormatting sqref="C2:C7 E2:E7 E13:E1048576 C13:C1048576">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>AND(NOT(ISBLANK(C2)),NOT(ISBLANK(D2)),C2&gt;D2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576 F2:F1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="D2:D7 F2:F7 F13:F1048576 D13:D1048576">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>AND(NOT(ISBLANK(D2)),NOT(ISBLANK(C2)),D2&lt;C2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B2:G7 B13:G1048576">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>AND(NOT(ISBLANK($A2)),ISBLANK(B2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C11 E8:E11">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND(NOT(ISBLANK(C8)),NOT(ISBLANK(D8)),C8&gt;D8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D11 F8:F11">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>AND(NOT(ISBLANK(D8)),NOT(ISBLANK(C8)),D8&lt;C8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:G11">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>AND(NOT(ISBLANK($A8)),ISBLANK(B8))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>AND(NOT(ISBLANK(A12)),COUNTIFS(A$2:A$1048576,A12,B$2:B$1048576,B12) &gt; 1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND(NOT(ISBLANK(A12)),COUNTIFS(A$2:A$1048576,A12,B$2:B$1048576,B12)&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12 E12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND(NOT(ISBLANK(C12)),NOT(ISBLANK(D12)),C12&gt;D12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 F12">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(NOT(ISBLANK(D12)),NOT(ISBLANK(C12)),D12&lt;C12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:G12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(NOT(ISBLANK($A12)),ISBLANK(B12))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="12">
@@ -4046,6 +4243,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pathway name" prompt="Enter a name for the biosecurity pathway. This name will be used in filenames and objects generated by the edmaps R package. Pathway names cannot be duplicated for a given species." sqref="B1" xr:uid="{5197A08A-8999-AB46-8730-855841E8CC82}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lower estimate of leakage rate" prompt="Enter the lower estimate (2.5th percentile) of the hazard's leakage rate. Cannot be greater than column D (upper estimate of leakage rate)." sqref="C1" xr:uid="{E67DB015-C3BB-FE47-BD92-D8BCE162651C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lower estimate of viability rate" prompt="Enter the lower estimate (2.5th percentile) of the hazard's viability rate. Cannot be greater than column F (upper estimate of viability rate)." sqref="E1" xr:uid="{3B23796C-73CB-5440-92F9-0462BC6AD1DB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Arrival weights raster path" prompt="Path to a raster file describing the relative likelihood of the biosecurity hazard arriving at a cell (assuming a leakage event)." sqref="G1:G1048576" xr:uid="{060FD0D3-723D-3448-A1AC-42D3F9945AC3}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicated pathway" error="Pathway name cannot be duplicated within species." promptTitle="Pathway name" prompt="Enter a name for the biosecurity pathway. This name will be used in filenames and objects generated by the edmaps R package. Pathway names cannot be duplicated for a given species." sqref="B2:B1048576" xr:uid="{FD4995E4-EE95-8F41-9C2D-46BFF18C6EC6}">
       <formula1>COUNTIFS(A$2:A$1048576,A2,B$2:B$1048576,B2)=1</formula1>
     </dataValidation>
@@ -4064,14 +4262,13 @@
       <formula1>E2</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Arrival weights raster path" prompt="Path to a raster file describing the relative likelihood of the biosecurity hazard arriving at a cell (assuming a leakage event)." sqref="G1:G1048576" xr:uid="{060FD0D3-723D-3448-A1AC-42D3F9945AC3}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{00000000-000E-0000-0400-000001000000}">
+          <x14:cfRule type="expression" priority="18" id="{00000000-000E-0000-0400-000001000000}">
             <xm:f>AND(NOT(ISBLANK($A2)), ISERROR(VLOOKUP(A2,_xlfn.ANCHORARRAY(species_set!$A$2), 1, FALSE)))</xm:f>
             <x14:dxf>
               <font>
@@ -4084,7 +4281,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A2:A7 A13:A1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4094,7 +4291,7 @@
           <x14:formula1>
             <xm:f>_xlfn.ANCHORARRAY(species_set!$A$2)</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A2:A7 A13:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4104,7 +4301,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9B2994-F348-FB43-AA88-713929604D2E}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -4122,7 +4319,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A22">_xlfn._xlws.FILTER(species,species&lt;&gt;"")</f>
+        <f t="array" ref="A2:A21">_xlfn._xlws.FILTER(species,species&lt;&gt;"")</f>
         <v>Citrus Canker</v>
       </c>
     </row>
@@ -4219,11 +4416,6 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <v>Asian Honey Bee</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="str">
-        <v>test</v>
       </c>
     </row>
   </sheetData>

</xml_diff>